<commit_message>
trying to sync computers
</commit_message>
<xml_diff>
--- a/RRAMassMods.xlsx
+++ b/RRAMassMods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5780E962-4BCC-4979-9C56-523DCDB84264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CD372A-AF8F-4A3F-A48C-957773CD636C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="welk001" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3918" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5220" uniqueCount="148">
   <si>
     <t>welk001</t>
   </si>
@@ -410,6 +410,78 @@
   <si>
     <t>dy</t>
   </si>
+  <si>
+    <t>=-0.03537,</t>
+  </si>
+  <si>
+    <t>~[-0.000397447,0.334426,0.0308154]</t>
+  </si>
+  <si>
+    <t>14.5382,</t>
+  </si>
+  <si>
+    <t>11.4821,</t>
+  </si>
+  <si>
+    <t>4.57674,</t>
+  </si>
+  <si>
+    <t>0.10641,</t>
+  </si>
+  <si>
+    <t>0.123445,</t>
+  </si>
+  <si>
+    <t>1.54307,</t>
+  </si>
+  <si>
+    <t>0.267383,</t>
+  </si>
+  <si>
+    <t>42.2635,</t>
+  </si>
+  <si>
+    <t>=-0.0413647,</t>
+  </si>
+  <si>
+    <t>~[0.00559728,0.334426,0.0297241]</t>
+  </si>
+  <si>
+    <t>=-0.0411367,</t>
+  </si>
+  <si>
+    <t>~[0.00536924,0.334426,0.0320484]</t>
+  </si>
+  <si>
+    <t>=-0.0338264,</t>
+  </si>
+  <si>
+    <t>~[-0.00194108,0.334426,0.0267107]</t>
+  </si>
+  <si>
+    <t>=-0.0360536,</t>
+  </si>
+  <si>
+    <t>~[0.000286145,0.334426,0.0241276]</t>
+  </si>
+  <si>
+    <t>=-0.0515889,</t>
+  </si>
+  <si>
+    <t>~[0.0158215,0.334426,0.032391]</t>
+  </si>
+  <si>
+    <t>=-0.037267,</t>
+  </si>
+  <si>
+    <t>~[0.00149951,0.334426,0.0527004]</t>
+  </si>
+  <si>
+    <t>=-0.0396001,</t>
+  </si>
+  <si>
+    <t>~[0.00383267,0.334426,0.039322]</t>
+  </si>
 </sst>
 </file>
 
@@ -771,7 +843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71628AC8-C740-47F3-9667-4E6EB10DD20F}">
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="AH24" sqref="AH24"/>
     </sheetView>
   </sheetViews>
@@ -5934,7 +6006,7 @@
         <v>9</v>
       </c>
       <c r="AD11">
-        <f t="shared" ref="AD11:AD26" si="1">AVERAGE(AA11,AA33,AA55,AA77)</f>
+        <f t="shared" ref="AD11:AD25" si="1">AVERAGE(AA11,AA33,AA55,AA77)</f>
         <v>8.5096300000000014</v>
       </c>
       <c r="AG11" s="1" t="s">
@@ -10344,7 +10416,7 @@
   <dimension ref="A1:AH92"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH26" sqref="AH26"/>
+      <selection activeCell="AG9" sqref="AG9:AI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15123,27 +15195,4779 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B594EC21-1ABB-4D3F-8A7D-CC790C91FD61}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AH10" sqref="AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
+      </c>
+      <c r="R3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5">
+        <f>-0.0308154</f>
+        <v>-3.08154E-2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" t="s">
+        <v>36</v>
+      </c>
+      <c r="V5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" t="s">
+        <v>38</v>
+      </c>
+      <c r="X5" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5">
+        <f>-0.0241276</f>
+        <v>-2.4127599999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>125</v>
+      </c>
+      <c r="R6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" t="s">
+        <v>43</v>
+      </c>
+      <c r="V6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="R8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S8" t="s">
+        <v>51</v>
+      </c>
+      <c r="T8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9">
+        <v>1.095</v>
+      </c>
+      <c r="L9" t="s">
+        <v>113</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T9" t="s">
+        <v>5</v>
+      </c>
+      <c r="U9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V9">
+        <v>1.6103000000000001</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>14.709300000000001</v>
+      </c>
+      <c r="L10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <f>AVERAGE(J10,J32,J54,J76)</f>
+        <v>14.693925000000002</v>
+      </c>
+      <c r="R10" t="s">
+        <v>2</v>
+      </c>
+      <c r="S10" t="s">
+        <v>3</v>
+      </c>
+      <c r="T10" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" t="s">
+        <v>126</v>
+      </c>
+      <c r="X10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10">
+        <v>14.789899999999999</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD10">
+        <f>AVERAGE(AA10,AA32,AA54,AA76)</f>
+        <v>14.787224999999999</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH10">
+        <f>AVERAGE(J10,J32,J54,J76,AA76,AA54,AA32,AA10)</f>
+        <v>14.740575000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>11.6173</v>
+      </c>
+      <c r="L11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11:M26" si="0">AVERAGE(J11,J33,J55,J77)</f>
+        <v>11.605174999999999</v>
+      </c>
+      <c r="R11" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" t="s">
+        <v>9</v>
+      </c>
+      <c r="T11" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" t="s">
+        <v>5</v>
+      </c>
+      <c r="V11" t="s">
+        <v>6</v>
+      </c>
+      <c r="W11" t="s">
+        <v>127</v>
+      </c>
+      <c r="X11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA11">
+        <v>11.680999999999999</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" ref="AD11:AD26" si="1">AVERAGE(AA11,AA33,AA55,AA77)</f>
+        <v>11.678849999999999</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" ref="AH11:AH23" si="2">AVERAGE(J11,J33,J55,J77,AA77,AA55,AA33,AA11)</f>
+        <v>11.642012499999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>4.6306200000000004</v>
+      </c>
+      <c r="L12" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>4.6257774999999999</v>
+      </c>
+      <c r="R12" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" t="s">
+        <v>11</v>
+      </c>
+      <c r="T12" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" t="s">
+        <v>5</v>
+      </c>
+      <c r="V12" t="s">
+        <v>6</v>
+      </c>
+      <c r="W12" t="s">
+        <v>128</v>
+      </c>
+      <c r="X12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA12">
+        <v>4.6559799999999996</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="1"/>
+        <v>4.6551425000000002</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="2"/>
+        <v>4.64046</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>0.10766299999999999</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>0.10755025</v>
+      </c>
+      <c r="R13" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" t="s">
+        <v>13</v>
+      </c>
+      <c r="T13" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" t="s">
+        <v>5</v>
+      </c>
+      <c r="V13" t="s">
+        <v>6</v>
+      </c>
+      <c r="W13" t="s">
+        <v>129</v>
+      </c>
+      <c r="X13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA13">
+        <v>0.108252</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="1"/>
+        <v>0.10823274999999999</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="2"/>
+        <v>0.10789150000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>0.124899</v>
+      </c>
+      <c r="L14" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>0.12476799999999999</v>
+      </c>
+      <c r="R14" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" t="s">
+        <v>15</v>
+      </c>
+      <c r="T14" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" t="s">
+        <v>5</v>
+      </c>
+      <c r="V14" t="s">
+        <v>6</v>
+      </c>
+      <c r="W14" t="s">
+        <v>130</v>
+      </c>
+      <c r="X14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA14">
+        <v>0.125583</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD14">
+        <f t="shared" si="1"/>
+        <v>0.12556</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="2"/>
+        <v>0.125164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>1.5612299999999999</v>
+      </c>
+      <c r="L15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>1.5596000000000001</v>
+      </c>
+      <c r="R15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" t="s">
+        <v>17</v>
+      </c>
+      <c r="T15" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" t="s">
+        <v>5</v>
+      </c>
+      <c r="V15" t="s">
+        <v>6</v>
+      </c>
+      <c r="W15" t="s">
+        <v>131</v>
+      </c>
+      <c r="X15" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA15">
+        <v>1.56978</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="1"/>
+        <v>1.5694999999999999</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="2"/>
+        <v>1.5645500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>0.27053100000000002</v>
+      </c>
+      <c r="L16" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.27024800000000004</v>
+      </c>
+      <c r="R16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" t="s">
+        <v>5</v>
+      </c>
+      <c r="V16" t="s">
+        <v>6</v>
+      </c>
+      <c r="W16" t="s">
+        <v>132</v>
+      </c>
+      <c r="X16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA16">
+        <v>0.27201199999999998</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="1"/>
+        <v>0.27196324999999999</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="2"/>
+        <v>0.27110562500000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>11.6173</v>
+      </c>
+      <c r="L17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>11.605174999999999</v>
+      </c>
+      <c r="R17" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" t="s">
+        <v>6</v>
+      </c>
+      <c r="W17" t="s">
+        <v>127</v>
+      </c>
+      <c r="X17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA17">
+        <v>11.680999999999999</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD17">
+        <f t="shared" si="1"/>
+        <v>11.678849999999999</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="2"/>
+        <v>11.642012499999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>4.6306200000000004</v>
+      </c>
+      <c r="L18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="0"/>
+        <v>4.6257774999999999</v>
+      </c>
+      <c r="R18" t="s">
+        <v>2</v>
+      </c>
+      <c r="S18" t="s">
+        <v>22</v>
+      </c>
+      <c r="T18" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" t="s">
+        <v>5</v>
+      </c>
+      <c r="V18" t="s">
+        <v>6</v>
+      </c>
+      <c r="W18" t="s">
+        <v>128</v>
+      </c>
+      <c r="X18" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA18">
+        <v>4.6559799999999996</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="1"/>
+        <v>4.6551425000000002</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="2"/>
+        <v>4.64046</v>
+      </c>
+    </row>
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>0.10766299999999999</v>
+      </c>
+      <c r="L19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>0.10755025</v>
+      </c>
+      <c r="R19" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" t="s">
+        <v>23</v>
+      </c>
+      <c r="T19" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" t="s">
+        <v>5</v>
+      </c>
+      <c r="V19" t="s">
+        <v>6</v>
+      </c>
+      <c r="W19" t="s">
+        <v>129</v>
+      </c>
+      <c r="X19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA19">
+        <v>0.108252</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="1"/>
+        <v>0.10823274999999999</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="2"/>
+        <v>0.10789150000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>0.124899</v>
+      </c>
+      <c r="L20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="0"/>
+        <v>0.12476799999999999</v>
+      </c>
+      <c r="R20" t="s">
+        <v>2</v>
+      </c>
+      <c r="S20" t="s">
+        <v>24</v>
+      </c>
+      <c r="T20" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" t="s">
+        <v>5</v>
+      </c>
+      <c r="V20" t="s">
+        <v>6</v>
+      </c>
+      <c r="W20" t="s">
+        <v>130</v>
+      </c>
+      <c r="X20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA20">
+        <v>0.125583</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD20">
+        <f t="shared" si="1"/>
+        <v>0.12556</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="2"/>
+        <v>0.125164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>1.5612299999999999</v>
+      </c>
+      <c r="L21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="0"/>
+        <v>1.5596000000000001</v>
+      </c>
+      <c r="R21" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" t="s">
+        <v>4</v>
+      </c>
+      <c r="U21" t="s">
+        <v>5</v>
+      </c>
+      <c r="V21" t="s">
+        <v>6</v>
+      </c>
+      <c r="W21" t="s">
+        <v>131</v>
+      </c>
+      <c r="X21" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA21">
+        <v>1.56978</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD21">
+        <f t="shared" si="1"/>
+        <v>1.5694999999999999</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="2"/>
+        <v>1.5645500000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22">
+        <v>0.27053100000000002</v>
+      </c>
+      <c r="L22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="0"/>
+        <v>0.27024800000000004</v>
+      </c>
+      <c r="R22" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" t="s">
+        <v>26</v>
+      </c>
+      <c r="T22" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" t="s">
+        <v>6</v>
+      </c>
+      <c r="W22" t="s">
+        <v>132</v>
+      </c>
+      <c r="X22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA22">
+        <v>0.27201199999999998</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD22">
+        <f t="shared" si="1"/>
+        <v>0.27196324999999999</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH22">
+        <f t="shared" si="2"/>
+        <v>0.27110562500000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>42.761099999999999</v>
+      </c>
+      <c r="L23" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="0"/>
+        <v>42.716349999999998</v>
+      </c>
+      <c r="R23" t="s">
+        <v>2</v>
+      </c>
+      <c r="S23" t="s">
+        <v>27</v>
+      </c>
+      <c r="T23" t="s">
+        <v>4</v>
+      </c>
+      <c r="U23" t="s">
+        <v>5</v>
+      </c>
+      <c r="V23" t="s">
+        <v>6</v>
+      </c>
+      <c r="W23" t="s">
+        <v>133</v>
+      </c>
+      <c r="X23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA23">
+        <v>42.9953</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD23">
+        <f t="shared" si="1"/>
+        <v>42.987524999999998</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH23">
+        <f t="shared" si="2"/>
+        <v>42.851937499999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24">
+        <v>-3.9744699999999999E-4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>38</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="0"/>
+        <v>2.1569982499999997E-3</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA24">
+        <v>2.8614500000000002E-4</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="1"/>
+        <v>5.3599562499999998E-3</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH24">
+        <f>AVERAGE(J24,J46,J68,J90,AA90,AA68,AA46,AA24)</f>
+        <v>3.75847725E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" t="s">
+        <v>123</v>
+      </c>
+      <c r="J25">
+        <v>0.334426</v>
+      </c>
+      <c r="L25" t="s">
+        <v>123</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="0"/>
+        <v>0.334426</v>
+      </c>
+      <c r="R25" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA25">
+        <v>0.334426</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" si="1"/>
+        <v>0.334426</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH25">
+        <f t="shared" ref="AH25:AH26" si="3">AVERAGE(J25,J47,J69,J91,AA91,AA69,AA47,AA25)</f>
+        <v>0.33442600000000006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J26">
+        <v>3.08154E-2</v>
+      </c>
+      <c r="L26" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="0"/>
+        <v>2.9824650000000001E-2</v>
+      </c>
+      <c r="R26" t="s">
+        <v>2</v>
+      </c>
+      <c r="S26" t="s">
+        <v>31</v>
+      </c>
+      <c r="T26" t="s">
+        <v>32</v>
+      </c>
+      <c r="U26" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA26">
+        <v>2.4127599999999999E-2</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="1"/>
+        <v>3.7135250000000002E-2</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="3"/>
+        <v>3.3479950000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I27">
+        <f>-0.0297241</f>
+        <v>-2.97241E-2</v>
+      </c>
+      <c r="R27" t="s">
+        <v>2</v>
+      </c>
+      <c r="S27" t="s">
+        <v>34</v>
+      </c>
+      <c r="T27" t="s">
+        <v>35</v>
+      </c>
+      <c r="U27" t="s">
+        <v>36</v>
+      </c>
+      <c r="V27" t="s">
+        <v>37</v>
+      </c>
+      <c r="W27" t="s">
+        <v>38</v>
+      </c>
+      <c r="X27" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z27">
+        <f>-0.032391</f>
+        <v>-3.2391000000000003E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>135</v>
+      </c>
+      <c r="R28" t="s">
+        <v>2</v>
+      </c>
+      <c r="S28" t="s">
+        <v>41</v>
+      </c>
+      <c r="T28" t="s">
+        <v>42</v>
+      </c>
+      <c r="U28" t="s">
+        <v>43</v>
+      </c>
+      <c r="V28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="R29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+      <c r="R30" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" t="s">
+        <v>51</v>
+      </c>
+      <c r="T30" t="s">
+        <v>5</v>
+      </c>
+      <c r="U30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31">
+        <v>0.74256999999999995</v>
+      </c>
+      <c r="R31" t="s">
+        <v>2</v>
+      </c>
+      <c r="S31" t="s">
+        <v>53</v>
+      </c>
+      <c r="T31" t="s">
+        <v>5</v>
+      </c>
+      <c r="U31" t="s">
+        <v>54</v>
+      </c>
+      <c r="V31">
+        <v>1.3371</v>
+      </c>
+    </row>
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <v>14.654199999999999</v>
+      </c>
+      <c r="R32" t="s">
+        <v>2</v>
+      </c>
+      <c r="S32" t="s">
+        <v>3</v>
+      </c>
+      <c r="T32" t="s">
+        <v>4</v>
+      </c>
+      <c r="U32" t="s">
+        <v>5</v>
+      </c>
+      <c r="V32" t="s">
+        <v>6</v>
+      </c>
+      <c r="W32" t="s">
+        <v>126</v>
+      </c>
+      <c r="X32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA32">
+        <v>14.747199999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>127</v>
+      </c>
+      <c r="G33" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <v>11.5738</v>
+      </c>
+      <c r="R33" t="s">
+        <v>2</v>
+      </c>
+      <c r="S33" t="s">
+        <v>9</v>
+      </c>
+      <c r="T33" t="s">
+        <v>4</v>
+      </c>
+      <c r="U33" t="s">
+        <v>5</v>
+      </c>
+      <c r="V33" t="s">
+        <v>6</v>
+      </c>
+      <c r="W33" t="s">
+        <v>127</v>
+      </c>
+      <c r="X33" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA33">
+        <v>11.6472</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34">
+        <v>4.6132799999999996</v>
+      </c>
+      <c r="R34" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" t="s">
+        <v>11</v>
+      </c>
+      <c r="T34" t="s">
+        <v>4</v>
+      </c>
+      <c r="U34" t="s">
+        <v>5</v>
+      </c>
+      <c r="V34" t="s">
+        <v>6</v>
+      </c>
+      <c r="W34" t="s">
+        <v>128</v>
+      </c>
+      <c r="X34" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA34">
+        <v>4.6425400000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35">
+        <v>0.10725999999999999</v>
+      </c>
+      <c r="R35" t="s">
+        <v>2</v>
+      </c>
+      <c r="S35" t="s">
+        <v>13</v>
+      </c>
+      <c r="T35" t="s">
+        <v>4</v>
+      </c>
+      <c r="U35" t="s">
+        <v>5</v>
+      </c>
+      <c r="V35" t="s">
+        <v>6</v>
+      </c>
+      <c r="W35" t="s">
+        <v>129</v>
+      </c>
+      <c r="X35" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA35">
+        <v>0.10793999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>0.124431</v>
+      </c>
+      <c r="R36" t="s">
+        <v>2</v>
+      </c>
+      <c r="S36" t="s">
+        <v>15</v>
+      </c>
+      <c r="T36" t="s">
+        <v>4</v>
+      </c>
+      <c r="U36" t="s">
+        <v>5</v>
+      </c>
+      <c r="V36" t="s">
+        <v>6</v>
+      </c>
+      <c r="W36" t="s">
+        <v>130</v>
+      </c>
+      <c r="X36" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA36">
+        <v>0.12522</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37">
+        <v>1.5553900000000001</v>
+      </c>
+      <c r="R37" t="s">
+        <v>2</v>
+      </c>
+      <c r="S37" t="s">
+        <v>17</v>
+      </c>
+      <c r="T37" t="s">
+        <v>4</v>
+      </c>
+      <c r="U37" t="s">
+        <v>5</v>
+      </c>
+      <c r="V37" t="s">
+        <v>6</v>
+      </c>
+      <c r="W37" t="s">
+        <v>131</v>
+      </c>
+      <c r="X37" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA37">
+        <v>1.56525</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>132</v>
+      </c>
+      <c r="G38" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38">
+        <v>0.26951799999999998</v>
+      </c>
+      <c r="R38" t="s">
+        <v>2</v>
+      </c>
+      <c r="S38" t="s">
+        <v>19</v>
+      </c>
+      <c r="T38" t="s">
+        <v>4</v>
+      </c>
+      <c r="U38" t="s">
+        <v>5</v>
+      </c>
+      <c r="V38" t="s">
+        <v>6</v>
+      </c>
+      <c r="W38" t="s">
+        <v>132</v>
+      </c>
+      <c r="X38" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA38">
+        <v>0.271227</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" t="s">
+        <v>5</v>
+      </c>
+      <c r="I39" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39">
+        <v>11.5738</v>
+      </c>
+      <c r="R39" t="s">
+        <v>2</v>
+      </c>
+      <c r="S39" t="s">
+        <v>21</v>
+      </c>
+      <c r="T39" t="s">
+        <v>4</v>
+      </c>
+      <c r="U39" t="s">
+        <v>5</v>
+      </c>
+      <c r="V39" t="s">
+        <v>6</v>
+      </c>
+      <c r="W39" t="s">
+        <v>127</v>
+      </c>
+      <c r="X39" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA39">
+        <v>11.6472</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>128</v>
+      </c>
+      <c r="G40" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" t="s">
+        <v>6</v>
+      </c>
+      <c r="J40">
+        <v>4.6132799999999996</v>
+      </c>
+      <c r="R40" t="s">
+        <v>2</v>
+      </c>
+      <c r="S40" t="s">
+        <v>22</v>
+      </c>
+      <c r="T40" t="s">
+        <v>4</v>
+      </c>
+      <c r="U40" t="s">
+        <v>5</v>
+      </c>
+      <c r="V40" t="s">
+        <v>6</v>
+      </c>
+      <c r="W40" t="s">
+        <v>128</v>
+      </c>
+      <c r="X40" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA40">
+        <v>4.6425400000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" t="s">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <v>0.10725999999999999</v>
+      </c>
+      <c r="R41" t="s">
+        <v>2</v>
+      </c>
+      <c r="S41" t="s">
+        <v>23</v>
+      </c>
+      <c r="T41" t="s">
+        <v>4</v>
+      </c>
+      <c r="U41" t="s">
+        <v>5</v>
+      </c>
+      <c r="V41" t="s">
+        <v>6</v>
+      </c>
+      <c r="W41" t="s">
+        <v>129</v>
+      </c>
+      <c r="X41" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA41">
+        <v>0.10793999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>130</v>
+      </c>
+      <c r="G42" t="s">
+        <v>8</v>
+      </c>
+      <c r="H42" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" t="s">
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <v>0.124431</v>
+      </c>
+      <c r="R42" t="s">
+        <v>2</v>
+      </c>
+      <c r="S42" t="s">
+        <v>24</v>
+      </c>
+      <c r="T42" t="s">
+        <v>4</v>
+      </c>
+      <c r="U42" t="s">
+        <v>5</v>
+      </c>
+      <c r="V42" t="s">
+        <v>6</v>
+      </c>
+      <c r="W42" t="s">
+        <v>130</v>
+      </c>
+      <c r="X42" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA42">
+        <v>0.12522</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" t="s">
+        <v>6</v>
+      </c>
+      <c r="J43">
+        <v>1.5553900000000001</v>
+      </c>
+      <c r="R43" t="s">
+        <v>2</v>
+      </c>
+      <c r="S43" t="s">
+        <v>25</v>
+      </c>
+      <c r="T43" t="s">
+        <v>4</v>
+      </c>
+      <c r="U43" t="s">
+        <v>5</v>
+      </c>
+      <c r="V43" t="s">
+        <v>6</v>
+      </c>
+      <c r="W43" t="s">
+        <v>131</v>
+      </c>
+      <c r="X43" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA43">
+        <v>1.56525</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>132</v>
+      </c>
+      <c r="G44" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>0.26951799999999998</v>
+      </c>
+      <c r="R44" t="s">
+        <v>2</v>
+      </c>
+      <c r="S44" t="s">
+        <v>26</v>
+      </c>
+      <c r="T44" t="s">
+        <v>4</v>
+      </c>
+      <c r="U44" t="s">
+        <v>5</v>
+      </c>
+      <c r="V44" t="s">
+        <v>6</v>
+      </c>
+      <c r="W44" t="s">
+        <v>132</v>
+      </c>
+      <c r="X44" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA44">
+        <v>0.271227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>133</v>
+      </c>
+      <c r="G45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <v>42.600900000000003</v>
+      </c>
+      <c r="R45" t="s">
+        <v>2</v>
+      </c>
+      <c r="S45" t="s">
+        <v>27</v>
+      </c>
+      <c r="T45" t="s">
+        <v>4</v>
+      </c>
+      <c r="U45" t="s">
+        <v>5</v>
+      </c>
+      <c r="V45" t="s">
+        <v>6</v>
+      </c>
+      <c r="W45" t="s">
+        <v>133</v>
+      </c>
+      <c r="X45" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA45">
+        <v>42.871099999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46">
+        <v>5.5972799999999996E-3</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA46">
+        <v>1.5821499999999999E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" t="s">
+        <v>123</v>
+      </c>
+      <c r="J47">
+        <v>0.334426</v>
+      </c>
+      <c r="R47" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA47">
+        <v>0.334426</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="I48" t="s">
+        <v>40</v>
+      </c>
+      <c r="J48">
+        <v>2.97241E-2</v>
+      </c>
+      <c r="R48" t="s">
+        <v>2</v>
+      </c>
+      <c r="S48" t="s">
+        <v>31</v>
+      </c>
+      <c r="T48" t="s">
+        <v>32</v>
+      </c>
+      <c r="U48" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA48">
+        <v>3.2391000000000003E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" t="s">
+        <v>36</v>
+      </c>
+      <c r="E49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" t="s">
+        <v>136</v>
+      </c>
+      <c r="H49" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49">
+        <f>-0.0320484</f>
+        <v>-3.2048399999999998E-2</v>
+      </c>
+      <c r="R49" t="s">
+        <v>2</v>
+      </c>
+      <c r="S49" t="s">
+        <v>34</v>
+      </c>
+      <c r="T49" t="s">
+        <v>35</v>
+      </c>
+      <c r="U49" t="s">
+        <v>36</v>
+      </c>
+      <c r="V49" t="s">
+        <v>37</v>
+      </c>
+      <c r="W49" t="s">
+        <v>38</v>
+      </c>
+      <c r="X49" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z49">
+        <f>-0.0527004</f>
+        <v>-5.2700400000000001E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" t="s">
+        <v>137</v>
+      </c>
+      <c r="R50" t="s">
+        <v>2</v>
+      </c>
+      <c r="S50" t="s">
+        <v>41</v>
+      </c>
+      <c r="T50" t="s">
+        <v>42</v>
+      </c>
+      <c r="U50" t="s">
+        <v>43</v>
+      </c>
+      <c r="V50" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="R51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
+      </c>
+      <c r="R52" t="s">
+        <v>2</v>
+      </c>
+      <c r="S52" t="s">
+        <v>51</v>
+      </c>
+      <c r="T52" t="s">
+        <v>5</v>
+      </c>
+      <c r="U52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>54</v>
+      </c>
+      <c r="E53">
+        <v>1.0434600000000001</v>
+      </c>
+      <c r="R53" t="s">
+        <v>2</v>
+      </c>
+      <c r="S53" t="s">
+        <v>53</v>
+      </c>
+      <c r="T53" t="s">
+        <v>5</v>
+      </c>
+      <c r="U53" t="s">
+        <v>54</v>
+      </c>
+      <c r="V53">
+        <v>1.70855</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" t="s">
+        <v>126</v>
+      </c>
+      <c r="G54" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" t="s">
+        <v>5</v>
+      </c>
+      <c r="I54" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54">
+        <v>14.7013</v>
+      </c>
+      <c r="R54" t="s">
+        <v>2</v>
+      </c>
+      <c r="S54" t="s">
+        <v>3</v>
+      </c>
+      <c r="T54" t="s">
+        <v>4</v>
+      </c>
+      <c r="U54" t="s">
+        <v>5</v>
+      </c>
+      <c r="V54" t="s">
+        <v>6</v>
+      </c>
+      <c r="W54" t="s">
+        <v>126</v>
+      </c>
+      <c r="X54" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA54">
+        <v>14.805199999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" t="s">
+        <v>127</v>
+      </c>
+      <c r="G55" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" t="s">
+        <v>5</v>
+      </c>
+      <c r="I55" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55">
+        <v>11.611000000000001</v>
+      </c>
+      <c r="R55" t="s">
+        <v>2</v>
+      </c>
+      <c r="S55" t="s">
+        <v>9</v>
+      </c>
+      <c r="T55" t="s">
+        <v>4</v>
+      </c>
+      <c r="U55" t="s">
+        <v>5</v>
+      </c>
+      <c r="V55" t="s">
+        <v>6</v>
+      </c>
+      <c r="W55" t="s">
+        <v>127</v>
+      </c>
+      <c r="X55" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA55">
+        <v>11.693099999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" t="s">
+        <v>128</v>
+      </c>
+      <c r="G56" t="s">
+        <v>8</v>
+      </c>
+      <c r="H56" t="s">
+        <v>5</v>
+      </c>
+      <c r="I56" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56">
+        <v>4.6280900000000003</v>
+      </c>
+      <c r="R56" t="s">
+        <v>2</v>
+      </c>
+      <c r="S56" t="s">
+        <v>11</v>
+      </c>
+      <c r="T56" t="s">
+        <v>4</v>
+      </c>
+      <c r="U56" t="s">
+        <v>5</v>
+      </c>
+      <c r="V56" t="s">
+        <v>6</v>
+      </c>
+      <c r="W56" t="s">
+        <v>128</v>
+      </c>
+      <c r="X56" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA56">
+        <v>4.6608200000000002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F57" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" t="s">
+        <v>5</v>
+      </c>
+      <c r="I57" t="s">
+        <v>6</v>
+      </c>
+      <c r="J57">
+        <v>0.10760400000000001</v>
+      </c>
+      <c r="R57" t="s">
+        <v>2</v>
+      </c>
+      <c r="S57" t="s">
+        <v>13</v>
+      </c>
+      <c r="T57" t="s">
+        <v>4</v>
+      </c>
+      <c r="U57" t="s">
+        <v>5</v>
+      </c>
+      <c r="V57" t="s">
+        <v>6</v>
+      </c>
+      <c r="W57" t="s">
+        <v>129</v>
+      </c>
+      <c r="X57" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA57">
+        <v>0.108365</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" t="s">
+        <v>130</v>
+      </c>
+      <c r="G58" t="s">
+        <v>8</v>
+      </c>
+      <c r="H58" t="s">
+        <v>5</v>
+      </c>
+      <c r="I58" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58">
+        <v>0.12483</v>
+      </c>
+      <c r="R58" t="s">
+        <v>2</v>
+      </c>
+      <c r="S58" t="s">
+        <v>15</v>
+      </c>
+      <c r="T58" t="s">
+        <v>4</v>
+      </c>
+      <c r="U58" t="s">
+        <v>5</v>
+      </c>
+      <c r="V58" t="s">
+        <v>6</v>
+      </c>
+      <c r="W58" t="s">
+        <v>130</v>
+      </c>
+      <c r="X58" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA58">
+        <v>0.12571299999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" t="s">
+        <v>131</v>
+      </c>
+      <c r="G59" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I59" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59">
+        <v>1.5603800000000001</v>
+      </c>
+      <c r="R59" t="s">
+        <v>2</v>
+      </c>
+      <c r="S59" t="s">
+        <v>17</v>
+      </c>
+      <c r="T59" t="s">
+        <v>4</v>
+      </c>
+      <c r="U59" t="s">
+        <v>5</v>
+      </c>
+      <c r="V59" t="s">
+        <v>6</v>
+      </c>
+      <c r="W59" t="s">
+        <v>131</v>
+      </c>
+      <c r="X59" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA59">
+        <v>1.57141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>132</v>
+      </c>
+      <c r="G60" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" t="s">
+        <v>5</v>
+      </c>
+      <c r="I60" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60">
+        <v>0.27038299999999998</v>
+      </c>
+      <c r="R60" t="s">
+        <v>2</v>
+      </c>
+      <c r="S60" t="s">
+        <v>19</v>
+      </c>
+      <c r="T60" t="s">
+        <v>4</v>
+      </c>
+      <c r="U60" t="s">
+        <v>5</v>
+      </c>
+      <c r="V60" t="s">
+        <v>6</v>
+      </c>
+      <c r="W60" t="s">
+        <v>132</v>
+      </c>
+      <c r="X60" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA60">
+        <v>0.27229500000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" t="s">
+        <v>127</v>
+      </c>
+      <c r="G61" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" t="s">
+        <v>5</v>
+      </c>
+      <c r="I61" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61">
+        <v>11.611000000000001</v>
+      </c>
+      <c r="R61" t="s">
+        <v>2</v>
+      </c>
+      <c r="S61" t="s">
+        <v>21</v>
+      </c>
+      <c r="T61" t="s">
+        <v>4</v>
+      </c>
+      <c r="U61" t="s">
+        <v>5</v>
+      </c>
+      <c r="V61" t="s">
+        <v>6</v>
+      </c>
+      <c r="W61" t="s">
+        <v>127</v>
+      </c>
+      <c r="X61" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA61">
+        <v>11.693099999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" t="s">
+        <v>128</v>
+      </c>
+      <c r="G62" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I62" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62">
+        <v>4.6280900000000003</v>
+      </c>
+      <c r="R62" t="s">
+        <v>2</v>
+      </c>
+      <c r="S62" t="s">
+        <v>22</v>
+      </c>
+      <c r="T62" t="s">
+        <v>4</v>
+      </c>
+      <c r="U62" t="s">
+        <v>5</v>
+      </c>
+      <c r="V62" t="s">
+        <v>6</v>
+      </c>
+      <c r="W62" t="s">
+        <v>128</v>
+      </c>
+      <c r="X62" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA62">
+        <v>4.6608200000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" t="s">
+        <v>129</v>
+      </c>
+      <c r="G63" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" t="s">
+        <v>5</v>
+      </c>
+      <c r="I63" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63">
+        <v>0.10760400000000001</v>
+      </c>
+      <c r="R63" t="s">
+        <v>2</v>
+      </c>
+      <c r="S63" t="s">
+        <v>23</v>
+      </c>
+      <c r="T63" t="s">
+        <v>4</v>
+      </c>
+      <c r="U63" t="s">
+        <v>5</v>
+      </c>
+      <c r="V63" t="s">
+        <v>6</v>
+      </c>
+      <c r="W63" t="s">
+        <v>129</v>
+      </c>
+      <c r="X63" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA63">
+        <v>0.108365</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" t="s">
+        <v>130</v>
+      </c>
+      <c r="G64" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" t="s">
+        <v>6</v>
+      </c>
+      <c r="J64">
+        <v>0.12483</v>
+      </c>
+      <c r="R64" t="s">
+        <v>2</v>
+      </c>
+      <c r="S64" t="s">
+        <v>24</v>
+      </c>
+      <c r="T64" t="s">
+        <v>4</v>
+      </c>
+      <c r="U64" t="s">
+        <v>5</v>
+      </c>
+      <c r="V64" t="s">
+        <v>6</v>
+      </c>
+      <c r="W64" t="s">
+        <v>130</v>
+      </c>
+      <c r="X64" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA64">
+        <v>0.12571299999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>131</v>
+      </c>
+      <c r="G65" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" t="s">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <v>1.5603800000000001</v>
+      </c>
+      <c r="R65" t="s">
+        <v>2</v>
+      </c>
+      <c r="S65" t="s">
+        <v>25</v>
+      </c>
+      <c r="T65" t="s">
+        <v>4</v>
+      </c>
+      <c r="U65" t="s">
+        <v>5</v>
+      </c>
+      <c r="V65" t="s">
+        <v>6</v>
+      </c>
+      <c r="W65" t="s">
+        <v>131</v>
+      </c>
+      <c r="X65" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA65">
+        <v>1.57141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" t="s">
+        <v>132</v>
+      </c>
+      <c r="G66" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66">
+        <v>0.27038299999999998</v>
+      </c>
+      <c r="R66" t="s">
+        <v>2</v>
+      </c>
+      <c r="S66" t="s">
+        <v>26</v>
+      </c>
+      <c r="T66" t="s">
+        <v>4</v>
+      </c>
+      <c r="U66" t="s">
+        <v>5</v>
+      </c>
+      <c r="V66" t="s">
+        <v>6</v>
+      </c>
+      <c r="W66" t="s">
+        <v>132</v>
+      </c>
+      <c r="X66" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA66">
+        <v>0.27229500000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" t="s">
+        <v>133</v>
+      </c>
+      <c r="G67" t="s">
+        <v>8</v>
+      </c>
+      <c r="H67" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67">
+        <v>42.737699999999997</v>
+      </c>
+      <c r="R67" t="s">
+        <v>2</v>
+      </c>
+      <c r="S67" t="s">
+        <v>27</v>
+      </c>
+      <c r="T67" t="s">
+        <v>4</v>
+      </c>
+      <c r="U67" t="s">
+        <v>5</v>
+      </c>
+      <c r="V67" t="s">
+        <v>6</v>
+      </c>
+      <c r="W67" t="s">
+        <v>133</v>
+      </c>
+      <c r="X67" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA67">
+        <v>43.039900000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>38</v>
+      </c>
+      <c r="J68">
+        <v>5.36924E-3</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA68">
+        <v>1.4995099999999999E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>55</v>
+      </c>
+      <c r="I69" t="s">
+        <v>123</v>
+      </c>
+      <c r="J69">
+        <v>0.334426</v>
+      </c>
+      <c r="R69" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA69">
+        <v>0.334426</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" t="s">
+        <v>33</v>
+      </c>
+      <c r="I70" t="s">
+        <v>40</v>
+      </c>
+      <c r="J70">
+        <v>3.2048399999999998E-2</v>
+      </c>
+      <c r="R70" t="s">
+        <v>2</v>
+      </c>
+      <c r="S70" t="s">
+        <v>31</v>
+      </c>
+      <c r="T70" t="s">
+        <v>32</v>
+      </c>
+      <c r="U70" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA70">
+        <v>5.2700400000000001E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" t="s">
+        <v>37</v>
+      </c>
+      <c r="F71" t="s">
+        <v>38</v>
+      </c>
+      <c r="G71" t="s">
+        <v>138</v>
+      </c>
+      <c r="H71" t="s">
+        <v>40</v>
+      </c>
+      <c r="I71">
+        <f>-0.0267107</f>
+        <v>-2.67107E-2</v>
+      </c>
+      <c r="R71" t="s">
+        <v>2</v>
+      </c>
+      <c r="S71" t="s">
+        <v>34</v>
+      </c>
+      <c r="T71" t="s">
+        <v>35</v>
+      </c>
+      <c r="U71" t="s">
+        <v>36</v>
+      </c>
+      <c r="V71" t="s">
+        <v>37</v>
+      </c>
+      <c r="W71" t="s">
+        <v>38</v>
+      </c>
+      <c r="X71" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z71">
+        <f>-0.039322</f>
+        <v>-3.9322000000000003E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>2</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" t="s">
+        <v>43</v>
+      </c>
+      <c r="E72" t="s">
+        <v>139</v>
+      </c>
+      <c r="R72" t="s">
+        <v>2</v>
+      </c>
+      <c r="S72" t="s">
+        <v>41</v>
+      </c>
+      <c r="T72" t="s">
+        <v>42</v>
+      </c>
+      <c r="U72" t="s">
+        <v>43</v>
+      </c>
+      <c r="V72" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>50</v>
+      </c>
+      <c r="R73" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>52</v>
+      </c>
+      <c r="R74" t="s">
+        <v>2</v>
+      </c>
+      <c r="S74" t="s">
+        <v>51</v>
+      </c>
+      <c r="T74" t="s">
+        <v>5</v>
+      </c>
+      <c r="U74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>54</v>
+      </c>
+      <c r="E75">
+        <v>1.10507</v>
+      </c>
+      <c r="R75" t="s">
+        <v>2</v>
+      </c>
+      <c r="S75" t="s">
+        <v>53</v>
+      </c>
+      <c r="T75" t="s">
+        <v>5</v>
+      </c>
+      <c r="U75" t="s">
+        <v>54</v>
+      </c>
+      <c r="V75">
+        <v>1.7170300000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" t="s">
+        <v>126</v>
+      </c>
+      <c r="G76" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" t="s">
+        <v>6</v>
+      </c>
+      <c r="J76">
+        <v>14.710900000000001</v>
+      </c>
+      <c r="R76" t="s">
+        <v>2</v>
+      </c>
+      <c r="S76" t="s">
+        <v>3</v>
+      </c>
+      <c r="T76" t="s">
+        <v>4</v>
+      </c>
+      <c r="U76" t="s">
+        <v>5</v>
+      </c>
+      <c r="V76" t="s">
+        <v>6</v>
+      </c>
+      <c r="W76" t="s">
+        <v>126</v>
+      </c>
+      <c r="X76" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA76">
+        <v>14.8066</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+      <c r="F77" t="s">
+        <v>127</v>
+      </c>
+      <c r="G77" t="s">
+        <v>8</v>
+      </c>
+      <c r="H77" t="s">
+        <v>5</v>
+      </c>
+      <c r="I77" t="s">
+        <v>6</v>
+      </c>
+      <c r="J77">
+        <v>11.618600000000001</v>
+      </c>
+      <c r="R77" t="s">
+        <v>2</v>
+      </c>
+      <c r="S77" t="s">
+        <v>9</v>
+      </c>
+      <c r="T77" t="s">
+        <v>4</v>
+      </c>
+      <c r="U77" t="s">
+        <v>5</v>
+      </c>
+      <c r="V77" t="s">
+        <v>6</v>
+      </c>
+      <c r="W77" t="s">
+        <v>127</v>
+      </c>
+      <c r="X77" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA77">
+        <v>11.694100000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+      <c r="F78" t="s">
+        <v>128</v>
+      </c>
+      <c r="G78" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I78" t="s">
+        <v>6</v>
+      </c>
+      <c r="J78">
+        <v>4.6311200000000001</v>
+      </c>
+      <c r="R78" t="s">
+        <v>2</v>
+      </c>
+      <c r="S78" t="s">
+        <v>11</v>
+      </c>
+      <c r="T78" t="s">
+        <v>4</v>
+      </c>
+      <c r="U78" t="s">
+        <v>5</v>
+      </c>
+      <c r="V78" t="s">
+        <v>6</v>
+      </c>
+      <c r="W78" t="s">
+        <v>128</v>
+      </c>
+      <c r="X78" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA78">
+        <v>4.6612299999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>2</v>
+      </c>
+      <c r="B79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+      <c r="F79" t="s">
+        <v>129</v>
+      </c>
+      <c r="G79" t="s">
+        <v>8</v>
+      </c>
+      <c r="H79" t="s">
+        <v>5</v>
+      </c>
+      <c r="I79" t="s">
+        <v>6</v>
+      </c>
+      <c r="J79">
+        <v>0.10767400000000001</v>
+      </c>
+      <c r="R79" t="s">
+        <v>2</v>
+      </c>
+      <c r="S79" t="s">
+        <v>13</v>
+      </c>
+      <c r="T79" t="s">
+        <v>4</v>
+      </c>
+      <c r="U79" t="s">
+        <v>5</v>
+      </c>
+      <c r="V79" t="s">
+        <v>6</v>
+      </c>
+      <c r="W79" t="s">
+        <v>129</v>
+      </c>
+      <c r="X79" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA79">
+        <v>0.108374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80" t="s">
+        <v>15</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+      <c r="F80" t="s">
+        <v>130</v>
+      </c>
+      <c r="G80" t="s">
+        <v>8</v>
+      </c>
+      <c r="H80" t="s">
+        <v>5</v>
+      </c>
+      <c r="I80" t="s">
+        <v>6</v>
+      </c>
+      <c r="J80">
+        <v>0.124912</v>
+      </c>
+      <c r="R80" t="s">
+        <v>2</v>
+      </c>
+      <c r="S80" t="s">
+        <v>15</v>
+      </c>
+      <c r="T80" t="s">
+        <v>4</v>
+      </c>
+      <c r="U80" t="s">
+        <v>5</v>
+      </c>
+      <c r="V80" t="s">
+        <v>6</v>
+      </c>
+      <c r="W80" t="s">
+        <v>130</v>
+      </c>
+      <c r="X80" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA80">
+        <v>0.125724</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+      <c r="F81" t="s">
+        <v>131</v>
+      </c>
+      <c r="G81" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" t="s">
+        <v>5</v>
+      </c>
+      <c r="I81" t="s">
+        <v>6</v>
+      </c>
+      <c r="J81">
+        <v>1.5613999999999999</v>
+      </c>
+      <c r="R81" t="s">
+        <v>2</v>
+      </c>
+      <c r="S81" t="s">
+        <v>17</v>
+      </c>
+      <c r="T81" t="s">
+        <v>4</v>
+      </c>
+      <c r="U81" t="s">
+        <v>5</v>
+      </c>
+      <c r="V81" t="s">
+        <v>6</v>
+      </c>
+      <c r="W81" t="s">
+        <v>131</v>
+      </c>
+      <c r="X81" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA81">
+        <v>1.5715600000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>5</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+      <c r="F82" t="s">
+        <v>132</v>
+      </c>
+      <c r="G82" t="s">
+        <v>8</v>
+      </c>
+      <c r="H82" t="s">
+        <v>5</v>
+      </c>
+      <c r="I82" t="s">
+        <v>6</v>
+      </c>
+      <c r="J82">
+        <v>0.27056000000000002</v>
+      </c>
+      <c r="R82" t="s">
+        <v>2</v>
+      </c>
+      <c r="S82" t="s">
+        <v>19</v>
+      </c>
+      <c r="T82" t="s">
+        <v>4</v>
+      </c>
+      <c r="U82" t="s">
+        <v>5</v>
+      </c>
+      <c r="V82" t="s">
+        <v>6</v>
+      </c>
+      <c r="W82" t="s">
+        <v>132</v>
+      </c>
+      <c r="X82" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA82">
+        <v>0.27231899999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" t="s">
+        <v>127</v>
+      </c>
+      <c r="G83" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" t="s">
+        <v>5</v>
+      </c>
+      <c r="I83" t="s">
+        <v>6</v>
+      </c>
+      <c r="J83">
+        <v>11.618600000000001</v>
+      </c>
+      <c r="R83" t="s">
+        <v>2</v>
+      </c>
+      <c r="S83" t="s">
+        <v>21</v>
+      </c>
+      <c r="T83" t="s">
+        <v>4</v>
+      </c>
+      <c r="U83" t="s">
+        <v>5</v>
+      </c>
+      <c r="V83" t="s">
+        <v>6</v>
+      </c>
+      <c r="W83" t="s">
+        <v>127</v>
+      </c>
+      <c r="X83" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA83">
+        <v>11.694100000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>5</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+      <c r="F84" t="s">
+        <v>128</v>
+      </c>
+      <c r="G84" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" t="s">
+        <v>5</v>
+      </c>
+      <c r="I84" t="s">
+        <v>6</v>
+      </c>
+      <c r="J84">
+        <v>4.6311200000000001</v>
+      </c>
+      <c r="R84" t="s">
+        <v>2</v>
+      </c>
+      <c r="S84" t="s">
+        <v>22</v>
+      </c>
+      <c r="T84" t="s">
+        <v>4</v>
+      </c>
+      <c r="U84" t="s">
+        <v>5</v>
+      </c>
+      <c r="V84" t="s">
+        <v>6</v>
+      </c>
+      <c r="W84" t="s">
+        <v>128</v>
+      </c>
+      <c r="X84" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA84">
+        <v>4.6612299999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>5</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" t="s">
+        <v>129</v>
+      </c>
+      <c r="G85" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" t="s">
+        <v>5</v>
+      </c>
+      <c r="I85" t="s">
+        <v>6</v>
+      </c>
+      <c r="J85">
+        <v>0.10767400000000001</v>
+      </c>
+      <c r="R85" t="s">
+        <v>2</v>
+      </c>
+      <c r="S85" t="s">
+        <v>23</v>
+      </c>
+      <c r="T85" t="s">
+        <v>4</v>
+      </c>
+      <c r="U85" t="s">
+        <v>5</v>
+      </c>
+      <c r="V85" t="s">
+        <v>6</v>
+      </c>
+      <c r="W85" t="s">
+        <v>129</v>
+      </c>
+      <c r="X85" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA85">
+        <v>0.108374</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>5</v>
+      </c>
+      <c r="E86" t="s">
+        <v>6</v>
+      </c>
+      <c r="F86" t="s">
+        <v>130</v>
+      </c>
+      <c r="G86" t="s">
+        <v>8</v>
+      </c>
+      <c r="H86" t="s">
+        <v>5</v>
+      </c>
+      <c r="I86" t="s">
+        <v>6</v>
+      </c>
+      <c r="J86">
+        <v>0.124912</v>
+      </c>
+      <c r="R86" t="s">
+        <v>2</v>
+      </c>
+      <c r="S86" t="s">
+        <v>24</v>
+      </c>
+      <c r="T86" t="s">
+        <v>4</v>
+      </c>
+      <c r="U86" t="s">
+        <v>5</v>
+      </c>
+      <c r="V86" t="s">
+        <v>6</v>
+      </c>
+      <c r="W86" t="s">
+        <v>130</v>
+      </c>
+      <c r="X86" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA86">
+        <v>0.125724</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+      <c r="F87" t="s">
+        <v>131</v>
+      </c>
+      <c r="G87" t="s">
+        <v>8</v>
+      </c>
+      <c r="H87" t="s">
+        <v>5</v>
+      </c>
+      <c r="I87" t="s">
+        <v>6</v>
+      </c>
+      <c r="J87">
+        <v>1.5613999999999999</v>
+      </c>
+      <c r="R87" t="s">
+        <v>2</v>
+      </c>
+      <c r="S87" t="s">
+        <v>25</v>
+      </c>
+      <c r="T87" t="s">
+        <v>4</v>
+      </c>
+      <c r="U87" t="s">
+        <v>5</v>
+      </c>
+      <c r="V87" t="s">
+        <v>6</v>
+      </c>
+      <c r="W87" t="s">
+        <v>131</v>
+      </c>
+      <c r="X87" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z87" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA87">
+        <v>1.5715600000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" t="s">
+        <v>26</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>5</v>
+      </c>
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" t="s">
+        <v>132</v>
+      </c>
+      <c r="G88" t="s">
+        <v>8</v>
+      </c>
+      <c r="H88" t="s">
+        <v>5</v>
+      </c>
+      <c r="I88" t="s">
+        <v>6</v>
+      </c>
+      <c r="J88">
+        <v>0.27056000000000002</v>
+      </c>
+      <c r="R88" t="s">
+        <v>2</v>
+      </c>
+      <c r="S88" t="s">
+        <v>26</v>
+      </c>
+      <c r="T88" t="s">
+        <v>4</v>
+      </c>
+      <c r="U88" t="s">
+        <v>5</v>
+      </c>
+      <c r="V88" t="s">
+        <v>6</v>
+      </c>
+      <c r="W88" t="s">
+        <v>132</v>
+      </c>
+      <c r="X88" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA88">
+        <v>0.27231899999999998</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>5</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" t="s">
+        <v>133</v>
+      </c>
+      <c r="G89" t="s">
+        <v>8</v>
+      </c>
+      <c r="H89" t="s">
+        <v>5</v>
+      </c>
+      <c r="I89" t="s">
+        <v>6</v>
+      </c>
+      <c r="J89">
+        <v>42.765700000000002</v>
+      </c>
+      <c r="R89" t="s">
+        <v>2</v>
+      </c>
+      <c r="S89" t="s">
+        <v>27</v>
+      </c>
+      <c r="T89" t="s">
+        <v>4</v>
+      </c>
+      <c r="U89" t="s">
+        <v>5</v>
+      </c>
+      <c r="V89" t="s">
+        <v>6</v>
+      </c>
+      <c r="W89" t="s">
+        <v>133</v>
+      </c>
+      <c r="X89" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z89" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA89">
+        <v>43.043799999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>38</v>
+      </c>
+      <c r="J90">
+        <v>-1.94108E-3</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA90">
+        <v>3.8326699999999998E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I91" t="s">
+        <v>123</v>
+      </c>
+      <c r="J91">
+        <v>0.334426</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA91">
+        <v>0.334426</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I92" t="s">
+        <v>40</v>
+      </c>
+      <c r="J92">
+        <v>2.67107E-2</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA92">
+        <v>3.9322000000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -15152,9 +19976,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15272,25 +20099,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15312,9 +20129,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated all of the scripts. changed a data structure from array to text cell array, and then had to change syntax in accessing it later on.
</commit_message>
<xml_diff>
--- a/RRAMassMods.xlsx
+++ b/RRAMassMods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAED0F8-4602-4FD6-A4F5-A0957353A8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BE6EA4-07A5-4F6F-B751-6A9C0283F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
+    <workbookView xWindow="3075" yWindow="2430" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="welk001" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="welk007" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6525" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6525" uniqueCount="168">
   <si>
     <t>welk001</t>
   </si>
@@ -495,6 +496,54 @@
   <si>
     <t>~[0.0661084,0.314147,0.0384651]</t>
   </si>
+  <si>
+    <t>=0.0139863,</t>
+  </si>
+  <si>
+    <t>~[-0.0478779,0.314147,0.0404682]</t>
+  </si>
+  <si>
+    <t>=0.0174725,</t>
+  </si>
+  <si>
+    <t>~[-0.0513641,0.314147,0.0274401]</t>
+  </si>
+  <si>
+    <t>=0.00957065,</t>
+  </si>
+  <si>
+    <t>~[-0.0434622,0.314147,0.0417722]</t>
+  </si>
+  <si>
+    <t>=0.00932871,</t>
+  </si>
+  <si>
+    <t>~[-0.0432203,0.314147,0.0411497]</t>
+  </si>
+  <si>
+    <t>=0.0152583,</t>
+  </si>
+  <si>
+    <t>~[-0.0491498,0.314147,0.0636487]</t>
+  </si>
+  <si>
+    <t>=0.0263827,</t>
+  </si>
+  <si>
+    <t>~[-0.0602743,0.314147,0.0610823]</t>
+  </si>
+  <si>
+    <t>=0.0257993,</t>
+  </si>
+  <si>
+    <t>~[-0.0596908,0.314147,0.0676044]</t>
+  </si>
+  <si>
+    <t>=0.0287816,</t>
+  </si>
+  <si>
+    <t>~[-0.0626732,0.314147,0.0659737]</t>
+  </si>
 </sst>
 </file>
 
@@ -856,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71628AC8-C740-47F3-9667-4E6EB10DD20F}">
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
@@ -19992,8 +20041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FE46D1-E00B-478F-BC49-0EAED21FA345}">
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="AD12" workbookViewId="0">
+      <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20065,14 +20114,14 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5">
-        <f>-0.0308154</f>
-        <v>-3.08154E-2</v>
+        <f>-0.0404682</f>
+        <v>-4.0468200000000003E-2</v>
       </c>
       <c r="R5" t="s">
         <v>2</v>
@@ -20093,14 +20142,14 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
       </c>
       <c r="Z5">
-        <f>-0.0241276</f>
-        <v>-2.4127599999999999E-2</v>
+        <f>-0.0636487</f>
+        <v>-6.3648700000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
@@ -20117,7 +20166,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -20132,7 +20181,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -20183,7 +20232,7 @@
         <v>48</v>
       </c>
       <c r="E9">
-        <v>1.095</v>
+        <v>1.8625700000000001</v>
       </c>
       <c r="L9" t="s">
         <v>105</v>
@@ -20201,7 +20250,7 @@
         <v>48</v>
       </c>
       <c r="V9">
-        <v>1.6103000000000001</v>
+        <v>2.9411</v>
       </c>
       <c r="AC9" t="s">
         <v>105</v>
@@ -20227,7 +20276,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -20239,14 +20288,14 @@
         <v>6</v>
       </c>
       <c r="J10">
-        <v>14.709300000000001</v>
+        <v>9.2329100000000004</v>
       </c>
       <c r="L10" t="s">
         <v>3</v>
       </c>
       <c r="M10">
         <f>AVERAGE(J10,J32,J54,J76)</f>
-        <v>14.693925000000002</v>
+        <v>9.2176000000000009</v>
       </c>
       <c r="R10" t="s">
         <v>2</v>
@@ -20264,7 +20313,7 @@
         <v>6</v>
       </c>
       <c r="W10" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="X10" t="s">
         <v>8</v>
@@ -20276,21 +20325,21 @@
         <v>6</v>
       </c>
       <c r="AA10">
-        <v>14.789899999999999</v>
+        <v>9.40151</v>
       </c>
       <c r="AC10" t="s">
         <v>3</v>
       </c>
       <c r="AD10">
         <f>AVERAGE(AA10,AA32,AA54,AA76)</f>
-        <v>14.787224999999999</v>
+        <v>9.410425</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AH10">
         <f>AVERAGE(J10,J32,J54,J76,AA76,AA54,AA32,AA10)</f>
-        <v>14.740575000000002</v>
+        <v>9.3140125000000005</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -20310,7 +20359,7 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -20322,14 +20371,14 @@
         <v>6</v>
       </c>
       <c r="J11">
-        <v>11.6173</v>
+        <v>7.2920999999999996</v>
       </c>
       <c r="L11" t="s">
         <v>9</v>
       </c>
       <c r="M11">
         <f t="shared" ref="M11:M26" si="0">AVERAGE(J11,J33,J55,J77)</f>
-        <v>11.605174999999999</v>
+        <v>7.2800050000000001</v>
       </c>
       <c r="R11" t="s">
         <v>2</v>
@@ -20347,7 +20396,7 @@
         <v>6</v>
       </c>
       <c r="W11" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X11" t="s">
         <v>8</v>
@@ -20359,21 +20408,21 @@
         <v>6</v>
       </c>
       <c r="AA11">
-        <v>11.680999999999999</v>
+        <v>7.4252599999999997</v>
       </c>
       <c r="AC11" t="s">
         <v>9</v>
       </c>
       <c r="AD11">
         <f t="shared" ref="AD11:AD26" si="1">AVERAGE(AA11,AA33,AA55,AA77)</f>
-        <v>11.678849999999999</v>
+        <v>7.4322949999999999</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AH11">
         <f t="shared" ref="AH11:AH23" si="2">AVERAGE(J11,J33,J55,J77,AA77,AA55,AA33,AA11)</f>
-        <v>11.642012499999998</v>
+        <v>7.3561500000000004</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -20393,7 +20442,7 @@
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -20405,14 +20454,14 @@
         <v>6</v>
       </c>
       <c r="J12">
-        <v>4.6306200000000004</v>
+        <v>2.9066000000000001</v>
       </c>
       <c r="L12" t="s">
         <v>11</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>4.6257774999999999</v>
+        <v>2.9017775000000001</v>
       </c>
       <c r="R12" t="s">
         <v>2</v>
@@ -20430,7 +20479,7 @@
         <v>6</v>
       </c>
       <c r="W12" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X12" t="s">
         <v>8</v>
@@ -20442,21 +20491,21 @@
         <v>6</v>
       </c>
       <c r="AA12">
-        <v>4.6559799999999996</v>
+        <v>2.9596800000000001</v>
       </c>
       <c r="AC12" t="s">
         <v>11</v>
       </c>
       <c r="AD12">
         <f t="shared" si="1"/>
-        <v>4.6551425000000002</v>
+        <v>2.962485</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AH12">
         <f t="shared" si="2"/>
-        <v>4.64046</v>
+        <v>2.9321312499999999</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -20476,7 +20525,7 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -20488,14 +20537,14 @@
         <v>6</v>
       </c>
       <c r="J13">
-        <v>0.10766299999999999</v>
+        <v>6.7578899999999997E-2</v>
       </c>
       <c r="L13" t="s">
         <v>13</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>0.10755025</v>
+        <v>6.7466875000000009E-2</v>
       </c>
       <c r="R13" t="s">
         <v>2</v>
@@ -20513,7 +20562,7 @@
         <v>6</v>
       </c>
       <c r="W13" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X13" t="s">
         <v>8</v>
@@ -20525,21 +20574,21 @@
         <v>6</v>
       </c>
       <c r="AA13">
-        <v>0.108252</v>
+        <v>6.8812999999999999E-2</v>
       </c>
       <c r="AC13" t="s">
         <v>13</v>
       </c>
       <c r="AD13">
         <f t="shared" si="1"/>
-        <v>0.10823274999999999</v>
+        <v>6.8878224999999987E-2</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AH13">
         <f t="shared" si="2"/>
-        <v>0.10789150000000002</v>
+        <v>6.8172549999999998E-2</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -20559,7 +20608,7 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -20571,14 +20620,14 @@
         <v>6</v>
       </c>
       <c r="J14">
-        <v>0.124899</v>
+        <v>7.8397800000000004E-2</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>0.12476799999999999</v>
+        <v>7.8267824999999999E-2</v>
       </c>
       <c r="R14" t="s">
         <v>2</v>
@@ -20596,7 +20645,7 @@
         <v>6</v>
       </c>
       <c r="W14" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X14" t="s">
         <v>8</v>
@@ -20608,21 +20657,21 @@
         <v>6</v>
       </c>
       <c r="AA14">
-        <v>0.125583</v>
+        <v>7.9829399999999995E-2</v>
       </c>
       <c r="AC14" t="s">
         <v>15</v>
       </c>
       <c r="AD14">
         <f t="shared" si="1"/>
-        <v>0.12556</v>
+        <v>7.9905125000000007E-2</v>
       </c>
       <c r="AG14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>0.125164</v>
+        <v>7.9086474999999989E-2</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
@@ -20642,7 +20691,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -20654,14 +20703,14 @@
         <v>6</v>
       </c>
       <c r="J15">
-        <v>1.5612299999999999</v>
+        <v>0.97997299999999998</v>
       </c>
       <c r="L15" t="s">
         <v>17</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>1.5596000000000001</v>
+        <v>0.978348</v>
       </c>
       <c r="R15" t="s">
         <v>2</v>
@@ -20679,7 +20728,7 @@
         <v>6</v>
       </c>
       <c r="W15" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X15" t="s">
         <v>8</v>
@@ -20691,21 +20740,21 @@
         <v>6</v>
       </c>
       <c r="AA15">
-        <v>1.56978</v>
+        <v>0.99786799999999998</v>
       </c>
       <c r="AC15" t="s">
         <v>17</v>
       </c>
       <c r="AD15">
         <f t="shared" si="1"/>
-        <v>1.5694999999999999</v>
+        <v>0.99881400000000009</v>
       </c>
       <c r="AG15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AH15">
         <f t="shared" si="2"/>
-        <v>1.5645500000000001</v>
+        <v>0.98858099999999993</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
@@ -20725,7 +20774,7 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -20737,14 +20786,14 @@
         <v>6</v>
       </c>
       <c r="J16">
-        <v>0.27053100000000002</v>
+        <v>0.16980999999999999</v>
       </c>
       <c r="L16" t="s">
         <v>19</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0.27024800000000004</v>
+        <v>0.16952825000000002</v>
       </c>
       <c r="R16" t="s">
         <v>2</v>
@@ -20762,7 +20811,7 @@
         <v>6</v>
       </c>
       <c r="W16" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X16" t="s">
         <v>8</v>
@@ -20774,21 +20823,21 @@
         <v>6</v>
       </c>
       <c r="AA16">
-        <v>0.27201199999999998</v>
+        <v>0.17291100000000001</v>
       </c>
       <c r="AC16" t="s">
         <v>19</v>
       </c>
       <c r="AD16">
         <f t="shared" si="1"/>
-        <v>0.27196324999999999</v>
+        <v>0.17307475</v>
       </c>
       <c r="AG16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AH16">
         <f t="shared" si="2"/>
-        <v>0.27110562500000002</v>
+        <v>0.17130150000000002</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -20808,7 +20857,7 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -20820,14 +20869,14 @@
         <v>6</v>
       </c>
       <c r="J17">
-        <v>11.6173</v>
+        <v>7.2920999999999996</v>
       </c>
       <c r="L17" t="s">
         <v>21</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>11.605174999999999</v>
+        <v>7.2800050000000001</v>
       </c>
       <c r="R17" t="s">
         <v>2</v>
@@ -20845,7 +20894,7 @@
         <v>6</v>
       </c>
       <c r="W17" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X17" t="s">
         <v>8</v>
@@ -20857,21 +20906,21 @@
         <v>6</v>
       </c>
       <c r="AA17">
-        <v>11.680999999999999</v>
+        <v>7.4252599999999997</v>
       </c>
       <c r="AC17" t="s">
         <v>21</v>
       </c>
       <c r="AD17">
         <f t="shared" si="1"/>
-        <v>11.678849999999999</v>
+        <v>7.4322949999999999</v>
       </c>
       <c r="AG17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="AH17">
         <f t="shared" si="2"/>
-        <v>11.642012499999998</v>
+        <v>7.3561500000000004</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -20891,7 +20940,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -20903,14 +20952,14 @@
         <v>6</v>
       </c>
       <c r="J18">
-        <v>4.6306200000000004</v>
+        <v>2.9066000000000001</v>
       </c>
       <c r="L18" t="s">
         <v>22</v>
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>4.6257774999999999</v>
+        <v>2.9017775000000001</v>
       </c>
       <c r="R18" t="s">
         <v>2</v>
@@ -20928,7 +20977,7 @@
         <v>6</v>
       </c>
       <c r="W18" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X18" t="s">
         <v>8</v>
@@ -20940,21 +20989,21 @@
         <v>6</v>
       </c>
       <c r="AA18">
-        <v>4.6559799999999996</v>
+        <v>2.9596800000000001</v>
       </c>
       <c r="AC18" t="s">
         <v>22</v>
       </c>
       <c r="AD18">
         <f t="shared" si="1"/>
-        <v>4.6551425000000002</v>
+        <v>2.962485</v>
       </c>
       <c r="AG18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="AH18">
         <f t="shared" si="2"/>
-        <v>4.64046</v>
+        <v>2.9321312499999999</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
@@ -20974,7 +21023,7 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -20986,14 +21035,14 @@
         <v>6</v>
       </c>
       <c r="J19">
-        <v>0.10766299999999999</v>
+        <v>6.7578899999999997E-2</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>0.10755025</v>
+        <v>6.7466875000000009E-2</v>
       </c>
       <c r="R19" t="s">
         <v>2</v>
@@ -21011,7 +21060,7 @@
         <v>6</v>
       </c>
       <c r="W19" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X19" t="s">
         <v>8</v>
@@ -21023,21 +21072,21 @@
         <v>6</v>
       </c>
       <c r="AA19">
-        <v>0.108252</v>
+        <v>6.8812999999999999E-2</v>
       </c>
       <c r="AC19" t="s">
         <v>23</v>
       </c>
       <c r="AD19">
         <f t="shared" si="1"/>
-        <v>0.10823274999999999</v>
+        <v>6.8878224999999987E-2</v>
       </c>
       <c r="AG19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AH19">
         <f t="shared" si="2"/>
-        <v>0.10789150000000002</v>
+        <v>6.8172549999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -21057,7 +21106,7 @@
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -21069,14 +21118,14 @@
         <v>6</v>
       </c>
       <c r="J20">
-        <v>0.124899</v>
+        <v>7.8397800000000004E-2</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
       </c>
       <c r="M20">
         <f t="shared" si="0"/>
-        <v>0.12476799999999999</v>
+        <v>7.8267824999999999E-2</v>
       </c>
       <c r="R20" t="s">
         <v>2</v>
@@ -21094,7 +21143,7 @@
         <v>6</v>
       </c>
       <c r="W20" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X20" t="s">
         <v>8</v>
@@ -21106,21 +21155,21 @@
         <v>6</v>
       </c>
       <c r="AA20">
-        <v>0.125583</v>
+        <v>7.9829399999999995E-2</v>
       </c>
       <c r="AC20" t="s">
         <v>24</v>
       </c>
       <c r="AD20">
         <f t="shared" si="1"/>
-        <v>0.12556</v>
+        <v>7.9905125000000007E-2</v>
       </c>
       <c r="AG20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="AH20">
         <f t="shared" si="2"/>
-        <v>0.125164</v>
+        <v>7.9086474999999989E-2</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
@@ -21140,7 +21189,7 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
@@ -21152,14 +21201,14 @@
         <v>6</v>
       </c>
       <c r="J21">
-        <v>1.5612299999999999</v>
+        <v>0.97997299999999998</v>
       </c>
       <c r="L21" t="s">
         <v>25</v>
       </c>
       <c r="M21">
         <f t="shared" si="0"/>
-        <v>1.5596000000000001</v>
+        <v>0.978348</v>
       </c>
       <c r="R21" t="s">
         <v>2</v>
@@ -21177,7 +21226,7 @@
         <v>6</v>
       </c>
       <c r="W21" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X21" t="s">
         <v>8</v>
@@ -21189,21 +21238,21 @@
         <v>6</v>
       </c>
       <c r="AA21">
-        <v>1.56978</v>
+        <v>0.99786799999999998</v>
       </c>
       <c r="AC21" t="s">
         <v>25</v>
       </c>
       <c r="AD21">
         <f t="shared" si="1"/>
-        <v>1.5694999999999999</v>
+        <v>0.99881400000000009</v>
       </c>
       <c r="AG21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AH21">
         <f t="shared" si="2"/>
-        <v>1.5645500000000001</v>
+        <v>0.98858099999999993</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -21223,7 +21272,7 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -21235,14 +21284,14 @@
         <v>6</v>
       </c>
       <c r="J22">
-        <v>0.27053100000000002</v>
+        <v>0.16980999999999999</v>
       </c>
       <c r="L22" t="s">
         <v>26</v>
       </c>
       <c r="M22">
         <f t="shared" si="0"/>
-        <v>0.27024800000000004</v>
+        <v>0.16952825000000002</v>
       </c>
       <c r="R22" t="s">
         <v>2</v>
@@ -21260,7 +21309,7 @@
         <v>6</v>
       </c>
       <c r="W22" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X22" t="s">
         <v>8</v>
@@ -21272,21 +21321,21 @@
         <v>6</v>
       </c>
       <c r="AA22">
-        <v>0.27201199999999998</v>
+        <v>0.17291100000000001</v>
       </c>
       <c r="AC22" t="s">
         <v>26</v>
       </c>
       <c r="AD22">
         <f t="shared" si="1"/>
-        <v>0.27196324999999999</v>
+        <v>0.17307475</v>
       </c>
       <c r="AG22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AH22">
         <f t="shared" si="2"/>
-        <v>0.27110562500000002</v>
+        <v>0.17130150000000002</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -21306,7 +21355,7 @@
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -21318,14 +21367,14 @@
         <v>6</v>
       </c>
       <c r="J23">
-        <v>42.761099999999999</v>
+        <v>26.840699999999998</v>
       </c>
       <c r="L23" t="s">
         <v>27</v>
       </c>
       <c r="M23">
         <f t="shared" si="0"/>
-        <v>42.716349999999998</v>
+        <v>26.796250000000001</v>
       </c>
       <c r="R23" t="s">
         <v>2</v>
@@ -21343,7 +21392,7 @@
         <v>6</v>
       </c>
       <c r="W23" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="X23" t="s">
         <v>8</v>
@@ -21355,21 +21404,21 @@
         <v>6</v>
       </c>
       <c r="AA23">
-        <v>42.9953</v>
+        <v>27.3309</v>
       </c>
       <c r="AC23" t="s">
         <v>27</v>
       </c>
       <c r="AD23">
         <f t="shared" si="1"/>
-        <v>42.987524999999998</v>
+        <v>27.3568</v>
       </c>
       <c r="AG23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AH23">
         <f t="shared" si="2"/>
-        <v>42.851937499999998</v>
+        <v>27.076524999999997</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -21377,34 +21426,34 @@
         <v>38</v>
       </c>
       <c r="J24">
-        <v>-3.9744699999999999E-4</v>
+        <v>-4.7877900000000001E-2</v>
       </c>
       <c r="L24" t="s">
         <v>38</v>
       </c>
       <c r="M24">
         <f t="shared" si="0"/>
-        <v>2.1569982499999997E-3</v>
+        <v>-4.6481124999999998E-2</v>
       </c>
       <c r="Z24" t="s">
         <v>38</v>
       </c>
       <c r="AA24">
-        <v>2.8614500000000002E-4</v>
+        <v>-4.91498E-2</v>
       </c>
       <c r="AC24" t="s">
         <v>38</v>
       </c>
       <c r="AD24">
         <f t="shared" si="1"/>
-        <v>5.3599562499999998E-3</v>
+        <v>-5.7947024999999999E-2</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="AH24">
         <f>AVERAGE(J24,J46,J68,J90,AA90,AA68,AA46,AA24)</f>
-        <v>3.75847725E-3</v>
+        <v>-5.2214074999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -21415,14 +21464,14 @@
         <v>115</v>
       </c>
       <c r="J25">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="L25" t="s">
         <v>115</v>
       </c>
       <c r="M25">
         <f t="shared" si="0"/>
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="R25" t="s">
         <v>29</v>
@@ -21431,21 +21480,21 @@
         <v>115</v>
       </c>
       <c r="AA25">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="AC25" t="s">
         <v>115</v>
       </c>
       <c r="AD25">
         <f t="shared" si="1"/>
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="AG25" s="1" t="s">
         <v>115</v>
       </c>
       <c r="AH25">
         <f t="shared" ref="AH25:AH26" si="3">AVERAGE(J25,J47,J69,J91,AA91,AA69,AA47,AA25)</f>
-        <v>0.33442600000000006</v>
+        <v>0.31414700000000001</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
@@ -21465,14 +21514,14 @@
         <v>39</v>
       </c>
       <c r="J26">
-        <v>3.08154E-2</v>
+        <v>4.0468200000000003E-2</v>
       </c>
       <c r="L26" t="s">
         <v>39</v>
       </c>
       <c r="M26">
         <f t="shared" si="0"/>
-        <v>2.9824650000000001E-2</v>
+        <v>3.7707550000000006E-2</v>
       </c>
       <c r="R26" t="s">
         <v>2</v>
@@ -21490,21 +21539,21 @@
         <v>39</v>
       </c>
       <c r="AA26">
-        <v>2.4127599999999999E-2</v>
+        <v>6.3648700000000002E-2</v>
       </c>
       <c r="AC26" t="s">
         <v>39</v>
       </c>
       <c r="AD26">
         <f t="shared" si="1"/>
-        <v>3.7135250000000002E-2</v>
+        <v>6.457727499999999E-2</v>
       </c>
       <c r="AG26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AH26">
         <f t="shared" si="3"/>
-        <v>3.3479950000000001E-2</v>
+        <v>5.1142412499999998E-2</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
@@ -21527,14 +21576,14 @@
         <v>38</v>
       </c>
       <c r="G27" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="H27" t="s">
         <v>39</v>
       </c>
       <c r="I27">
-        <f>-0.0297241</f>
-        <v>-2.97241E-2</v>
+        <f>-0.0274401</f>
+        <v>-2.7440099999999999E-2</v>
       </c>
       <c r="R27" t="s">
         <v>2</v>
@@ -21555,14 +21604,14 @@
         <v>38</v>
       </c>
       <c r="X27" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="Y27" t="s">
         <v>39</v>
       </c>
       <c r="Z27">
-        <f>-0.032391</f>
-        <v>-3.2391000000000003E-2</v>
+        <f>-0.0610823</f>
+        <v>-6.1082299999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -21579,7 +21628,7 @@
         <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="R28" t="s">
         <v>2</v>
@@ -21594,7 +21643,7 @@
         <v>42</v>
       </c>
       <c r="V28" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
@@ -21645,7 +21694,7 @@
         <v>48</v>
       </c>
       <c r="E31">
-        <v>0.74256999999999995</v>
+        <v>1.55277</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -21660,7 +21709,7 @@
         <v>48</v>
       </c>
       <c r="V31">
-        <v>1.3371</v>
+        <v>2.8892799999999998</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -21680,7 +21729,7 @@
         <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
@@ -21692,7 +21741,7 @@
         <v>6</v>
       </c>
       <c r="J32">
-        <v>14.654199999999999</v>
+        <v>9.1844800000000006</v>
       </c>
       <c r="R32" t="s">
         <v>2</v>
@@ -21710,7 +21759,7 @@
         <v>6</v>
       </c>
       <c r="W32" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="X32" t="s">
         <v>8</v>
@@ -21722,7 +21771,7 @@
         <v>6</v>
       </c>
       <c r="AA32">
-        <v>14.747199999999999</v>
+        <v>9.3934099999999994</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.25">
@@ -21742,7 +21791,7 @@
         <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G33" t="s">
         <v>8</v>
@@ -21754,7 +21803,7 @@
         <v>6</v>
       </c>
       <c r="J33">
-        <v>11.5738</v>
+        <v>7.2538499999999999</v>
       </c>
       <c r="R33" t="s">
         <v>2</v>
@@ -21772,7 +21821,7 @@
         <v>6</v>
       </c>
       <c r="W33" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X33" t="s">
         <v>8</v>
@@ -21784,7 +21833,7 @@
         <v>6</v>
       </c>
       <c r="AA33">
-        <v>11.6472</v>
+        <v>7.4188599999999996</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
@@ -21804,7 +21853,7 @@
         <v>6</v>
       </c>
       <c r="F34" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G34" t="s">
         <v>8</v>
@@ -21816,7 +21865,7 @@
         <v>6</v>
       </c>
       <c r="J34">
-        <v>4.6132799999999996</v>
+        <v>2.8913500000000001</v>
       </c>
       <c r="R34" t="s">
         <v>2</v>
@@ -21834,7 +21883,7 @@
         <v>6</v>
       </c>
       <c r="W34" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X34" t="s">
         <v>8</v>
@@ -21846,7 +21895,7 @@
         <v>6</v>
       </c>
       <c r="AA34">
-        <v>4.6425400000000003</v>
+        <v>2.9571299999999998</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
@@ -21866,7 +21915,7 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G35" t="s">
         <v>8</v>
@@ -21878,7 +21927,7 @@
         <v>6</v>
       </c>
       <c r="J35">
-        <v>0.10725999999999999</v>
+        <v>6.7224500000000006E-2</v>
       </c>
       <c r="R35" t="s">
         <v>2</v>
@@ -21896,7 +21945,7 @@
         <v>6</v>
       </c>
       <c r="W35" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X35" t="s">
         <v>8</v>
@@ -21908,7 +21957,7 @@
         <v>6</v>
       </c>
       <c r="AA35">
-        <v>0.10793999999999999</v>
+        <v>6.8753700000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -21928,7 +21977,7 @@
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G36" t="s">
         <v>8</v>
@@ -21940,7 +21989,7 @@
         <v>6</v>
       </c>
       <c r="J36">
-        <v>0.124431</v>
+        <v>7.7986600000000003E-2</v>
       </c>
       <c r="R36" t="s">
         <v>2</v>
@@ -21958,7 +22007,7 @@
         <v>6</v>
       </c>
       <c r="W36" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X36" t="s">
         <v>8</v>
@@ -21970,7 +22019,7 @@
         <v>6</v>
       </c>
       <c r="AA36">
-        <v>0.12522</v>
+        <v>7.9760700000000004E-2</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -21990,7 +22039,7 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -22002,7 +22051,7 @@
         <v>6</v>
       </c>
       <c r="J37">
-        <v>1.5553900000000001</v>
+        <v>0.97483299999999995</v>
       </c>
       <c r="R37" t="s">
         <v>2</v>
@@ -22020,7 +22069,7 @@
         <v>6</v>
       </c>
       <c r="W37" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X37" t="s">
         <v>8</v>
@@ -22032,7 +22081,7 @@
         <v>6</v>
       </c>
       <c r="AA37">
-        <v>1.56525</v>
+        <v>0.99700800000000001</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
@@ -22052,7 +22101,7 @@
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G38" t="s">
         <v>8</v>
@@ -22064,7 +22113,7 @@
         <v>6</v>
       </c>
       <c r="J38">
-        <v>0.26951799999999998</v>
+        <v>0.16891900000000001</v>
       </c>
       <c r="R38" t="s">
         <v>2</v>
@@ -22082,7 +22131,7 @@
         <v>6</v>
       </c>
       <c r="W38" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X38" t="s">
         <v>8</v>
@@ -22094,7 +22143,7 @@
         <v>6</v>
       </c>
       <c r="AA38">
-        <v>0.271227</v>
+        <v>0.172762</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
@@ -22114,7 +22163,7 @@
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G39" t="s">
         <v>8</v>
@@ -22126,7 +22175,7 @@
         <v>6</v>
       </c>
       <c r="J39">
-        <v>11.5738</v>
+        <v>7.2538499999999999</v>
       </c>
       <c r="R39" t="s">
         <v>2</v>
@@ -22144,7 +22193,7 @@
         <v>6</v>
       </c>
       <c r="W39" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X39" t="s">
         <v>8</v>
@@ -22156,7 +22205,7 @@
         <v>6</v>
       </c>
       <c r="AA39">
-        <v>11.6472</v>
+        <v>7.4188599999999996</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -22176,7 +22225,7 @@
         <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G40" t="s">
         <v>8</v>
@@ -22188,7 +22237,7 @@
         <v>6</v>
       </c>
       <c r="J40">
-        <v>4.6132799999999996</v>
+        <v>2.8913500000000001</v>
       </c>
       <c r="R40" t="s">
         <v>2</v>
@@ -22206,7 +22255,7 @@
         <v>6</v>
       </c>
       <c r="W40" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X40" t="s">
         <v>8</v>
@@ -22218,7 +22267,7 @@
         <v>6</v>
       </c>
       <c r="AA40">
-        <v>4.6425400000000003</v>
+        <v>2.9571299999999998</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -22238,7 +22287,7 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G41" t="s">
         <v>8</v>
@@ -22250,7 +22299,7 @@
         <v>6</v>
       </c>
       <c r="J41">
-        <v>0.10725999999999999</v>
+        <v>6.7224500000000006E-2</v>
       </c>
       <c r="R41" t="s">
         <v>2</v>
@@ -22268,7 +22317,7 @@
         <v>6</v>
       </c>
       <c r="W41" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X41" t="s">
         <v>8</v>
@@ -22280,7 +22329,7 @@
         <v>6</v>
       </c>
       <c r="AA41">
-        <v>0.10793999999999999</v>
+        <v>6.8753700000000001E-2</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -22300,7 +22349,7 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G42" t="s">
         <v>8</v>
@@ -22312,7 +22361,7 @@
         <v>6</v>
       </c>
       <c r="J42">
-        <v>0.124431</v>
+        <v>7.7986600000000003E-2</v>
       </c>
       <c r="R42" t="s">
         <v>2</v>
@@ -22330,7 +22379,7 @@
         <v>6</v>
       </c>
       <c r="W42" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X42" t="s">
         <v>8</v>
@@ -22342,7 +22391,7 @@
         <v>6</v>
       </c>
       <c r="AA42">
-        <v>0.12522</v>
+        <v>7.9760700000000004E-2</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
@@ -22362,7 +22411,7 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
@@ -22374,7 +22423,7 @@
         <v>6</v>
       </c>
       <c r="J43">
-        <v>1.5553900000000001</v>
+        <v>0.97483299999999995</v>
       </c>
       <c r="R43" t="s">
         <v>2</v>
@@ -22392,7 +22441,7 @@
         <v>6</v>
       </c>
       <c r="W43" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X43" t="s">
         <v>8</v>
@@ -22404,7 +22453,7 @@
         <v>6</v>
       </c>
       <c r="AA43">
-        <v>1.56525</v>
+        <v>0.99700800000000001</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -22424,7 +22473,7 @@
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G44" t="s">
         <v>8</v>
@@ -22436,7 +22485,7 @@
         <v>6</v>
       </c>
       <c r="J44">
-        <v>0.26951799999999998</v>
+        <v>0.16891900000000001</v>
       </c>
       <c r="R44" t="s">
         <v>2</v>
@@ -22454,7 +22503,7 @@
         <v>6</v>
       </c>
       <c r="W44" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X44" t="s">
         <v>8</v>
@@ -22466,7 +22515,7 @@
         <v>6</v>
       </c>
       <c r="AA44">
-        <v>0.271227</v>
+        <v>0.172762</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -22486,7 +22535,7 @@
         <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G45" t="s">
         <v>8</v>
@@ -22498,7 +22547,7 @@
         <v>6</v>
       </c>
       <c r="J45">
-        <v>42.600900000000003</v>
+        <v>26.7</v>
       </c>
       <c r="R45" t="s">
         <v>2</v>
@@ -22516,7 +22565,7 @@
         <v>6</v>
       </c>
       <c r="W45" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="X45" t="s">
         <v>8</v>
@@ -22528,7 +22577,7 @@
         <v>6</v>
       </c>
       <c r="AA45">
-        <v>42.871099999999998</v>
+        <v>27.307300000000001</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -22536,13 +22585,13 @@
         <v>38</v>
       </c>
       <c r="J46">
-        <v>5.5972799999999996E-3</v>
+        <v>-5.1364100000000003E-2</v>
       </c>
       <c r="Z46" t="s">
         <v>38</v>
       </c>
       <c r="AA46">
-        <v>1.5821499999999999E-2</v>
+        <v>-6.0274300000000003E-2</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -22553,7 +22602,7 @@
         <v>115</v>
       </c>
       <c r="J47">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="R47" t="s">
         <v>30</v>
@@ -22562,7 +22611,7 @@
         <v>115</v>
       </c>
       <c r="AA47">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -22582,7 +22631,7 @@
         <v>39</v>
       </c>
       <c r="J48">
-        <v>2.97241E-2</v>
+        <v>2.7440099999999999E-2</v>
       </c>
       <c r="R48" t="s">
         <v>2</v>
@@ -22600,7 +22649,7 @@
         <v>39</v>
       </c>
       <c r="AA48">
-        <v>3.2391000000000003E-2</v>
+        <v>6.1082299999999999E-2</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
@@ -22623,14 +22672,14 @@
         <v>38</v>
       </c>
       <c r="G49" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="H49" t="s">
         <v>39</v>
       </c>
       <c r="I49">
-        <f>-0.0320484</f>
-        <v>-3.2048399999999998E-2</v>
+        <f>-0.0417722</f>
+        <v>-4.1772200000000002E-2</v>
       </c>
       <c r="R49" t="s">
         <v>2</v>
@@ -22651,14 +22700,14 @@
         <v>38</v>
       </c>
       <c r="X49" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="Y49" t="s">
         <v>39</v>
       </c>
       <c r="Z49">
-        <f>-0.0527004</f>
-        <v>-5.2700400000000001E-2</v>
+        <f>-0.0676044</f>
+        <v>-6.7604399999999995E-2</v>
       </c>
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.25">
@@ -22675,7 +22724,7 @@
         <v>42</v>
       </c>
       <c r="E50" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="R50" t="s">
         <v>2</v>
@@ -22690,7 +22739,7 @@
         <v>42</v>
       </c>
       <c r="V50" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
@@ -22741,7 +22790,7 @@
         <v>48</v>
       </c>
       <c r="E53">
-        <v>1.0434600000000001</v>
+        <v>1.6167800000000001</v>
       </c>
       <c r="R53" t="s">
         <v>2</v>
@@ -22756,7 +22805,7 @@
         <v>48</v>
       </c>
       <c r="V53">
-        <v>1.70855</v>
+        <v>3.1208200000000001</v>
       </c>
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.25">
@@ -22776,7 +22825,7 @@
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G54" t="s">
         <v>8</v>
@@ -22788,7 +22837,7 @@
         <v>6</v>
       </c>
       <c r="J54">
-        <v>14.7013</v>
+        <v>9.1944900000000001</v>
       </c>
       <c r="R54" t="s">
         <v>2</v>
@@ -22806,7 +22855,7 @@
         <v>6</v>
       </c>
       <c r="W54" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="X54" t="s">
         <v>8</v>
@@ -22818,7 +22867,7 @@
         <v>6</v>
       </c>
       <c r="AA54">
-        <v>14.805199999999999</v>
+        <v>9.4296100000000003</v>
       </c>
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.25">
@@ -22838,7 +22887,7 @@
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G55" t="s">
         <v>8</v>
@@ -22850,7 +22899,7 @@
         <v>6</v>
       </c>
       <c r="J55">
-        <v>11.611000000000001</v>
+        <v>7.2617500000000001</v>
       </c>
       <c r="R55" t="s">
         <v>2</v>
@@ -22868,7 +22917,7 @@
         <v>6</v>
       </c>
       <c r="W55" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X55" t="s">
         <v>8</v>
@@ -22880,7 +22929,7 @@
         <v>6</v>
       </c>
       <c r="AA55">
-        <v>11.693099999999999</v>
+        <v>7.4474400000000003</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
@@ -22900,7 +22949,7 @@
         <v>6</v>
       </c>
       <c r="F56" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G56" t="s">
         <v>8</v>
@@ -22912,7 +22961,7 @@
         <v>6</v>
       </c>
       <c r="J56">
-        <v>4.6280900000000003</v>
+        <v>2.8944999999999999</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -22930,7 +22979,7 @@
         <v>6</v>
       </c>
       <c r="W56" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X56" t="s">
         <v>8</v>
@@ -22942,7 +22991,7 @@
         <v>6</v>
       </c>
       <c r="AA56">
-        <v>4.6608200000000002</v>
+        <v>2.9685199999999998</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -22962,7 +23011,7 @@
         <v>6</v>
       </c>
       <c r="F57" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G57" t="s">
         <v>8</v>
@@ -22974,7 +23023,7 @@
         <v>6</v>
       </c>
       <c r="J57">
-        <v>0.10760400000000001</v>
+        <v>6.7297700000000002E-2</v>
       </c>
       <c r="R57" t="s">
         <v>2</v>
@@ -22992,7 +23041,7 @@
         <v>6</v>
       </c>
       <c r="W57" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X57" t="s">
         <v>8</v>
@@ -23004,7 +23053,7 @@
         <v>6</v>
       </c>
       <c r="AA57">
-        <v>0.108365</v>
+        <v>6.9018599999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
@@ -23024,7 +23073,7 @@
         <v>6</v>
       </c>
       <c r="F58" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G58" t="s">
         <v>8</v>
@@ -23036,7 +23085,7 @@
         <v>6</v>
       </c>
       <c r="J58">
-        <v>0.12483</v>
+        <v>7.8071600000000005E-2</v>
       </c>
       <c r="R58" t="s">
         <v>2</v>
@@ -23054,7 +23103,7 @@
         <v>6</v>
       </c>
       <c r="W58" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X58" t="s">
         <v>8</v>
@@ -23066,7 +23115,7 @@
         <v>6</v>
       </c>
       <c r="AA58">
-        <v>0.12571299999999999</v>
+        <v>8.0068E-2</v>
       </c>
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.25">
@@ -23086,7 +23135,7 @@
         <v>6</v>
       </c>
       <c r="F59" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G59" t="s">
         <v>8</v>
@@ -23098,7 +23147,7 @@
         <v>6</v>
       </c>
       <c r="J59">
-        <v>1.5603800000000001</v>
+        <v>0.97589499999999996</v>
       </c>
       <c r="R59" t="s">
         <v>2</v>
@@ -23116,7 +23165,7 @@
         <v>6</v>
       </c>
       <c r="W59" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X59" t="s">
         <v>8</v>
@@ -23128,7 +23177,7 @@
         <v>6</v>
       </c>
       <c r="AA59">
-        <v>1.57141</v>
+        <v>1.00085</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
@@ -23148,7 +23197,7 @@
         <v>6</v>
       </c>
       <c r="F60" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G60" t="s">
         <v>8</v>
@@ -23160,7 +23209,7 @@
         <v>6</v>
       </c>
       <c r="J60">
-        <v>0.27038299999999998</v>
+        <v>0.169103</v>
       </c>
       <c r="R60" t="s">
         <v>2</v>
@@ -23178,7 +23227,7 @@
         <v>6</v>
       </c>
       <c r="W60" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X60" t="s">
         <v>8</v>
@@ -23190,7 +23239,7 @@
         <v>6</v>
       </c>
       <c r="AA60">
-        <v>0.27229500000000001</v>
+        <v>0.173427</v>
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
@@ -23210,7 +23259,7 @@
         <v>6</v>
       </c>
       <c r="F61" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G61" t="s">
         <v>8</v>
@@ -23222,7 +23271,7 @@
         <v>6</v>
       </c>
       <c r="J61">
-        <v>11.611000000000001</v>
+        <v>7.2617500000000001</v>
       </c>
       <c r="R61" t="s">
         <v>2</v>
@@ -23240,7 +23289,7 @@
         <v>6</v>
       </c>
       <c r="W61" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X61" t="s">
         <v>8</v>
@@ -23252,7 +23301,7 @@
         <v>6</v>
       </c>
       <c r="AA61">
-        <v>11.693099999999999</v>
+        <v>7.4474400000000003</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
@@ -23272,7 +23321,7 @@
         <v>6</v>
       </c>
       <c r="F62" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G62" t="s">
         <v>8</v>
@@ -23284,7 +23333,7 @@
         <v>6</v>
       </c>
       <c r="J62">
-        <v>4.6280900000000003</v>
+        <v>2.8944999999999999</v>
       </c>
       <c r="R62" t="s">
         <v>2</v>
@@ -23302,7 +23351,7 @@
         <v>6</v>
       </c>
       <c r="W62" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X62" t="s">
         <v>8</v>
@@ -23314,7 +23363,7 @@
         <v>6</v>
       </c>
       <c r="AA62">
-        <v>4.6608200000000002</v>
+        <v>2.9685199999999998</v>
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
@@ -23334,7 +23383,7 @@
         <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G63" t="s">
         <v>8</v>
@@ -23346,7 +23395,7 @@
         <v>6</v>
       </c>
       <c r="J63">
-        <v>0.10760400000000001</v>
+        <v>6.7297700000000002E-2</v>
       </c>
       <c r="R63" t="s">
         <v>2</v>
@@ -23364,7 +23413,7 @@
         <v>6</v>
       </c>
       <c r="W63" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X63" t="s">
         <v>8</v>
@@ -23376,7 +23425,7 @@
         <v>6</v>
       </c>
       <c r="AA63">
-        <v>0.108365</v>
+        <v>6.9018599999999999E-2</v>
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
@@ -23396,7 +23445,7 @@
         <v>6</v>
       </c>
       <c r="F64" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G64" t="s">
         <v>8</v>
@@ -23408,7 +23457,7 @@
         <v>6</v>
       </c>
       <c r="J64">
-        <v>0.12483</v>
+        <v>7.8071600000000005E-2</v>
       </c>
       <c r="R64" t="s">
         <v>2</v>
@@ -23426,7 +23475,7 @@
         <v>6</v>
       </c>
       <c r="W64" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X64" t="s">
         <v>8</v>
@@ -23438,7 +23487,7 @@
         <v>6</v>
       </c>
       <c r="AA64">
-        <v>0.12571299999999999</v>
+        <v>8.0068E-2</v>
       </c>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
@@ -23458,7 +23507,7 @@
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G65" t="s">
         <v>8</v>
@@ -23470,7 +23519,7 @@
         <v>6</v>
       </c>
       <c r="J65">
-        <v>1.5603800000000001</v>
+        <v>0.97589499999999996</v>
       </c>
       <c r="R65" t="s">
         <v>2</v>
@@ -23488,7 +23537,7 @@
         <v>6</v>
       </c>
       <c r="W65" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X65" t="s">
         <v>8</v>
@@ -23500,7 +23549,7 @@
         <v>6</v>
       </c>
       <c r="AA65">
-        <v>1.57141</v>
+        <v>1.00085</v>
       </c>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
@@ -23520,7 +23569,7 @@
         <v>6</v>
       </c>
       <c r="F66" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G66" t="s">
         <v>8</v>
@@ -23532,7 +23581,7 @@
         <v>6</v>
       </c>
       <c r="J66">
-        <v>0.27038299999999998</v>
+        <v>0.169103</v>
       </c>
       <c r="R66" t="s">
         <v>2</v>
@@ -23550,7 +23599,7 @@
         <v>6</v>
       </c>
       <c r="W66" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X66" t="s">
         <v>8</v>
@@ -23562,7 +23611,7 @@
         <v>6</v>
       </c>
       <c r="AA66">
-        <v>0.27229500000000001</v>
+        <v>0.173427</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
@@ -23582,7 +23631,7 @@
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G67" t="s">
         <v>8</v>
@@ -23594,7 +23643,7 @@
         <v>6</v>
       </c>
       <c r="J67">
-        <v>42.737699999999997</v>
+        <v>26.729099999999999</v>
       </c>
       <c r="R67" t="s">
         <v>2</v>
@@ -23612,7 +23661,7 @@
         <v>6</v>
       </c>
       <c r="W67" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="X67" t="s">
         <v>8</v>
@@ -23624,7 +23673,7 @@
         <v>6</v>
       </c>
       <c r="AA67">
-        <v>43.039900000000003</v>
+        <v>27.412600000000001</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
@@ -23632,13 +23681,13 @@
         <v>38</v>
       </c>
       <c r="J68">
-        <v>5.36924E-3</v>
+        <v>-4.3462199999999999E-2</v>
       </c>
       <c r="Z68" t="s">
         <v>38</v>
       </c>
       <c r="AA68">
-        <v>1.4995099999999999E-3</v>
+        <v>-5.9690800000000002E-2</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
@@ -23649,7 +23698,7 @@
         <v>115</v>
       </c>
       <c r="J69">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="R69" t="s">
         <v>49</v>
@@ -23658,7 +23707,7 @@
         <v>115</v>
       </c>
       <c r="AA69">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -23678,7 +23727,7 @@
         <v>39</v>
       </c>
       <c r="J70">
-        <v>3.2048399999999998E-2</v>
+        <v>4.1772200000000002E-2</v>
       </c>
       <c r="R70" t="s">
         <v>2</v>
@@ -23696,7 +23745,7 @@
         <v>39</v>
       </c>
       <c r="AA70">
-        <v>5.2700400000000001E-2</v>
+        <v>6.7604399999999995E-2</v>
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
@@ -23719,14 +23768,14 @@
         <v>38</v>
       </c>
       <c r="G71" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="H71" t="s">
         <v>39</v>
       </c>
       <c r="I71">
-        <f>-0.0267107</f>
-        <v>-2.67107E-2</v>
+        <f>-0.0411497</f>
+        <v>-4.1149699999999997E-2</v>
       </c>
       <c r="R71" t="s">
         <v>2</v>
@@ -23747,14 +23796,14 @@
         <v>38</v>
       </c>
       <c r="X71" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="Y71" t="s">
         <v>39</v>
       </c>
       <c r="Z71">
-        <f>-0.039322</f>
-        <v>-3.9322000000000003E-2</v>
+        <f>-0.0659737</f>
+        <v>-6.5973699999999996E-2</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
@@ -23771,7 +23820,7 @@
         <v>42</v>
       </c>
       <c r="E72" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="R72" t="s">
         <v>2</v>
@@ -23786,7 +23835,7 @@
         <v>42</v>
       </c>
       <c r="V72" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
@@ -23837,7 +23886,7 @@
         <v>48</v>
       </c>
       <c r="E75">
-        <v>1.10507</v>
+        <v>2.0263900000000001</v>
       </c>
       <c r="R75" t="s">
         <v>2</v>
@@ -23852,7 +23901,7 @@
         <v>48</v>
       </c>
       <c r="V75">
-        <v>1.7170300000000001</v>
+        <v>3.04128</v>
       </c>
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.25">
@@ -23872,7 +23921,7 @@
         <v>6</v>
       </c>
       <c r="F76" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="G76" t="s">
         <v>8</v>
@@ -23884,7 +23933,7 @@
         <v>6</v>
       </c>
       <c r="J76">
-        <v>14.710900000000001</v>
+        <v>9.2585200000000007</v>
       </c>
       <c r="R76" t="s">
         <v>2</v>
@@ -23902,7 +23951,7 @@
         <v>6</v>
       </c>
       <c r="W76" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
       <c r="X76" t="s">
         <v>8</v>
@@ -23914,7 +23963,7 @@
         <v>6</v>
       </c>
       <c r="AA76">
-        <v>14.8066</v>
+        <v>9.4171700000000005</v>
       </c>
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.25">
@@ -23934,7 +23983,7 @@
         <v>6</v>
       </c>
       <c r="F77" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G77" t="s">
         <v>8</v>
@@ -23946,7 +23995,7 @@
         <v>6</v>
       </c>
       <c r="J77">
-        <v>11.618600000000001</v>
+        <v>7.3123199999999997</v>
       </c>
       <c r="R77" t="s">
         <v>2</v>
@@ -23964,7 +24013,7 @@
         <v>6</v>
       </c>
       <c r="W77" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X77" t="s">
         <v>8</v>
@@ -23976,7 +24025,7 @@
         <v>6</v>
       </c>
       <c r="AA77">
-        <v>11.694100000000001</v>
+        <v>7.4376199999999999</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
@@ -23996,7 +24045,7 @@
         <v>6</v>
       </c>
       <c r="F78" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G78" t="s">
         <v>8</v>
@@ -24008,7 +24057,7 @@
         <v>6</v>
       </c>
       <c r="J78">
-        <v>4.6311200000000001</v>
+        <v>2.91466</v>
       </c>
       <c r="R78" t="s">
         <v>2</v>
@@ -24026,7 +24075,7 @@
         <v>6</v>
       </c>
       <c r="W78" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X78" t="s">
         <v>8</v>
@@ -24038,7 +24087,7 @@
         <v>6</v>
       </c>
       <c r="AA78">
-        <v>4.6612299999999998</v>
+        <v>2.96461</v>
       </c>
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.25">
@@ -24058,7 +24107,7 @@
         <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G79" t="s">
         <v>8</v>
@@ -24070,7 +24119,7 @@
         <v>6</v>
       </c>
       <c r="J79">
-        <v>0.10767400000000001</v>
+        <v>6.7766400000000004E-2</v>
       </c>
       <c r="R79" t="s">
         <v>2</v>
@@ -24088,7 +24137,7 @@
         <v>6</v>
       </c>
       <c r="W79" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X79" t="s">
         <v>8</v>
@@ -24100,7 +24149,7 @@
         <v>6</v>
       </c>
       <c r="AA79">
-        <v>0.108374</v>
+        <v>6.8927600000000006E-2</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.25">
@@ -24120,7 +24169,7 @@
         <v>6</v>
       </c>
       <c r="F80" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G80" t="s">
         <v>8</v>
@@ -24132,7 +24181,7 @@
         <v>6</v>
       </c>
       <c r="J80">
-        <v>0.124912</v>
+        <v>7.8615299999999999E-2</v>
       </c>
       <c r="R80" t="s">
         <v>2</v>
@@ -24150,7 +24199,7 @@
         <v>6</v>
       </c>
       <c r="W80" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X80" t="s">
         <v>8</v>
@@ -24162,7 +24211,7 @@
         <v>6</v>
       </c>
       <c r="AA80">
-        <v>0.125724</v>
+        <v>7.9962400000000003E-2</v>
       </c>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
@@ -24182,7 +24231,7 @@
         <v>6</v>
       </c>
       <c r="F81" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G81" t="s">
         <v>8</v>
@@ -24194,7 +24243,7 @@
         <v>6</v>
       </c>
       <c r="J81">
-        <v>1.5613999999999999</v>
+        <v>0.98269099999999998</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -24212,7 +24261,7 @@
         <v>6</v>
       </c>
       <c r="W81" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X81" t="s">
         <v>8</v>
@@ -24224,7 +24273,7 @@
         <v>6</v>
       </c>
       <c r="AA81">
-        <v>1.5715600000000001</v>
+        <v>0.99953000000000003</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -24244,7 +24293,7 @@
         <v>6</v>
       </c>
       <c r="F82" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G82" t="s">
         <v>8</v>
@@ -24256,7 +24305,7 @@
         <v>6</v>
       </c>
       <c r="J82">
-        <v>0.27056000000000002</v>
+        <v>0.17028099999999999</v>
       </c>
       <c r="R82" t="s">
         <v>2</v>
@@ -24274,7 +24323,7 @@
         <v>6</v>
       </c>
       <c r="W82" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X82" t="s">
         <v>8</v>
@@ -24286,7 +24335,7 @@
         <v>6</v>
       </c>
       <c r="AA82">
-        <v>0.27231899999999998</v>
+        <v>0.17319899999999999</v>
       </c>
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.25">
@@ -24306,7 +24355,7 @@
         <v>6</v>
       </c>
       <c r="F83" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="G83" t="s">
         <v>8</v>
@@ -24318,7 +24367,7 @@
         <v>6</v>
       </c>
       <c r="J83">
-        <v>11.618600000000001</v>
+        <v>7.3123199999999997</v>
       </c>
       <c r="R83" t="s">
         <v>2</v>
@@ -24336,7 +24385,7 @@
         <v>6</v>
       </c>
       <c r="W83" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
       <c r="X83" t="s">
         <v>8</v>
@@ -24348,7 +24397,7 @@
         <v>6</v>
       </c>
       <c r="AA83">
-        <v>11.694100000000001</v>
+        <v>7.4376199999999999</v>
       </c>
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.25">
@@ -24368,7 +24417,7 @@
         <v>6</v>
       </c>
       <c r="F84" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="G84" t="s">
         <v>8</v>
@@ -24380,7 +24429,7 @@
         <v>6</v>
       </c>
       <c r="J84">
-        <v>4.6311200000000001</v>
+        <v>2.91466</v>
       </c>
       <c r="R84" t="s">
         <v>2</v>
@@ -24398,7 +24447,7 @@
         <v>6</v>
       </c>
       <c r="W84" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="X84" t="s">
         <v>8</v>
@@ -24410,7 +24459,7 @@
         <v>6</v>
       </c>
       <c r="AA84">
-        <v>4.6612299999999998</v>
+        <v>2.96461</v>
       </c>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
@@ -24430,7 +24479,7 @@
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="G85" t="s">
         <v>8</v>
@@ -24442,7 +24491,7 @@
         <v>6</v>
       </c>
       <c r="J85">
-        <v>0.10767400000000001</v>
+        <v>6.7766400000000004E-2</v>
       </c>
       <c r="R85" t="s">
         <v>2</v>
@@ -24460,7 +24509,7 @@
         <v>6</v>
       </c>
       <c r="W85" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="X85" t="s">
         <v>8</v>
@@ -24472,7 +24521,7 @@
         <v>6</v>
       </c>
       <c r="AA85">
-        <v>0.108374</v>
+        <v>6.8927600000000006E-2</v>
       </c>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
@@ -24492,7 +24541,7 @@
         <v>6</v>
       </c>
       <c r="F86" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G86" t="s">
         <v>8</v>
@@ -24504,7 +24553,7 @@
         <v>6</v>
       </c>
       <c r="J86">
-        <v>0.124912</v>
+        <v>7.8615299999999999E-2</v>
       </c>
       <c r="R86" t="s">
         <v>2</v>
@@ -24522,7 +24571,7 @@
         <v>6</v>
       </c>
       <c r="W86" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="X86" t="s">
         <v>8</v>
@@ -24534,7 +24583,7 @@
         <v>6</v>
       </c>
       <c r="AA86">
-        <v>0.125724</v>
+        <v>7.9962400000000003E-2</v>
       </c>
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
@@ -24554,7 +24603,7 @@
         <v>6</v>
       </c>
       <c r="F87" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="G87" t="s">
         <v>8</v>
@@ -24566,7 +24615,7 @@
         <v>6</v>
       </c>
       <c r="J87">
-        <v>1.5613999999999999</v>
+        <v>0.98269099999999998</v>
       </c>
       <c r="R87" t="s">
         <v>2</v>
@@ -24584,7 +24633,7 @@
         <v>6</v>
       </c>
       <c r="W87" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="X87" t="s">
         <v>8</v>
@@ -24596,7 +24645,7 @@
         <v>6</v>
       </c>
       <c r="AA87">
-        <v>1.5715600000000001</v>
+        <v>0.99953000000000003</v>
       </c>
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
@@ -24616,7 +24665,7 @@
         <v>6</v>
       </c>
       <c r="F88" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="G88" t="s">
         <v>8</v>
@@ -24628,7 +24677,7 @@
         <v>6</v>
       </c>
       <c r="J88">
-        <v>0.27056000000000002</v>
+        <v>0.17028099999999999</v>
       </c>
       <c r="R88" t="s">
         <v>2</v>
@@ -24646,7 +24695,7 @@
         <v>6</v>
       </c>
       <c r="W88" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="X88" t="s">
         <v>8</v>
@@ -24658,7 +24707,7 @@
         <v>6</v>
       </c>
       <c r="AA88">
-        <v>0.27231899999999998</v>
+        <v>0.17319899999999999</v>
       </c>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
@@ -24678,7 +24727,7 @@
         <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="G89" t="s">
         <v>8</v>
@@ -24690,7 +24739,7 @@
         <v>6</v>
       </c>
       <c r="J89">
-        <v>42.765700000000002</v>
+        <v>26.915199999999999</v>
       </c>
       <c r="R89" t="s">
         <v>2</v>
@@ -24708,7 +24757,7 @@
         <v>6</v>
       </c>
       <c r="W89" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="X89" t="s">
         <v>8</v>
@@ -24720,7 +24769,7 @@
         <v>6</v>
       </c>
       <c r="AA89">
-        <v>43.043799999999997</v>
+        <v>27.3764</v>
       </c>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
@@ -24728,13 +24777,13 @@
         <v>38</v>
       </c>
       <c r="J90">
-        <v>-1.94108E-3</v>
+        <v>-4.3220300000000003E-2</v>
       </c>
       <c r="Z90" t="s">
         <v>38</v>
       </c>
       <c r="AA90">
-        <v>3.8326699999999998E-3</v>
+        <v>-6.2673199999999998E-2</v>
       </c>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
@@ -24742,13 +24791,13 @@
         <v>115</v>
       </c>
       <c r="J91">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
       <c r="Z91" t="s">
         <v>115</v>
       </c>
       <c r="AA91">
-        <v>0.334426</v>
+        <v>0.31414700000000001</v>
       </c>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
@@ -24756,13 +24805,13 @@
         <v>39</v>
       </c>
       <c r="J92">
-        <v>2.67107E-2</v>
+        <v>4.1149699999999997E-2</v>
       </c>
       <c r="Z92" t="s">
         <v>39</v>
       </c>
       <c r="AA92">
-        <v>3.9322000000000003E-2</v>
+        <v>6.5973699999999996E-2</v>
       </c>
     </row>
   </sheetData>
@@ -24771,12 +24820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE1E5043F2CF384FB5FE4BAABF9D3983" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0614cff9d23b461af25b2cda1cf9368">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="386adf9787ee73c67b04c35b5de66464">
     <xsd:element name="properties">
@@ -24890,7 +24933,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -24899,22 +24942,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15B9ACA7-37DF-4944-968A-289D2787D7C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24930,10 +24964,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
just opened and resaved this. May need to check on subject 1, 4, and 7 to make sure no one got overwritten
</commit_message>
<xml_diff>
--- a/RRAMassMods.xlsx
+++ b/RRAMassMods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BE6EA4-07A5-4F6F-B751-6A9C0283F494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB25416-573B-4BF6-9D78-B09F08D55CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="2430" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
+    <workbookView xWindow="6210" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="welk001" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="welk007" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20041,7 +20040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FE46D1-E00B-478F-BC49-0EAED21FA345}">
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AD28" workbookViewId="0">
       <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
@@ -24820,6 +24819,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE1E5043F2CF384FB5FE4BAABF9D3983" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0614cff9d23b461af25b2cda1cf9368">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="386adf9787ee73c67b04c35b5de66464">
     <xsd:element name="properties">
@@ -24933,15 +24941,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -24949,6 +24948,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15B9ACA7-37DF-4944-968A-289D2787D7C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24960,14 +24967,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated welk009 bc I had the wrong GRF files for the natural before.
</commit_message>
<xml_diff>
--- a/RRAMassMods.xlsx
+++ b/RRAMassMods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F568079-8AB1-4823-A7D3-09B7997E1527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F1B6D9-37FB-41A0-871E-E555D189D697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" firstSheet="4" activeTab="7" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="welk001" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10440" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10440" uniqueCount="243">
   <si>
     <t>welk001</t>
   </si>
@@ -625,12 +625,6 @@
     <t>welk009</t>
   </si>
   <si>
-    <t>=0.1,</t>
-  </si>
-  <si>
-    <t>~[-0.133964,0.278266,0.0237279]</t>
-  </si>
-  <si>
     <t>8.43838,</t>
   </si>
   <si>
@@ -653,21 +647,6 @@
   </si>
   <si>
     <t>24.531,</t>
-  </si>
-  <si>
-    <t>~[-0.133964,0.278266,0.0222433]</t>
-  </si>
-  <si>
-    <t>=0.0224708,</t>
-  </si>
-  <si>
-    <t>~[-0.0564351,0.278266,0.00610217]</t>
-  </si>
-  <si>
-    <t>=0.0552515,</t>
-  </si>
-  <si>
-    <t>~[-0.0892159,0.278266,0.0367411]</t>
   </si>
   <si>
     <t>=-0.0429843,</t>
@@ -767,6 +746,30 @@
   </si>
   <si>
     <t>~[-0.032916,0.30212,0.0172133]</t>
+  </si>
+  <si>
+    <t>=-0.01355,</t>
+  </si>
+  <si>
+    <t>~[-0.0204144,0.278266,0.0658313]</t>
+  </si>
+  <si>
+    <t>=-0.00316132,</t>
+  </si>
+  <si>
+    <t>~[-0.0308031,0.278266,0.0546345]</t>
+  </si>
+  <si>
+    <t>=-0.00713543,</t>
+  </si>
+  <si>
+    <t>~[-0.0236676,0.278266,0.062557]</t>
+  </si>
+  <si>
+    <t>=-0.0113703,</t>
+  </si>
+  <si>
+    <t>~[-0.0225941,0.278266,0.0625015]</t>
   </si>
 </sst>
 </file>
@@ -20646,7 +20649,7 @@
         <v>9</v>
       </c>
       <c r="AH11">
-        <f t="shared" ref="AH11:AH26" si="2">AVERAGE(AA11,AA35,AA60,AA85,J86,J61,J36,J11)</f>
+        <f t="shared" ref="AH11:AH25" si="2">AVERAGE(AA11,AA35,AA60,AA85,J86,J61,J36,J11)</f>
         <v>7.3578449999999993</v>
       </c>
     </row>
@@ -29860,7 +29863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53024F3-9755-4748-94E9-291178E5B6E2}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView topLeftCell="W4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
@@ -29933,14 +29936,14 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>194</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5">
-        <f>-0.0222433</f>
-        <v>-2.2243300000000001E-2</v>
+        <f>-0.0658313</f>
+        <v>-6.5831299999999995E-2</v>
       </c>
       <c r="R5" t="s">
         <v>2</v>
@@ -29961,7 +29964,7 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
@@ -29985,7 +29988,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>204</v>
+        <v>236</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -30000,7 +30003,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -30051,7 +30054,7 @@
         <v>48</v>
       </c>
       <c r="E9">
-        <v>7.3939700000000004</v>
+        <v>1.8156600000000001</v>
       </c>
       <c r="L9" t="s">
         <v>105</v>
@@ -30095,7 +30098,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -30107,14 +30110,14 @@
         <v>6</v>
       </c>
       <c r="J10">
-        <v>9.5942399999999992</v>
+        <v>8.7222200000000001</v>
       </c>
       <c r="L10" t="s">
         <v>3</v>
       </c>
       <c r="M10">
         <f>AVERAGE(J10,J35,J60,J85)</f>
-        <v>8.4684925</v>
+        <v>8.7185799999999993</v>
       </c>
       <c r="R10" t="s">
         <v>2</v>
@@ -30132,7 +30135,7 @@
         <v>6</v>
       </c>
       <c r="W10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="X10" t="s">
         <v>8</v>
@@ -30158,7 +30161,7 @@
       </c>
       <c r="AH10">
         <f>AVERAGE(AA10,AA35,AA60,AA85,J85,J60,J35,J10)</f>
-        <v>8.5077737500000001</v>
+        <v>8.6328175000000016</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -30178,7 +30181,7 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -30190,14 +30193,14 @@
         <v>6</v>
       </c>
       <c r="J11">
-        <v>7.5774699999999999</v>
+        <v>6.8887499999999999</v>
       </c>
       <c r="L11" t="s">
         <v>9</v>
       </c>
       <c r="M11">
         <f t="shared" ref="M11:M26" si="0">AVERAGE(J11,J36,J61,J86)</f>
-        <v>6.6883649999999992</v>
+        <v>6.8858800000000002</v>
       </c>
       <c r="R11" t="s">
         <v>2</v>
@@ -30215,7 +30218,7 @@
         <v>6</v>
       </c>
       <c r="W11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X11" t="s">
         <v>8</v>
@@ -30241,7 +30244,7 @@
       </c>
       <c r="AH11">
         <f t="shared" ref="AH11:AH26" si="2">AVERAGE(AA11,AA36,AA61,AA86,J86,J61,J36,J11)</f>
-        <v>6.7193862500000003</v>
+        <v>6.8181437500000008</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -30261,7 +30264,7 @@
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -30273,14 +30276,14 @@
         <v>6</v>
       </c>
       <c r="J12">
-        <v>3.0203500000000001</v>
+        <v>2.7458300000000002</v>
       </c>
       <c r="L12" t="s">
         <v>11</v>
       </c>
       <c r="M12">
         <f t="shared" si="0"/>
-        <v>2.6659550000000003</v>
+        <v>2.744685</v>
       </c>
       <c r="R12" t="s">
         <v>2</v>
@@ -30298,7 +30301,7 @@
         <v>6</v>
       </c>
       <c r="W12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X12" t="s">
         <v>8</v>
@@ -30324,7 +30327,7 @@
       </c>
       <c r="AH12">
         <f t="shared" si="2"/>
-        <v>2.6783199999999998</v>
+        <v>2.7176849999999999</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -30344,7 +30347,7 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -30356,14 +30359,14 @@
         <v>6</v>
       </c>
       <c r="J13">
-        <v>7.0223599999999997E-2</v>
+        <v>6.3840999999999995E-2</v>
       </c>
       <c r="L13" t="s">
         <v>13</v>
       </c>
       <c r="M13">
         <f t="shared" si="0"/>
-        <v>6.1983900000000008E-2</v>
+        <v>6.3814375000000007E-2</v>
       </c>
       <c r="R13" t="s">
         <v>2</v>
@@ -30381,7 +30384,7 @@
         <v>6</v>
       </c>
       <c r="W13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X13" t="s">
         <v>8</v>
@@ -30407,7 +30410,7 @@
       </c>
       <c r="AH13">
         <f t="shared" si="2"/>
-        <v>6.2271400000000005E-2</v>
+        <v>6.3186637500000004E-2</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -30427,7 +30430,7 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -30439,14 +30442,14 @@
         <v>6</v>
       </c>
       <c r="J14">
-        <v>8.1465899999999994E-2</v>
+        <v>7.4061399999999999E-2</v>
       </c>
       <c r="L14" t="s">
         <v>15</v>
       </c>
       <c r="M14">
         <f t="shared" si="0"/>
-        <v>7.190705E-2</v>
+        <v>7.4030550000000001E-2</v>
       </c>
       <c r="R14" t="s">
         <v>2</v>
@@ -30464,7 +30467,7 @@
         <v>6</v>
       </c>
       <c r="W14" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X14" t="s">
         <v>8</v>
@@ -30490,7 +30493,7 @@
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>7.2240575000000001E-2</v>
+        <v>7.3302325000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
@@ -30510,7 +30513,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -30522,14 +30525,14 @@
         <v>6</v>
       </c>
       <c r="J15">
-        <v>1.0183199999999999</v>
+        <v>0.92576800000000004</v>
       </c>
       <c r="L15" t="s">
         <v>17</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>0.898837</v>
+        <v>0.92538200000000004</v>
       </c>
       <c r="R15" t="s">
         <v>2</v>
@@ -30547,7 +30550,7 @@
         <v>6</v>
       </c>
       <c r="W15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X15" t="s">
         <v>8</v>
@@ -30573,7 +30576,7 @@
       </c>
       <c r="AH15">
         <f t="shared" si="2"/>
-        <v>0.90300674999999997</v>
+        <v>0.9162792500000001</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
@@ -30593,7 +30596,7 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -30605,14 +30608,14 @@
         <v>6</v>
       </c>
       <c r="J16">
-        <v>0.176455</v>
+        <v>0.160417</v>
       </c>
       <c r="L16" t="s">
         <v>19</v>
       </c>
       <c r="M16">
         <f t="shared" si="0"/>
-        <v>0.15575050000000001</v>
+        <v>0.16035025</v>
       </c>
       <c r="R16" t="s">
         <v>2</v>
@@ -30630,7 +30633,7 @@
         <v>6</v>
       </c>
       <c r="W16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X16" t="s">
         <v>8</v>
@@ -30656,7 +30659,7 @@
       </c>
       <c r="AH16">
         <f t="shared" si="2"/>
-        <v>0.156473</v>
+        <v>0.15877287500000001</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -30676,7 +30679,7 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -30688,14 +30691,14 @@
         <v>6</v>
       </c>
       <c r="J17">
-        <v>7.5774699999999999</v>
+        <v>6.8887499999999999</v>
       </c>
       <c r="L17" t="s">
         <v>21</v>
       </c>
       <c r="M17">
         <f t="shared" si="0"/>
-        <v>6.6883649999999992</v>
+        <v>6.8858800000000002</v>
       </c>
       <c r="R17" t="s">
         <v>2</v>
@@ -30713,7 +30716,7 @@
         <v>6</v>
       </c>
       <c r="W17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X17" t="s">
         <v>8</v>
@@ -30739,7 +30742,7 @@
       </c>
       <c r="AH17">
         <f t="shared" si="2"/>
-        <v>6.7193862500000003</v>
+        <v>6.8181437500000008</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -30759,7 +30762,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -30771,14 +30774,14 @@
         <v>6</v>
       </c>
       <c r="J18">
-        <v>3.0203500000000001</v>
+        <v>2.7458300000000002</v>
       </c>
       <c r="L18" t="s">
         <v>22</v>
       </c>
       <c r="M18">
         <f t="shared" si="0"/>
-        <v>2.6659550000000003</v>
+        <v>2.744685</v>
       </c>
       <c r="R18" t="s">
         <v>2</v>
@@ -30796,7 +30799,7 @@
         <v>6</v>
       </c>
       <c r="W18" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X18" t="s">
         <v>8</v>
@@ -30822,7 +30825,7 @@
       </c>
       <c r="AH18">
         <f t="shared" si="2"/>
-        <v>2.6783199999999998</v>
+        <v>2.7176849999999999</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
@@ -30842,7 +30845,7 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -30854,14 +30857,14 @@
         <v>6</v>
       </c>
       <c r="J19">
-        <v>7.0223599999999997E-2</v>
+        <v>6.3840999999999995E-2</v>
       </c>
       <c r="L19" t="s">
         <v>23</v>
       </c>
       <c r="M19">
         <f t="shared" si="0"/>
-        <v>6.1983900000000008E-2</v>
+        <v>6.3814375000000007E-2</v>
       </c>
       <c r="R19" t="s">
         <v>2</v>
@@ -30879,7 +30882,7 @@
         <v>6</v>
       </c>
       <c r="W19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X19" t="s">
         <v>8</v>
@@ -30905,7 +30908,7 @@
       </c>
       <c r="AH19">
         <f t="shared" si="2"/>
-        <v>6.2271400000000005E-2</v>
+        <v>6.3186637500000004E-2</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -30925,7 +30928,7 @@
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -30937,14 +30940,14 @@
         <v>6</v>
       </c>
       <c r="J20">
-        <v>8.1465899999999994E-2</v>
+        <v>7.4061399999999999E-2</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
       </c>
       <c r="M20">
         <f t="shared" si="0"/>
-        <v>7.190705E-2</v>
+        <v>7.4030550000000001E-2</v>
       </c>
       <c r="R20" t="s">
         <v>2</v>
@@ -30962,7 +30965,7 @@
         <v>6</v>
       </c>
       <c r="W20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X20" t="s">
         <v>8</v>
@@ -30988,7 +30991,7 @@
       </c>
       <c r="AH20">
         <f t="shared" si="2"/>
-        <v>7.2240575000000001E-2</v>
+        <v>7.3302325000000002E-2</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
@@ -31008,7 +31011,7 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
@@ -31020,14 +31023,14 @@
         <v>6</v>
       </c>
       <c r="J21">
-        <v>1.0183199999999999</v>
+        <v>0.92576800000000004</v>
       </c>
       <c r="L21" t="s">
         <v>25</v>
       </c>
       <c r="M21">
         <f t="shared" si="0"/>
-        <v>0.898837</v>
+        <v>0.92538200000000004</v>
       </c>
       <c r="R21" t="s">
         <v>2</v>
@@ -31045,7 +31048,7 @@
         <v>6</v>
       </c>
       <c r="W21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X21" t="s">
         <v>8</v>
@@ -31071,7 +31074,7 @@
       </c>
       <c r="AH21">
         <f t="shared" si="2"/>
-        <v>0.90300674999999997</v>
+        <v>0.9162792500000001</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -31091,7 +31094,7 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -31103,14 +31106,14 @@
         <v>6</v>
       </c>
       <c r="J22">
-        <v>0.176455</v>
+        <v>0.160417</v>
       </c>
       <c r="L22" t="s">
         <v>26</v>
       </c>
       <c r="M22">
         <f t="shared" si="0"/>
-        <v>0.15575050000000001</v>
+        <v>0.16035025</v>
       </c>
       <c r="R22" t="s">
         <v>2</v>
@@ -31128,7 +31131,7 @@
         <v>6</v>
       </c>
       <c r="W22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X22" t="s">
         <v>8</v>
@@ -31154,7 +31157,7 @@
       </c>
       <c r="AH22">
         <f t="shared" si="2"/>
-        <v>0.156473</v>
+        <v>0.15877287500000001</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -31174,7 +31177,7 @@
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -31186,14 +31189,14 @@
         <v>6</v>
       </c>
       <c r="J23">
-        <v>27.891200000000001</v>
+        <v>25.356100000000001</v>
       </c>
       <c r="L23" t="s">
         <v>27</v>
       </c>
       <c r="M23">
         <f t="shared" si="0"/>
-        <v>24.618550000000003</v>
+        <v>25.345550000000003</v>
       </c>
       <c r="R23" t="s">
         <v>2</v>
@@ -31211,7 +31214,7 @@
         <v>6</v>
       </c>
       <c r="W23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="X23" t="s">
         <v>8</v>
@@ -31237,7 +31240,7 @@
       </c>
       <c r="AH23">
         <f t="shared" si="2"/>
-        <v>24.732724999999999</v>
+        <v>25.096225</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -31245,14 +31248,14 @@
         <v>38</v>
       </c>
       <c r="J24" s="2">
-        <v>-0.133964</v>
+        <v>-2.0414399999999999E-2</v>
       </c>
       <c r="L24" t="s">
         <v>38</v>
       </c>
       <c r="M24">
         <f t="shared" si="0"/>
-        <v>-0.10339475000000001</v>
+        <v>-2.4369799999999997E-2</v>
       </c>
       <c r="Z24" t="s">
         <v>38</v>
@@ -31272,7 +31275,7 @@
       </c>
       <c r="AH24">
         <f t="shared" si="2"/>
-        <v>-4.7856823749999999E-2</v>
+        <v>-8.3443487499999993E-3</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -31315,14 +31318,14 @@
         <v>39</v>
       </c>
       <c r="J26">
-        <v>2.2243300000000001E-2</v>
+        <v>6.5831299999999995E-2</v>
       </c>
       <c r="L26" t="s">
         <v>39</v>
       </c>
       <c r="M26">
         <f t="shared" si="0"/>
-        <v>2.2203617500000002E-2</v>
+        <v>6.1381074999999993E-2</v>
       </c>
       <c r="Z26" t="s">
         <v>39</v>
@@ -31342,7 +31345,7 @@
       </c>
       <c r="AH26">
         <f t="shared" si="2"/>
-        <v>3.408357125E-2</v>
+        <v>5.3672299999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -31399,14 +31402,14 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>194</v>
+        <v>237</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
       </c>
       <c r="I30">
-        <f>-0.0237279</f>
-        <v>-2.37279E-2</v>
+        <f>-0.0546345</f>
+        <v>-5.4634500000000003E-2</v>
       </c>
       <c r="R30" t="s">
         <v>2</v>
@@ -31427,7 +31430,7 @@
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="Y30" t="s">
         <v>39</v>
@@ -31451,7 +31454,7 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -31466,7 +31469,7 @@
         <v>42</v>
       </c>
       <c r="V31" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -31517,7 +31520,7 @@
         <v>48</v>
       </c>
       <c r="E34">
-        <v>-3.4220100000000002</v>
+        <v>1.79531</v>
       </c>
       <c r="R34" t="s">
         <v>2</v>
@@ -31552,7 +31555,7 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G35" t="s">
         <v>8</v>
@@ -31564,7 +31567,7 @@
         <v>6</v>
       </c>
       <c r="J35">
-        <v>7.9034399999999998</v>
+        <v>8.7190300000000001</v>
       </c>
       <c r="R35" t="s">
         <v>2</v>
@@ -31582,7 +31585,7 @@
         <v>6</v>
       </c>
       <c r="W35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="X35" t="s">
         <v>8</v>
@@ -31614,7 +31617,7 @@
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G36" t="s">
         <v>8</v>
@@ -31626,7 +31629,7 @@
         <v>6</v>
       </c>
       <c r="J36">
-        <v>6.2420900000000001</v>
+        <v>6.8862399999999999</v>
       </c>
       <c r="R36" t="s">
         <v>2</v>
@@ -31644,7 +31647,7 @@
         <v>6</v>
       </c>
       <c r="W36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X36" t="s">
         <v>8</v>
@@ -31676,7 +31679,7 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -31688,7 +31691,7 @@
         <v>6</v>
       </c>
       <c r="J37">
-        <v>2.48807</v>
+        <v>2.7448299999999999</v>
       </c>
       <c r="R37" t="s">
         <v>2</v>
@@ -31706,7 +31709,7 @@
         <v>6</v>
       </c>
       <c r="W37" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X37" t="s">
         <v>8</v>
@@ -31738,7 +31741,7 @@
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G38" t="s">
         <v>8</v>
@@ -31750,7 +31753,7 @@
         <v>6</v>
       </c>
       <c r="J38">
-        <v>5.78481E-2</v>
+        <v>6.3817700000000005E-2</v>
       </c>
       <c r="R38" t="s">
         <v>2</v>
@@ -31768,7 +31771,7 @@
         <v>6</v>
       </c>
       <c r="W38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X38" t="s">
         <v>8</v>
@@ -31800,7 +31803,7 @@
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G39" t="s">
         <v>8</v>
@@ -31812,7 +31815,7 @@
         <v>6</v>
       </c>
       <c r="J39">
-        <v>6.7109100000000005E-2</v>
+        <v>7.40344E-2</v>
       </c>
       <c r="R39" t="s">
         <v>2</v>
@@ -31830,7 +31833,7 @@
         <v>6</v>
       </c>
       <c r="W39" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X39" t="s">
         <v>8</v>
@@ -31862,7 +31865,7 @@
         <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G40" t="s">
         <v>8</v>
@@ -31874,7 +31877,7 @@
         <v>6</v>
       </c>
       <c r="J40">
-        <v>0.83886400000000005</v>
+        <v>0.92542999999999997</v>
       </c>
       <c r="R40" t="s">
         <v>2</v>
@@ -31892,7 +31895,7 @@
         <v>6</v>
       </c>
       <c r="W40" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X40" t="s">
         <v>8</v>
@@ -31924,7 +31927,7 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G41" t="s">
         <v>8</v>
@@ -31936,7 +31939,7 @@
         <v>6</v>
       </c>
       <c r="J41">
-        <v>0.14535799999999999</v>
+        <v>0.160359</v>
       </c>
       <c r="R41" t="s">
         <v>2</v>
@@ -31954,7 +31957,7 @@
         <v>6</v>
       </c>
       <c r="W41" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X41" t="s">
         <v>8</v>
@@ -31986,7 +31989,7 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G42" t="s">
         <v>8</v>
@@ -31998,7 +32001,7 @@
         <v>6</v>
       </c>
       <c r="J42">
-        <v>6.2420900000000001</v>
+        <v>6.8862399999999999</v>
       </c>
       <c r="R42" t="s">
         <v>2</v>
@@ -32016,7 +32019,7 @@
         <v>6</v>
       </c>
       <c r="W42" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X42" t="s">
         <v>8</v>
@@ -32048,7 +32051,7 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
@@ -32060,7 +32063,7 @@
         <v>6</v>
       </c>
       <c r="J43">
-        <v>2.48807</v>
+        <v>2.7448299999999999</v>
       </c>
       <c r="R43" t="s">
         <v>2</v>
@@ -32078,7 +32081,7 @@
         <v>6</v>
       </c>
       <c r="W43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X43" t="s">
         <v>8</v>
@@ -32110,7 +32113,7 @@
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G44" t="s">
         <v>8</v>
@@ -32122,7 +32125,7 @@
         <v>6</v>
       </c>
       <c r="J44">
-        <v>5.78481E-2</v>
+        <v>6.3817700000000005E-2</v>
       </c>
       <c r="R44" t="s">
         <v>2</v>
@@ -32140,7 +32143,7 @@
         <v>6</v>
       </c>
       <c r="W44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X44" t="s">
         <v>8</v>
@@ -32172,7 +32175,7 @@
         <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G45" t="s">
         <v>8</v>
@@ -32184,7 +32187,7 @@
         <v>6</v>
       </c>
       <c r="J45">
-        <v>6.7109100000000005E-2</v>
+        <v>7.40344E-2</v>
       </c>
       <c r="R45" t="s">
         <v>2</v>
@@ -32202,7 +32205,7 @@
         <v>6</v>
       </c>
       <c r="W45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X45" t="s">
         <v>8</v>
@@ -32234,7 +32237,7 @@
         <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G46" t="s">
         <v>8</v>
@@ -32246,7 +32249,7 @@
         <v>6</v>
       </c>
       <c r="J46">
-        <v>0.83886400000000005</v>
+        <v>0.92542999999999997</v>
       </c>
       <c r="R46" t="s">
         <v>2</v>
@@ -32264,7 +32267,7 @@
         <v>6</v>
       </c>
       <c r="W46" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X46" t="s">
         <v>8</v>
@@ -32296,7 +32299,7 @@
         <v>6</v>
       </c>
       <c r="F47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G47" t="s">
         <v>8</v>
@@ -32308,7 +32311,7 @@
         <v>6</v>
       </c>
       <c r="J47">
-        <v>0.14535799999999999</v>
+        <v>0.160359</v>
       </c>
       <c r="R47" t="s">
         <v>2</v>
@@ -32326,7 +32329,7 @@
         <v>6</v>
       </c>
       <c r="W47" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X47" t="s">
         <v>8</v>
@@ -32358,7 +32361,7 @@
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G48" t="s">
         <v>8</v>
@@ -32370,7 +32373,7 @@
         <v>6</v>
       </c>
       <c r="J48">
-        <v>22.975899999999999</v>
+        <v>25.346900000000002</v>
       </c>
       <c r="R48" t="s">
         <v>2</v>
@@ -32388,7 +32391,7 @@
         <v>6</v>
       </c>
       <c r="W48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="X48" t="s">
         <v>8</v>
@@ -32408,7 +32411,7 @@
         <v>38</v>
       </c>
       <c r="J49">
-        <v>-0.133964</v>
+        <v>-3.08031E-2</v>
       </c>
       <c r="Z49" t="s">
         <v>38</v>
@@ -32436,7 +32439,7 @@
         <v>39</v>
       </c>
       <c r="J51">
-        <v>2.37279E-2</v>
+        <v>5.4634500000000003E-2</v>
       </c>
       <c r="Z51" t="s">
         <v>39</v>
@@ -32499,14 +32502,14 @@
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="H55" t="s">
         <v>39</v>
       </c>
       <c r="I55">
-        <f>-0.00610217</f>
-        <v>-6.1021699999999996E-3</v>
+        <f>-0.00792246</f>
+        <v>-7.9224599999999992E-3</v>
       </c>
       <c r="R55" t="s">
         <v>2</v>
@@ -32527,7 +32530,7 @@
         <v>38</v>
       </c>
       <c r="X55" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="Y55" t="s">
         <v>39</v>
@@ -32551,7 +32554,7 @@
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -32566,7 +32569,7 @@
         <v>42</v>
       </c>
       <c r="V56" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -32617,7 +32620,7 @@
         <v>48</v>
       </c>
       <c r="E59">
-        <v>-5.5506500000000001</v>
+        <v>1.9633700000000001</v>
       </c>
       <c r="R59" t="s">
         <v>2</v>
@@ -32652,7 +32655,7 @@
         <v>6</v>
       </c>
       <c r="F60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G60" t="s">
         <v>8</v>
@@ -32664,7 +32667,7 @@
         <v>6</v>
       </c>
       <c r="J60">
-        <v>7.5706800000000003</v>
+        <v>8.7453099999999999</v>
       </c>
       <c r="R60" t="s">
         <v>2</v>
@@ -32682,7 +32685,7 @@
         <v>6</v>
       </c>
       <c r="W60" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="X60" t="s">
         <v>8</v>
@@ -32714,7 +32717,7 @@
         <v>6</v>
       </c>
       <c r="F61" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G61" t="s">
         <v>8</v>
@@ -32726,7 +32729,7 @@
         <v>6</v>
       </c>
       <c r="J61">
-        <v>5.9792800000000002</v>
+        <v>6.9069900000000004</v>
       </c>
       <c r="R61" t="s">
         <v>2</v>
@@ -32744,7 +32747,7 @@
         <v>6</v>
       </c>
       <c r="W61" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X61" t="s">
         <v>8</v>
@@ -32776,7 +32779,7 @@
         <v>6</v>
       </c>
       <c r="F62" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G62" t="s">
         <v>8</v>
@@ -32788,7 +32791,7 @@
         <v>6</v>
       </c>
       <c r="J62">
-        <v>2.3833199999999999</v>
+        <v>2.7530999999999999</v>
       </c>
       <c r="R62" t="s">
         <v>2</v>
@@ -32806,7 +32809,7 @@
         <v>6</v>
       </c>
       <c r="W62" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X62" t="s">
         <v>8</v>
@@ -32838,7 +32841,7 @@
         <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G63" t="s">
         <v>8</v>
@@ -32850,7 +32853,7 @@
         <v>6</v>
       </c>
       <c r="J63">
-        <v>5.5412500000000003E-2</v>
+        <v>6.4009999999999997E-2</v>
       </c>
       <c r="R63" t="s">
         <v>2</v>
@@ -32868,7 +32871,7 @@
         <v>6</v>
       </c>
       <c r="W63" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X63" t="s">
         <v>8</v>
@@ -32900,7 +32903,7 @@
         <v>6</v>
       </c>
       <c r="F64" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G64" t="s">
         <v>8</v>
@@ -32912,7 +32915,7 @@
         <v>6</v>
       </c>
       <c r="J64">
-        <v>6.4283599999999996E-2</v>
+        <v>7.4257500000000004E-2</v>
       </c>
       <c r="R64" t="s">
         <v>2</v>
@@ -32930,7 +32933,7 @@
         <v>6</v>
       </c>
       <c r="W64" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X64" t="s">
         <v>8</v>
@@ -32962,7 +32965,7 @@
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G65" t="s">
         <v>8</v>
@@ -32974,7 +32977,7 @@
         <v>6</v>
       </c>
       <c r="J65">
-        <v>0.80354499999999995</v>
+        <v>0.92821900000000002</v>
       </c>
       <c r="R65" t="s">
         <v>2</v>
@@ -32992,7 +32995,7 @@
         <v>6</v>
       </c>
       <c r="W65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X65" t="s">
         <v>8</v>
@@ -33024,7 +33027,7 @@
         <v>6</v>
       </c>
       <c r="F66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G66" t="s">
         <v>8</v>
@@ -33036,7 +33039,7 @@
         <v>6</v>
       </c>
       <c r="J66">
-        <v>0.139238</v>
+        <v>0.16084200000000001</v>
       </c>
       <c r="R66" t="s">
         <v>2</v>
@@ -33054,7 +33057,7 @@
         <v>6</v>
       </c>
       <c r="W66" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X66" t="s">
         <v>8</v>
@@ -33086,7 +33089,7 @@
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G67" t="s">
         <v>8</v>
@@ -33098,7 +33101,7 @@
         <v>6</v>
       </c>
       <c r="J67">
-        <v>5.9792800000000002</v>
+        <v>6.9069900000000004</v>
       </c>
       <c r="R67" t="s">
         <v>2</v>
@@ -33116,7 +33119,7 @@
         <v>6</v>
       </c>
       <c r="W67" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X67" t="s">
         <v>8</v>
@@ -33148,7 +33151,7 @@
         <v>6</v>
       </c>
       <c r="F68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G68" t="s">
         <v>8</v>
@@ -33160,7 +33163,7 @@
         <v>6</v>
       </c>
       <c r="J68">
-        <v>2.3833199999999999</v>
+        <v>2.7530999999999999</v>
       </c>
       <c r="R68" t="s">
         <v>2</v>
@@ -33178,7 +33181,7 @@
         <v>6</v>
       </c>
       <c r="W68" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X68" t="s">
         <v>8</v>
@@ -33210,7 +33213,7 @@
         <v>6</v>
       </c>
       <c r="F69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G69" t="s">
         <v>8</v>
@@ -33222,7 +33225,7 @@
         <v>6</v>
       </c>
       <c r="J69">
-        <v>5.5412500000000003E-2</v>
+        <v>6.4009999999999997E-2</v>
       </c>
       <c r="R69" t="s">
         <v>2</v>
@@ -33240,7 +33243,7 @@
         <v>6</v>
       </c>
       <c r="W69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X69" t="s">
         <v>8</v>
@@ -33272,7 +33275,7 @@
         <v>6</v>
       </c>
       <c r="F70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G70" t="s">
         <v>8</v>
@@ -33284,7 +33287,7 @@
         <v>6</v>
       </c>
       <c r="J70">
-        <v>6.4283599999999996E-2</v>
+        <v>7.4257500000000004E-2</v>
       </c>
       <c r="R70" t="s">
         <v>2</v>
@@ -33302,7 +33305,7 @@
         <v>6</v>
       </c>
       <c r="W70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X70" t="s">
         <v>8</v>
@@ -33334,7 +33337,7 @@
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G71" t="s">
         <v>8</v>
@@ -33346,7 +33349,7 @@
         <v>6</v>
       </c>
       <c r="J71">
-        <v>0.80354499999999995</v>
+        <v>0.92821900000000002</v>
       </c>
       <c r="R71" t="s">
         <v>2</v>
@@ -33364,7 +33367,7 @@
         <v>6</v>
       </c>
       <c r="W71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X71" t="s">
         <v>8</v>
@@ -33396,7 +33399,7 @@
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G72" t="s">
         <v>8</v>
@@ -33408,7 +33411,7 @@
         <v>6</v>
       </c>
       <c r="J72">
-        <v>0.139238</v>
+        <v>0.16084200000000001</v>
       </c>
       <c r="R72" t="s">
         <v>2</v>
@@ -33426,7 +33429,7 @@
         <v>6</v>
       </c>
       <c r="W72" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X72" t="s">
         <v>8</v>
@@ -33458,7 +33461,7 @@
         <v>6</v>
       </c>
       <c r="F73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G73" t="s">
         <v>8</v>
@@ -33470,7 +33473,7 @@
         <v>6</v>
       </c>
       <c r="J73">
-        <v>22.008500000000002</v>
+        <v>25.423200000000001</v>
       </c>
       <c r="R73" t="s">
         <v>2</v>
@@ -33488,7 +33491,7 @@
         <v>6</v>
       </c>
       <c r="W73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="X73" t="s">
         <v>8</v>
@@ -33508,7 +33511,7 @@
         <v>38</v>
       </c>
       <c r="J74">
-        <v>-5.6435100000000002E-2</v>
+        <v>-2.36676E-2</v>
       </c>
       <c r="Z74" t="s">
         <v>38</v>
@@ -33536,7 +33539,7 @@
         <v>39</v>
       </c>
       <c r="J76">
-        <v>6.1021699999999996E-3</v>
+        <v>6.2557000000000001E-2</v>
       </c>
       <c r="Z76" t="s">
         <v>39</v>
@@ -33599,14 +33602,14 @@
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="H80" t="s">
         <v>39</v>
       </c>
       <c r="I80">
-        <f>-0.0367411</f>
-        <v>-3.6741099999999999E-2</v>
+        <f>-0.0625015</f>
+        <v>-6.2501500000000002E-2</v>
       </c>
       <c r="R80" t="s">
         <v>2</v>
@@ -33627,7 +33630,7 @@
         <v>38</v>
       </c>
       <c r="X80" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="Y80" t="s">
         <v>39</v>
@@ -33651,7 +33654,7 @@
         <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -33666,7 +33669,7 @@
         <v>42</v>
       </c>
       <c r="V81" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -33717,7 +33720,7 @@
         <v>48</v>
       </c>
       <c r="E84">
-        <v>2.3491399999999998</v>
+        <v>1.5952599999999999</v>
       </c>
       <c r="R84" t="s">
         <v>2</v>
@@ -33752,7 +33755,7 @@
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G85" t="s">
         <v>8</v>
@@ -33764,7 +33767,7 @@
         <v>6</v>
       </c>
       <c r="J85">
-        <v>8.8056099999999997</v>
+        <v>8.6877600000000008</v>
       </c>
       <c r="R85" t="s">
         <v>2</v>
@@ -33782,7 +33785,7 @@
         <v>6</v>
       </c>
       <c r="W85" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="X85" t="s">
         <v>8</v>
@@ -33814,7 +33817,7 @@
         <v>6</v>
       </c>
       <c r="F86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G86" t="s">
         <v>8</v>
@@ -33826,7 +33829,7 @@
         <v>6</v>
       </c>
       <c r="J86">
-        <v>6.9546200000000002</v>
+        <v>6.8615399999999998</v>
       </c>
       <c r="R86" t="s">
         <v>2</v>
@@ -33844,7 +33847,7 @@
         <v>6</v>
       </c>
       <c r="W86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X86" t="s">
         <v>8</v>
@@ -33876,7 +33879,7 @@
         <v>6</v>
       </c>
       <c r="F87" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G87" t="s">
         <v>8</v>
@@ -33888,7 +33891,7 @@
         <v>6</v>
       </c>
       <c r="J87">
-        <v>2.7720799999999999</v>
+        <v>2.7349800000000002</v>
       </c>
       <c r="R87" t="s">
         <v>2</v>
@@ -33906,7 +33909,7 @@
         <v>6</v>
       </c>
       <c r="W87" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X87" t="s">
         <v>8</v>
@@ -33938,7 +33941,7 @@
         <v>6</v>
       </c>
       <c r="F88" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G88" t="s">
         <v>8</v>
@@ -33950,7 +33953,7 @@
         <v>6</v>
       </c>
       <c r="J88">
-        <v>6.4451400000000006E-2</v>
+        <v>6.3588800000000001E-2</v>
       </c>
       <c r="R88" t="s">
         <v>2</v>
@@ -33968,7 +33971,7 @@
         <v>6</v>
       </c>
       <c r="W88" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X88" t="s">
         <v>8</v>
@@ -34000,7 +34003,7 @@
         <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G89" t="s">
         <v>8</v>
@@ -34012,7 +34015,7 @@
         <v>6</v>
       </c>
       <c r="J89">
-        <v>7.4769600000000006E-2</v>
+        <v>7.3768899999999998E-2</v>
       </c>
       <c r="R89" t="s">
         <v>2</v>
@@ -34030,7 +34033,7 @@
         <v>6</v>
       </c>
       <c r="W89" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X89" t="s">
         <v>8</v>
@@ -34062,7 +34065,7 @@
         <v>6</v>
       </c>
       <c r="F90" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G90" t="s">
         <v>8</v>
@@ -34074,7 +34077,7 @@
         <v>6</v>
       </c>
       <c r="J90">
-        <v>0.93461899999999998</v>
+        <v>0.92211100000000001</v>
       </c>
       <c r="R90" t="s">
         <v>2</v>
@@ -34092,7 +34095,7 @@
         <v>6</v>
       </c>
       <c r="W90" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X90" t="s">
         <v>8</v>
@@ -34124,7 +34127,7 @@
         <v>6</v>
       </c>
       <c r="F91" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G91" t="s">
         <v>8</v>
@@ -34136,7 +34139,7 @@
         <v>6</v>
       </c>
       <c r="J91">
-        <v>0.16195100000000001</v>
+        <v>0.15978300000000001</v>
       </c>
       <c r="R91" t="s">
         <v>2</v>
@@ -34154,7 +34157,7 @@
         <v>6</v>
       </c>
       <c r="W91" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X91" t="s">
         <v>8</v>
@@ -34186,7 +34189,7 @@
         <v>6</v>
       </c>
       <c r="F92" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G92" t="s">
         <v>8</v>
@@ -34198,7 +34201,7 @@
         <v>6</v>
       </c>
       <c r="J92">
-        <v>6.9546200000000002</v>
+        <v>6.8615399999999998</v>
       </c>
       <c r="R92" t="s">
         <v>2</v>
@@ -34216,7 +34219,7 @@
         <v>6</v>
       </c>
       <c r="W92" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="X92" t="s">
         <v>8</v>
@@ -34248,7 +34251,7 @@
         <v>6</v>
       </c>
       <c r="F93" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G93" t="s">
         <v>8</v>
@@ -34260,7 +34263,7 @@
         <v>6</v>
       </c>
       <c r="J93">
-        <v>2.7720799999999999</v>
+        <v>2.7349800000000002</v>
       </c>
       <c r="R93" t="s">
         <v>2</v>
@@ -34278,7 +34281,7 @@
         <v>6</v>
       </c>
       <c r="W93" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X93" t="s">
         <v>8</v>
@@ -34310,7 +34313,7 @@
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G94" t="s">
         <v>8</v>
@@ -34322,7 +34325,7 @@
         <v>6</v>
       </c>
       <c r="J94">
-        <v>6.4451400000000006E-2</v>
+        <v>6.3588800000000001E-2</v>
       </c>
       <c r="R94" t="s">
         <v>2</v>
@@ -34340,7 +34343,7 @@
         <v>6</v>
       </c>
       <c r="W94" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="X94" t="s">
         <v>8</v>
@@ -34372,7 +34375,7 @@
         <v>6</v>
       </c>
       <c r="F95" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G95" t="s">
         <v>8</v>
@@ -34384,7 +34387,7 @@
         <v>6</v>
       </c>
       <c r="J95">
-        <v>7.4769600000000006E-2</v>
+        <v>7.3768899999999998E-2</v>
       </c>
       <c r="R95" t="s">
         <v>2</v>
@@ -34402,7 +34405,7 @@
         <v>6</v>
       </c>
       <c r="W95" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="X95" t="s">
         <v>8</v>
@@ -34434,7 +34437,7 @@
         <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G96" t="s">
         <v>8</v>
@@ -34446,7 +34449,7 @@
         <v>6</v>
       </c>
       <c r="J96">
-        <v>0.93461899999999998</v>
+        <v>0.92211100000000001</v>
       </c>
       <c r="R96" t="s">
         <v>2</v>
@@ -34464,7 +34467,7 @@
         <v>6</v>
       </c>
       <c r="W96" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="X96" t="s">
         <v>8</v>
@@ -34496,7 +34499,7 @@
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G97" t="s">
         <v>8</v>
@@ -34508,7 +34511,7 @@
         <v>6</v>
       </c>
       <c r="J97">
-        <v>0.16195100000000001</v>
+        <v>0.15978300000000001</v>
       </c>
       <c r="R97" t="s">
         <v>2</v>
@@ -34526,7 +34529,7 @@
         <v>6</v>
       </c>
       <c r="W97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X97" t="s">
         <v>8</v>
@@ -34558,7 +34561,7 @@
         <v>6</v>
       </c>
       <c r="F98" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G98" t="s">
         <v>8</v>
@@ -34570,7 +34573,7 @@
         <v>6</v>
       </c>
       <c r="J98">
-        <v>25.598600000000001</v>
+        <v>25.256</v>
       </c>
       <c r="R98" t="s">
         <v>2</v>
@@ -34588,7 +34591,7 @@
         <v>6</v>
       </c>
       <c r="W98" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="X98" t="s">
         <v>8</v>
@@ -34608,7 +34611,7 @@
         <v>38</v>
       </c>
       <c r="J99">
-        <v>-8.9215900000000001E-2</v>
+        <v>-2.2594099999999999E-2</v>
       </c>
       <c r="Z99" t="s">
         <v>38</v>
@@ -34636,7 +34639,7 @@
         <v>39</v>
       </c>
       <c r="J101">
-        <v>3.6741099999999999E-2</v>
+        <v>6.2501500000000002E-2</v>
       </c>
       <c r="Z101" t="s">
         <v>39</v>
@@ -34654,7 +34657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7434A9A0-AC1F-42B5-B8C4-F9AFA5AAB5A4}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="W1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
@@ -34662,7 +34665,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
@@ -34727,7 +34730,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
@@ -34755,7 +34758,7 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
@@ -34779,7 +34782,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -34794,7 +34797,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -34889,7 +34892,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -34926,7 +34929,7 @@
         <v>6</v>
       </c>
       <c r="W10" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="X10" t="s">
         <v>8</v>
@@ -34972,7 +34975,7 @@
         <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -35009,7 +35012,7 @@
         <v>6</v>
       </c>
       <c r="W11" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X11" t="s">
         <v>8</v>
@@ -35055,7 +35058,7 @@
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
@@ -35092,7 +35095,7 @@
         <v>6</v>
       </c>
       <c r="W12" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X12" t="s">
         <v>8</v>
@@ -35138,7 +35141,7 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -35175,7 +35178,7 @@
         <v>6</v>
       </c>
       <c r="W13" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X13" t="s">
         <v>8</v>
@@ -35221,7 +35224,7 @@
         <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -35258,7 +35261,7 @@
         <v>6</v>
       </c>
       <c r="W14" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X14" t="s">
         <v>8</v>
@@ -35304,7 +35307,7 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -35341,7 +35344,7 @@
         <v>6</v>
       </c>
       <c r="W15" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X15" t="s">
         <v>8</v>
@@ -35387,7 +35390,7 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -35424,7 +35427,7 @@
         <v>6</v>
       </c>
       <c r="W16" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X16" t="s">
         <v>8</v>
@@ -35470,7 +35473,7 @@
         <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -35507,7 +35510,7 @@
         <v>6</v>
       </c>
       <c r="W17" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X17" t="s">
         <v>8</v>
@@ -35553,7 +35556,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -35590,7 +35593,7 @@
         <v>6</v>
       </c>
       <c r="W18" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X18" t="s">
         <v>8</v>
@@ -35636,7 +35639,7 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -35673,7 +35676,7 @@
         <v>6</v>
       </c>
       <c r="W19" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X19" t="s">
         <v>8</v>
@@ -35719,7 +35722,7 @@
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -35756,7 +35759,7 @@
         <v>6</v>
       </c>
       <c r="W20" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X20" t="s">
         <v>8</v>
@@ -35802,7 +35805,7 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
@@ -35839,7 +35842,7 @@
         <v>6</v>
       </c>
       <c r="W21" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X21" t="s">
         <v>8</v>
@@ -35885,7 +35888,7 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G22" t="s">
         <v>8</v>
@@ -35922,7 +35925,7 @@
         <v>6</v>
       </c>
       <c r="W22" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X22" t="s">
         <v>8</v>
@@ -35968,7 +35971,7 @@
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -36005,7 +36008,7 @@
         <v>6</v>
       </c>
       <c r="W23" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="X23" t="s">
         <v>8</v>
@@ -36193,7 +36196,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
@@ -36221,7 +36224,7 @@
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="Y30" t="s">
         <v>39</v>
@@ -36245,7 +36248,7 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -36260,7 +36263,7 @@
         <v>42</v>
       </c>
       <c r="V31" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -36346,7 +36349,7 @@
         <v>6</v>
       </c>
       <c r="F35" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G35" t="s">
         <v>8</v>
@@ -36376,7 +36379,7 @@
         <v>6</v>
       </c>
       <c r="W35" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="X35" t="s">
         <v>8</v>
@@ -36408,7 +36411,7 @@
         <v>6</v>
       </c>
       <c r="F36" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G36" t="s">
         <v>8</v>
@@ -36438,7 +36441,7 @@
         <v>6</v>
       </c>
       <c r="W36" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X36" t="s">
         <v>8</v>
@@ -36470,7 +36473,7 @@
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -36500,7 +36503,7 @@
         <v>6</v>
       </c>
       <c r="W37" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X37" t="s">
         <v>8</v>
@@ -36532,7 +36535,7 @@
         <v>6</v>
       </c>
       <c r="F38" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G38" t="s">
         <v>8</v>
@@ -36562,7 +36565,7 @@
         <v>6</v>
       </c>
       <c r="W38" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X38" t="s">
         <v>8</v>
@@ -36594,7 +36597,7 @@
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G39" t="s">
         <v>8</v>
@@ -36624,7 +36627,7 @@
         <v>6</v>
       </c>
       <c r="W39" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X39" t="s">
         <v>8</v>
@@ -36656,7 +36659,7 @@
         <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G40" t="s">
         <v>8</v>
@@ -36686,7 +36689,7 @@
         <v>6</v>
       </c>
       <c r="W40" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X40" t="s">
         <v>8</v>
@@ -36718,7 +36721,7 @@
         <v>6</v>
       </c>
       <c r="F41" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G41" t="s">
         <v>8</v>
@@ -36748,7 +36751,7 @@
         <v>6</v>
       </c>
       <c r="W41" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X41" t="s">
         <v>8</v>
@@ -36780,7 +36783,7 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G42" t="s">
         <v>8</v>
@@ -36810,7 +36813,7 @@
         <v>6</v>
       </c>
       <c r="W42" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X42" t="s">
         <v>8</v>
@@ -36842,7 +36845,7 @@
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G43" t="s">
         <v>8</v>
@@ -36872,7 +36875,7 @@
         <v>6</v>
       </c>
       <c r="W43" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X43" t="s">
         <v>8</v>
@@ -36904,7 +36907,7 @@
         <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G44" t="s">
         <v>8</v>
@@ -36934,7 +36937,7 @@
         <v>6</v>
       </c>
       <c r="W44" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X44" t="s">
         <v>8</v>
@@ -36966,7 +36969,7 @@
         <v>6</v>
       </c>
       <c r="F45" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G45" t="s">
         <v>8</v>
@@ -36996,7 +36999,7 @@
         <v>6</v>
       </c>
       <c r="W45" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X45" t="s">
         <v>8</v>
@@ -37028,7 +37031,7 @@
         <v>6</v>
       </c>
       <c r="F46" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G46" t="s">
         <v>8</v>
@@ -37058,7 +37061,7 @@
         <v>6</v>
       </c>
       <c r="W46" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X46" t="s">
         <v>8</v>
@@ -37090,7 +37093,7 @@
         <v>6</v>
       </c>
       <c r="F47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G47" t="s">
         <v>8</v>
@@ -37120,7 +37123,7 @@
         <v>6</v>
       </c>
       <c r="W47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X47" t="s">
         <v>8</v>
@@ -37152,7 +37155,7 @@
         <v>6</v>
       </c>
       <c r="F48" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G48" t="s">
         <v>8</v>
@@ -37182,7 +37185,7 @@
         <v>6</v>
       </c>
       <c r="W48" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="X48" t="s">
         <v>8</v>
@@ -37293,7 +37296,7 @@
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="H55" t="s">
         <v>39</v>
@@ -37321,7 +37324,7 @@
         <v>38</v>
       </c>
       <c r="X55" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="Y55" t="s">
         <v>39</v>
@@ -37345,7 +37348,7 @@
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -37360,7 +37363,7 @@
         <v>42</v>
       </c>
       <c r="V56" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -37446,7 +37449,7 @@
         <v>6</v>
       </c>
       <c r="F60" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G60" t="s">
         <v>8</v>
@@ -37476,7 +37479,7 @@
         <v>6</v>
       </c>
       <c r="W60" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="X60" t="s">
         <v>8</v>
@@ -37508,7 +37511,7 @@
         <v>6</v>
       </c>
       <c r="F61" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G61" t="s">
         <v>8</v>
@@ -37538,7 +37541,7 @@
         <v>6</v>
       </c>
       <c r="W61" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X61" t="s">
         <v>8</v>
@@ -37570,7 +37573,7 @@
         <v>6</v>
       </c>
       <c r="F62" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G62" t="s">
         <v>8</v>
@@ -37600,7 +37603,7 @@
         <v>6</v>
       </c>
       <c r="W62" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X62" t="s">
         <v>8</v>
@@ -37632,7 +37635,7 @@
         <v>6</v>
       </c>
       <c r="F63" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G63" t="s">
         <v>8</v>
@@ -37662,7 +37665,7 @@
         <v>6</v>
       </c>
       <c r="W63" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X63" t="s">
         <v>8</v>
@@ -37694,7 +37697,7 @@
         <v>6</v>
       </c>
       <c r="F64" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G64" t="s">
         <v>8</v>
@@ -37724,7 +37727,7 @@
         <v>6</v>
       </c>
       <c r="W64" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X64" t="s">
         <v>8</v>
@@ -37756,7 +37759,7 @@
         <v>6</v>
       </c>
       <c r="F65" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G65" t="s">
         <v>8</v>
@@ -37786,7 +37789,7 @@
         <v>6</v>
       </c>
       <c r="W65" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X65" t="s">
         <v>8</v>
@@ -37818,7 +37821,7 @@
         <v>6</v>
       </c>
       <c r="F66" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G66" t="s">
         <v>8</v>
@@ -37848,7 +37851,7 @@
         <v>6</v>
       </c>
       <c r="W66" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X66" t="s">
         <v>8</v>
@@ -37880,7 +37883,7 @@
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G67" t="s">
         <v>8</v>
@@ -37910,7 +37913,7 @@
         <v>6</v>
       </c>
       <c r="W67" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X67" t="s">
         <v>8</v>
@@ -37942,7 +37945,7 @@
         <v>6</v>
       </c>
       <c r="F68" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G68" t="s">
         <v>8</v>
@@ -37972,7 +37975,7 @@
         <v>6</v>
       </c>
       <c r="W68" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X68" t="s">
         <v>8</v>
@@ -38004,7 +38007,7 @@
         <v>6</v>
       </c>
       <c r="F69" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G69" t="s">
         <v>8</v>
@@ -38034,7 +38037,7 @@
         <v>6</v>
       </c>
       <c r="W69" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X69" t="s">
         <v>8</v>
@@ -38066,7 +38069,7 @@
         <v>6</v>
       </c>
       <c r="F70" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G70" t="s">
         <v>8</v>
@@ -38096,7 +38099,7 @@
         <v>6</v>
       </c>
       <c r="W70" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X70" t="s">
         <v>8</v>
@@ -38128,7 +38131,7 @@
         <v>6</v>
       </c>
       <c r="F71" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G71" t="s">
         <v>8</v>
@@ -38158,7 +38161,7 @@
         <v>6</v>
       </c>
       <c r="W71" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X71" t="s">
         <v>8</v>
@@ -38190,7 +38193,7 @@
         <v>6</v>
       </c>
       <c r="F72" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G72" t="s">
         <v>8</v>
@@ -38220,7 +38223,7 @@
         <v>6</v>
       </c>
       <c r="W72" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X72" t="s">
         <v>8</v>
@@ -38252,7 +38255,7 @@
         <v>6</v>
       </c>
       <c r="F73" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G73" t="s">
         <v>8</v>
@@ -38282,7 +38285,7 @@
         <v>6</v>
       </c>
       <c r="W73" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="X73" t="s">
         <v>8</v>
@@ -38393,7 +38396,7 @@
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H80" t="s">
         <v>39</v>
@@ -38421,7 +38424,7 @@
         <v>38</v>
       </c>
       <c r="X80" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="Y80" t="s">
         <v>39</v>
@@ -38445,7 +38448,7 @@
         <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -38460,7 +38463,7 @@
         <v>42</v>
       </c>
       <c r="V81" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -38546,7 +38549,7 @@
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G85" t="s">
         <v>8</v>
@@ -38576,7 +38579,7 @@
         <v>6</v>
       </c>
       <c r="W85" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="X85" t="s">
         <v>8</v>
@@ -38608,7 +38611,7 @@
         <v>6</v>
       </c>
       <c r="F86" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G86" t="s">
         <v>8</v>
@@ -38638,7 +38641,7 @@
         <v>6</v>
       </c>
       <c r="W86" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X86" t="s">
         <v>8</v>
@@ -38670,7 +38673,7 @@
         <v>6</v>
       </c>
       <c r="F87" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G87" t="s">
         <v>8</v>
@@ -38700,7 +38703,7 @@
         <v>6</v>
       </c>
       <c r="W87" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X87" t="s">
         <v>8</v>
@@ -38732,7 +38735,7 @@
         <v>6</v>
       </c>
       <c r="F88" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G88" t="s">
         <v>8</v>
@@ -38762,7 +38765,7 @@
         <v>6</v>
       </c>
       <c r="W88" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X88" t="s">
         <v>8</v>
@@ -38794,7 +38797,7 @@
         <v>6</v>
       </c>
       <c r="F89" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G89" t="s">
         <v>8</v>
@@ -38824,7 +38827,7 @@
         <v>6</v>
       </c>
       <c r="W89" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X89" t="s">
         <v>8</v>
@@ -38856,7 +38859,7 @@
         <v>6</v>
       </c>
       <c r="F90" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G90" t="s">
         <v>8</v>
@@ -38886,7 +38889,7 @@
         <v>6</v>
       </c>
       <c r="W90" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X90" t="s">
         <v>8</v>
@@ -38918,7 +38921,7 @@
         <v>6</v>
       </c>
       <c r="F91" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G91" t="s">
         <v>8</v>
@@ -38948,7 +38951,7 @@
         <v>6</v>
       </c>
       <c r="W91" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X91" t="s">
         <v>8</v>
@@ -38980,7 +38983,7 @@
         <v>6</v>
       </c>
       <c r="F92" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G92" t="s">
         <v>8</v>
@@ -39010,7 +39013,7 @@
         <v>6</v>
       </c>
       <c r="W92" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="X92" t="s">
         <v>8</v>
@@ -39042,7 +39045,7 @@
         <v>6</v>
       </c>
       <c r="F93" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G93" t="s">
         <v>8</v>
@@ -39072,7 +39075,7 @@
         <v>6</v>
       </c>
       <c r="W93" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="X93" t="s">
         <v>8</v>
@@ -39104,7 +39107,7 @@
         <v>6</v>
       </c>
       <c r="F94" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G94" t="s">
         <v>8</v>
@@ -39134,7 +39137,7 @@
         <v>6</v>
       </c>
       <c r="W94" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="X94" t="s">
         <v>8</v>
@@ -39166,7 +39169,7 @@
         <v>6</v>
       </c>
       <c r="F95" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G95" t="s">
         <v>8</v>
@@ -39196,7 +39199,7 @@
         <v>6</v>
       </c>
       <c r="W95" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="X95" t="s">
         <v>8</v>
@@ -39228,7 +39231,7 @@
         <v>6</v>
       </c>
       <c r="F96" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G96" t="s">
         <v>8</v>
@@ -39258,7 +39261,7 @@
         <v>6</v>
       </c>
       <c r="W96" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="X96" t="s">
         <v>8</v>
@@ -39290,7 +39293,7 @@
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G97" t="s">
         <v>8</v>
@@ -39320,7 +39323,7 @@
         <v>6</v>
       </c>
       <c r="W97" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="X97" t="s">
         <v>8</v>
@@ -39352,7 +39355,7 @@
         <v>6</v>
       </c>
       <c r="F98" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G98" t="s">
         <v>8</v>
@@ -39382,7 +39385,7 @@
         <v>6</v>
       </c>
       <c r="W98" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="X98" t="s">
         <v>8</v>
@@ -39445,6 +39448,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE1E5043F2CF384FB5FE4BAABF9D3983" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0614cff9d23b461af25b2cda1cf9368">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="386adf9787ee73c67b04c35b5de66464">
     <xsd:element name="properties">
@@ -39558,22 +39576,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15B9ACA7-37DF-4944-968A-289D2787D7C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39587,27 +39613,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF0E59F2-971D-44F0-9248-BBD9881E8E1B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added some analysis for the biomechnet model and the RRA recommendations for it. Turns out very similar to the regular model.
</commit_message>
<xml_diff>
--- a/RRAMassMods.xlsx
+++ b/RRAMassMods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F1B6D9-37FB-41A0-871E-E555D189D697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5FC593-46D4-4BAA-A695-424B9BFC1539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="5" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="welk001" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="welk003" sheetId="3" r:id="rId3"/>
     <sheet name="welk004" sheetId="4" r:id="rId4"/>
     <sheet name="welk007" sheetId="5" r:id="rId5"/>
-    <sheet name="welk008" sheetId="6" r:id="rId6"/>
-    <sheet name="welk009" sheetId="8" r:id="rId7"/>
-    <sheet name="welk010" sheetId="9" r:id="rId8"/>
+    <sheet name="scalecomparison_welk007" sheetId="10" r:id="rId6"/>
+    <sheet name="welk008" sheetId="6" r:id="rId7"/>
+    <sheet name="welk009" sheetId="8" r:id="rId8"/>
+    <sheet name="welk010" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10440" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10747" uniqueCount="257">
   <si>
     <t>welk001</t>
   </si>
@@ -771,6 +772,48 @@
   <si>
     <t>~[-0.0225941,0.278266,0.0625015]</t>
   </si>
+  <si>
+    <t>=0.1,</t>
+  </si>
+  <si>
+    <t>~[-0.1225,0.297823,0.0566875]</t>
+  </si>
+  <si>
+    <t>4.81156,</t>
+  </si>
+  <si>
+    <t>12.393,</t>
+  </si>
+  <si>
+    <t>3.44679,</t>
+  </si>
+  <si>
+    <t>0.0588736,</t>
+  </si>
+  <si>
+    <t>0.0603738,</t>
+  </si>
+  <si>
+    <t>1.09908,</t>
+  </si>
+  <si>
+    <t>0.197674,</t>
+  </si>
+  <si>
+    <t>11.9396,</t>
+  </si>
+  <si>
+    <t>3.21747,</t>
+  </si>
+  <si>
+    <t>0.0776112,</t>
+  </si>
+  <si>
+    <t>0.912511,</t>
+  </si>
+  <si>
+    <t>18.73,</t>
+  </si>
 </sst>
 </file>
 
@@ -20269,8 +20312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FE46D1-E00B-478F-BC49-0EAED21FA345}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25066,6 +25109,1118 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEEB2EB-E9EC-4D82-BF7C-6EAF7158FF55}">
+  <dimension ref="A1:U23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6:X23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2">
+        <f>-0.0566875</f>
+        <v>-5.6687500000000002E-2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T2">
+        <f>-0.0429516</f>
+        <v>-4.29516E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>1.8652299999999999</v>
+      </c>
+      <c r="L6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6">
+        <v>1.80986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>4.9684600000000003</v>
+      </c>
+      <c r="L7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>143</v>
+      </c>
+      <c r="R7" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U7">
+        <v>9.2246699999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>246</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>12.7971</v>
+      </c>
+      <c r="L8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>144</v>
+      </c>
+      <c r="R8" t="s">
+        <v>8</v>
+      </c>
+      <c r="S8" t="s">
+        <v>5</v>
+      </c>
+      <c r="T8" t="s">
+        <v>6</v>
+      </c>
+      <c r="U8">
+        <v>7.28559</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>3.55918</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>145</v>
+      </c>
+      <c r="R9" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" t="s">
+        <v>5</v>
+      </c>
+      <c r="T9" t="s">
+        <v>6</v>
+      </c>
+      <c r="U9">
+        <v>2.90401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>248</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>6.0793399999999997E-2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>146</v>
+      </c>
+      <c r="R10" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" t="s">
+        <v>5</v>
+      </c>
+      <c r="T10" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10">
+        <v>6.7518599999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>6.2342500000000002E-2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>147</v>
+      </c>
+      <c r="R11" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" t="s">
+        <v>5</v>
+      </c>
+      <c r="T11" t="s">
+        <v>6</v>
+      </c>
+      <c r="U11">
+        <v>7.8327900000000006E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>250</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>1.1349199999999999</v>
+      </c>
+      <c r="L12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>148</v>
+      </c>
+      <c r="R12" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" t="s">
+        <v>5</v>
+      </c>
+      <c r="T12" t="s">
+        <v>6</v>
+      </c>
+      <c r="U12">
+        <v>0.97909800000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>251</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>0.20412</v>
+      </c>
+      <c r="L13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>149</v>
+      </c>
+      <c r="R13" t="s">
+        <v>8</v>
+      </c>
+      <c r="S13" t="s">
+        <v>5</v>
+      </c>
+      <c r="T13" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13">
+        <v>0.169658</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>252</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>12.329000000000001</v>
+      </c>
+      <c r="L14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" t="s">
+        <v>4</v>
+      </c>
+      <c r="O14" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>144</v>
+      </c>
+      <c r="R14" t="s">
+        <v>8</v>
+      </c>
+      <c r="S14" t="s">
+        <v>5</v>
+      </c>
+      <c r="T14" t="s">
+        <v>6</v>
+      </c>
+      <c r="U14">
+        <v>7.28559</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>253</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>3.32239</v>
+      </c>
+      <c r="L15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>145</v>
+      </c>
+      <c r="R15" t="s">
+        <v>8</v>
+      </c>
+      <c r="S15" t="s">
+        <v>5</v>
+      </c>
+      <c r="T15" t="s">
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <v>2.90401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>248</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>6.0793399999999997E-2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" t="s">
+        <v>4</v>
+      </c>
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>146</v>
+      </c>
+      <c r="R16" t="s">
+        <v>8</v>
+      </c>
+      <c r="S16" t="s">
+        <v>5</v>
+      </c>
+      <c r="T16" t="s">
+        <v>6</v>
+      </c>
+      <c r="U16">
+        <v>6.7518599999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>254</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>8.0141900000000002E-2</v>
+      </c>
+      <c r="L17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>147</v>
+      </c>
+      <c r="R17" t="s">
+        <v>8</v>
+      </c>
+      <c r="S17" t="s">
+        <v>5</v>
+      </c>
+      <c r="T17" t="s">
+        <v>6</v>
+      </c>
+      <c r="U17">
+        <v>7.8327900000000006E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>255</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>0.94226600000000005</v>
+      </c>
+      <c r="L18" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O18" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>148</v>
+      </c>
+      <c r="R18" t="s">
+        <v>8</v>
+      </c>
+      <c r="S18" t="s">
+        <v>5</v>
+      </c>
+      <c r="T18" t="s">
+        <v>6</v>
+      </c>
+      <c r="U18">
+        <v>0.97909800000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>251</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>0.20412</v>
+      </c>
+      <c r="L19" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" t="s">
+        <v>26</v>
+      </c>
+      <c r="N19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>149</v>
+      </c>
+      <c r="R19" t="s">
+        <v>8</v>
+      </c>
+      <c r="S19" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" t="s">
+        <v>6</v>
+      </c>
+      <c r="U19">
+        <v>0.169658</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>256</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>19.340800000000002</v>
+      </c>
+      <c r="L20" t="s">
+        <v>2</v>
+      </c>
+      <c r="M20" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" t="s">
+        <v>4</v>
+      </c>
+      <c r="O20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>150</v>
+      </c>
+      <c r="R20" t="s">
+        <v>8</v>
+      </c>
+      <c r="S20" t="s">
+        <v>5</v>
+      </c>
+      <c r="T20" t="s">
+        <v>6</v>
+      </c>
+      <c r="U20">
+        <v>26.816800000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T21" t="s">
+        <v>38</v>
+      </c>
+      <c r="U21">
+        <v>-4.1842499999999998E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T22" t="s">
+        <v>115</v>
+      </c>
+      <c r="U22">
+        <v>0.28064099999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T23" t="s">
+        <v>39</v>
+      </c>
+      <c r="U23">
+        <v>4.29516E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496F406B-9F45-42EE-B158-3DE2F835AB32}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
@@ -29859,11 +31014,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53024F3-9755-4748-94E9-291178E5B6E2}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
@@ -34653,7 +35808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7434A9A0-AC1F-42B5-B8C4-F9AFA5AAB5A4}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
@@ -39448,21 +40603,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AE1E5043F2CF384FB5FE4BAABF9D3983" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b0614cff9d23b461af25b2cda1cf9368">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="386adf9787ee73c67b04c35b5de66464">
     <xsd:element name="properties">
@@ -39576,17 +40716,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15B9ACA7-37DF-4944-968A-289D2787D7C8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39600,17 +40756,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15B9ACA7-37DF-4944-968A-289D2787D7C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{399FE168-8224-4CD3-BB9D-EAE6AF2DB1C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating some of the subjects. Last one was a change for subject 9 b/c a gait cycle had some weird marker issues.
</commit_message>
<xml_diff>
--- a/RRAMassMods.xlsx
+++ b/RRAMassMods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Exotendon\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EA43BA-45B0-435A-9A5D-CA5BC679F978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CE97E2-F6E2-43BF-9ACB-1D7B968A8E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="732" firstSheet="3" activeTab="7" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="732" firstSheet="3" activeTab="8" xr2:uid="{A9A968C2-5FC9-4213-B348-16BA6D341DAE}"/>
   </bookViews>
   <sheets>
     <sheet name="welk001" sheetId="1" r:id="rId1"/>
@@ -763,15 +763,6 @@
     <t>~[0.0218834,0.280641,0.00342408]</t>
   </si>
   <si>
-    <t>~[0.0661084,0.280641,0.00500517]</t>
-  </si>
-  <si>
-    <t>=-0.0960399,</t>
-  </si>
-  <si>
-    <t>~[0.0621483,0.280641,0.00238657]</t>
-  </si>
-  <si>
     <t>=-0.0975418,</t>
   </si>
   <si>
@@ -848,18 +839,6 @@
   </si>
   <si>
     <t>~[-0.0240261,0.278266,0.0398701]</t>
-  </si>
-  <si>
-    <t>=-0.00599552,</t>
-  </si>
-  <si>
-    <t>~[-0.0279689,0.278266,0.0657692]</t>
-  </si>
-  <si>
-    <t>=-0.0151985,</t>
-  </si>
-  <si>
-    <t>~[-0.0187659,0.278266,0.0566468]</t>
   </si>
   <si>
     <t>=-0.0803238,</t>
@@ -962,6 +941,27 @@
   </si>
   <si>
     <t>~[0.0656651,0.326035,0.0088235]</t>
+  </si>
+  <si>
+    <t>=-0.0978895,</t>
+  </si>
+  <si>
+    <t>~[0.063998,0.280641,0.0101076]</t>
+  </si>
+  <si>
+    <t>~[0.0661084,0.280641,0.0127857]</t>
+  </si>
+  <si>
+    <t>=-0.0141532,</t>
+  </si>
+  <si>
+    <t>~[-0.0198112,0.278266,0.0637831]</t>
+  </si>
+  <si>
+    <t>=-0.0184548,</t>
+  </si>
+  <si>
+    <t>~[-0.0155096,0.278266,0.0513122]</t>
   </si>
 </sst>
 </file>
@@ -6188,7 +6188,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
@@ -6216,7 +6216,7 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
@@ -6240,7 +6240,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -6255,7 +6255,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -7654,7 +7654,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
@@ -7682,7 +7682,7 @@
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="Y30" t="s">
         <v>39</v>
@@ -7706,7 +7706,7 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -7721,7 +7721,7 @@
         <v>42</v>
       </c>
       <c r="V31" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -8754,7 +8754,7 @@
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H55" t="s">
         <v>39</v>
@@ -8782,7 +8782,7 @@
         <v>38</v>
       </c>
       <c r="X55" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="Y55" t="s">
         <v>39</v>
@@ -8806,7 +8806,7 @@
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -8821,7 +8821,7 @@
         <v>42</v>
       </c>
       <c r="V56" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -9854,7 +9854,7 @@
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="H80" t="s">
         <v>39</v>
@@ -9882,7 +9882,7 @@
         <v>38</v>
       </c>
       <c r="X80" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="Y80" t="s">
         <v>39</v>
@@ -9906,7 +9906,7 @@
         <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -9921,7 +9921,7 @@
         <v>42</v>
       </c>
       <c r="V81" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -11536,7 +11536,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
@@ -11564,7 +11564,7 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
@@ -11588,7 +11588,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -11603,7 +11603,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -13002,7 +13002,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
@@ -13030,7 +13030,7 @@
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="Y30" t="s">
         <v>39</v>
@@ -13054,7 +13054,7 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -13069,7 +13069,7 @@
         <v>42</v>
       </c>
       <c r="V31" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -14102,7 +14102,7 @@
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H55" t="s">
         <v>39</v>
@@ -14130,7 +14130,7 @@
         <v>38</v>
       </c>
       <c r="X55" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="Y55" t="s">
         <v>39</v>
@@ -14154,7 +14154,7 @@
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -14169,7 +14169,7 @@
         <v>42</v>
       </c>
       <c r="V56" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -15202,7 +15202,7 @@
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H80" t="s">
         <v>39</v>
@@ -15230,7 +15230,7 @@
         <v>38</v>
       </c>
       <c r="X80" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="Y80" t="s">
         <v>39</v>
@@ -15254,7 +15254,7 @@
         <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -15269,7 +15269,7 @@
         <v>42</v>
       </c>
       <c r="V81" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -35500,14 +35500,14 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>141</v>
+        <v>298</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
       </c>
       <c r="Z5">
-        <f>-0.00500517</f>
-        <v>-5.0051699999999998E-3</v>
+        <f>-0.0101076</f>
+        <v>-1.01076E-2</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
@@ -35539,7 +35539,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>238</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -35608,7 +35608,7 @@
         <v>48</v>
       </c>
       <c r="V9">
-        <v>2.99607</v>
+        <v>3.1435599999999999</v>
       </c>
       <c r="AC9" t="s">
         <v>105</v>
@@ -35683,21 +35683,21 @@
         <v>6</v>
       </c>
       <c r="AA10">
-        <v>9.4101099999999995</v>
+        <v>9.4331600000000009</v>
       </c>
       <c r="AC10" t="s">
         <v>3</v>
       </c>
       <c r="AD10">
         <f>AVERAGE(AA10,AA34,AA59,AA84)</f>
-        <v>9.4128249999999998</v>
+        <v>9.4229824999999998</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AH10">
         <f>AVERAGE(AA10,AA34,AA59,AA84,J85,J60,J35,J10)</f>
-        <v>9.3159187500000016</v>
+        <v>9.3209975000000007</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -35766,21 +35766,21 @@
         <v>6</v>
       </c>
       <c r="AA11">
-        <v>7.4320399999999998</v>
+        <v>7.4502499999999996</v>
       </c>
       <c r="AC11" t="s">
         <v>9</v>
       </c>
       <c r="AD11">
         <f t="shared" ref="AD11:AD26" si="1">AVERAGE(AA11,AA35,AA60,AA85)</f>
-        <v>7.4341875000000002</v>
+        <v>7.4422125000000001</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AH11">
         <f t="shared" ref="AH11:AH25" si="2">AVERAGE(AA11,AA35,AA60,AA85,J86,J61,J36,J11)</f>
-        <v>7.3576524999999995</v>
+        <v>7.3616649999999995</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -35849,21 +35849,21 @@
         <v>6</v>
       </c>
       <c r="AA12">
-        <v>2.96238</v>
+        <v>2.9696400000000001</v>
       </c>
       <c r="AC12" t="s">
         <v>11</v>
       </c>
       <c r="AD12">
         <f t="shared" si="1"/>
-        <v>2.9632375</v>
+        <v>2.9664349999999997</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AH12">
         <f>AVERAGE(AA12,AA36,AA61,AA86,J87,J62,J37,J12)</f>
-        <v>2.9327312500000002</v>
+        <v>2.9343300000000001</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -35932,21 +35932,21 @@
         <v>6</v>
       </c>
       <c r="AA13">
-        <v>6.8875900000000004E-2</v>
+        <v>6.9044599999999998E-2</v>
       </c>
       <c r="AC13" t="s">
         <v>13</v>
       </c>
       <c r="AD13">
         <f t="shared" si="1"/>
-        <v>6.8895750000000006E-2</v>
+        <v>6.8970100000000006E-2</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AH13">
         <f t="shared" si="2"/>
-        <v>6.8186474999999996E-2</v>
+        <v>6.8223649999999997E-2</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -36015,21 +36015,21 @@
         <v>6</v>
       </c>
       <c r="AA14">
-        <v>7.9902399999999998E-2</v>
+        <v>8.0098199999999994E-2</v>
       </c>
       <c r="AC14" t="s">
         <v>15</v>
       </c>
       <c r="AD14">
         <f t="shared" si="1"/>
-        <v>7.9925474999999996E-2</v>
+        <v>8.0011749999999993E-2</v>
       </c>
       <c r="AG14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>7.9102649999999997E-2</v>
+        <v>7.9145787499999995E-2</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
@@ -36098,21 +36098,21 @@
         <v>6</v>
       </c>
       <c r="AA15">
-        <v>0.99878</v>
+        <v>1.0012300000000001</v>
       </c>
       <c r="AC15" t="s">
         <v>17</v>
       </c>
       <c r="AD15">
         <f t="shared" si="1"/>
-        <v>0.99906875000000006</v>
+        <v>1.00014775</v>
       </c>
       <c r="AG15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AH15">
         <f t="shared" si="2"/>
-        <v>0.98878325000000022</v>
+        <v>0.98932275000000014</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
@@ -36181,21 +36181,21 @@
         <v>6</v>
       </c>
       <c r="AA16">
-        <v>0.173069</v>
+        <v>0.17349300000000001</v>
       </c>
       <c r="AC16" t="s">
         <v>19</v>
       </c>
       <c r="AD16">
         <f t="shared" si="1"/>
-        <v>0.17311874999999999</v>
+        <v>0.1733055</v>
       </c>
       <c r="AG16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AH16">
         <f t="shared" si="2"/>
-        <v>0.17133637499999999</v>
+        <v>0.17142974999999999</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -36264,21 +36264,21 @@
         <v>6</v>
       </c>
       <c r="AA17">
-        <v>7.4320399999999998</v>
+        <v>7.4502499999999996</v>
       </c>
       <c r="AC17" t="s">
         <v>21</v>
       </c>
       <c r="AD17">
         <f t="shared" si="1"/>
-        <v>7.4341875000000002</v>
+        <v>7.4422125000000001</v>
       </c>
       <c r="AG17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="AH17">
         <f t="shared" si="2"/>
-        <v>7.3576524999999995</v>
+        <v>7.3616649999999995</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -36347,21 +36347,21 @@
         <v>6</v>
       </c>
       <c r="AA18">
-        <v>2.96238</v>
+        <v>2.9696400000000001</v>
       </c>
       <c r="AC18" t="s">
         <v>22</v>
       </c>
       <c r="AD18">
         <f t="shared" si="1"/>
-        <v>2.9632375</v>
+        <v>2.9664349999999997</v>
       </c>
       <c r="AG18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="AH18">
         <f t="shared" si="2"/>
-        <v>2.9327312500000002</v>
+        <v>2.9343300000000001</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
@@ -36430,21 +36430,21 @@
         <v>6</v>
       </c>
       <c r="AA19">
-        <v>6.8875900000000004E-2</v>
+        <v>6.9044599999999998E-2</v>
       </c>
       <c r="AC19" t="s">
         <v>23</v>
       </c>
       <c r="AD19">
         <f t="shared" si="1"/>
-        <v>6.8895750000000006E-2</v>
+        <v>6.8970100000000006E-2</v>
       </c>
       <c r="AG19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AH19">
         <f t="shared" si="2"/>
-        <v>6.8186474999999996E-2</v>
+        <v>6.8223649999999997E-2</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -36513,21 +36513,21 @@
         <v>6</v>
       </c>
       <c r="AA20">
-        <v>7.9902399999999998E-2</v>
+        <v>8.0098199999999994E-2</v>
       </c>
       <c r="AC20" t="s">
         <v>24</v>
       </c>
       <c r="AD20">
         <f t="shared" si="1"/>
-        <v>7.9925474999999996E-2</v>
+        <v>8.0011749999999993E-2</v>
       </c>
       <c r="AG20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="AH20">
         <f t="shared" si="2"/>
-        <v>7.9102649999999997E-2</v>
+        <v>7.9145787499999995E-2</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
@@ -36596,21 +36596,21 @@
         <v>6</v>
       </c>
       <c r="AA21">
-        <v>0.99878</v>
+        <v>1.0012300000000001</v>
       </c>
       <c r="AC21" t="s">
         <v>25</v>
       </c>
       <c r="AD21">
         <f t="shared" si="1"/>
-        <v>0.99906875000000006</v>
+        <v>1.00014775</v>
       </c>
       <c r="AG21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AH21">
         <f t="shared" si="2"/>
-        <v>0.98878325000000022</v>
+        <v>0.98932275000000014</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -36679,21 +36679,21 @@
         <v>6</v>
       </c>
       <c r="AA22">
-        <v>0.173069</v>
+        <v>0.17349300000000001</v>
       </c>
       <c r="AC22" t="s">
         <v>26</v>
       </c>
       <c r="AD22">
         <f t="shared" si="1"/>
-        <v>0.17311874999999999</v>
+        <v>0.1733055</v>
       </c>
       <c r="AG22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AH22">
         <f t="shared" si="2"/>
-        <v>0.17133637499999999</v>
+        <v>0.17142974999999999</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -36762,21 +36762,21 @@
         <v>6</v>
       </c>
       <c r="AA23">
-        <v>27.355899999999998</v>
+        <v>27.422899999999998</v>
       </c>
       <c r="AC23" t="s">
         <v>27</v>
       </c>
       <c r="AD23">
         <f t="shared" si="1"/>
-        <v>27.363775000000004</v>
+        <v>27.393300000000004</v>
       </c>
       <c r="AG23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AH23">
         <f t="shared" si="2"/>
-        <v>27.082062500000003</v>
+        <v>27.096825000000003</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -36797,21 +36797,21 @@
         <v>38</v>
       </c>
       <c r="AA24">
-        <v>6.6108399999999998E-2</v>
+        <v>6.3997999999999999E-2</v>
       </c>
       <c r="AC24" t="s">
         <v>38</v>
       </c>
       <c r="AD24">
         <f t="shared" si="1"/>
-        <v>6.3083324999999996E-2</v>
+        <v>6.3545749999999998E-2</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="AH24">
         <f t="shared" si="2"/>
-        <v>4.1118362499999998E-2</v>
+        <v>4.1349575E-2</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -36867,21 +36867,21 @@
         <v>39</v>
       </c>
       <c r="AA26">
-        <v>5.0051699999999998E-3</v>
+        <v>1.01076E-2</v>
       </c>
       <c r="AC26" t="s">
         <v>39</v>
       </c>
       <c r="AD26">
         <f t="shared" si="1"/>
-        <v>5.5405999999999997E-3</v>
+        <v>9.4159900000000008E-3</v>
       </c>
       <c r="AG26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AH26">
         <f>AVERAGE(AA26,AA50,AA75,AA100,J101,J76,J51,J26)</f>
-        <v>3.5423550000000001E-3</v>
+        <v>5.4800500000000011E-3</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
@@ -36938,14 +36938,14 @@
         <v>38</v>
       </c>
       <c r="X29" t="s">
-        <v>239</v>
+        <v>141</v>
       </c>
       <c r="Y29" t="s">
         <v>39</v>
       </c>
       <c r="Z29">
-        <f>-0.00238657</f>
-        <v>-2.3865700000000002E-3</v>
+        <f>-0.0127857</f>
+        <v>-1.2785700000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
@@ -36990,7 +36990,7 @@
         <v>42</v>
       </c>
       <c r="V30" t="s">
-        <v>240</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
@@ -37056,7 +37056,7 @@
         <v>48</v>
       </c>
       <c r="V33">
-        <v>2.8673899999999999</v>
+        <v>2.9798399999999998</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.25">
@@ -37103,7 +37103,7 @@
         <v>6</v>
       </c>
       <c r="AA34">
-        <v>9.3899899999999992</v>
+        <v>9.4075699999999998</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.25">
@@ -37165,7 +37165,7 @@
         <v>6</v>
       </c>
       <c r="AA35">
-        <v>7.41615</v>
+        <v>7.43004</v>
       </c>
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.25">
@@ -37227,7 +37227,7 @@
         <v>6</v>
       </c>
       <c r="AA36">
-        <v>2.9560499999999998</v>
+        <v>2.9615800000000001</v>
       </c>
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
@@ -37289,7 +37289,7 @@
         <v>6</v>
       </c>
       <c r="AA37">
-        <v>6.8728600000000001E-2</v>
+        <v>6.8857299999999996E-2</v>
       </c>
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.25">
@@ -37351,7 +37351,7 @@
         <v>6</v>
       </c>
       <c r="AA38">
-        <v>7.97316E-2</v>
+        <v>7.9880900000000005E-2</v>
       </c>
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.25">
@@ -37413,7 +37413,7 @@
         <v>6</v>
       </c>
       <c r="AA39">
-        <v>0.996645</v>
+        <v>0.99851100000000004</v>
       </c>
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.25">
@@ -37475,7 +37475,7 @@
         <v>6</v>
       </c>
       <c r="AA40">
-        <v>0.17269899999999999</v>
+        <v>0.17302200000000001</v>
       </c>
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.25">
@@ -37537,7 +37537,7 @@
         <v>6</v>
       </c>
       <c r="AA41">
-        <v>7.41615</v>
+        <v>7.43004</v>
       </c>
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.25">
@@ -37599,7 +37599,7 @@
         <v>6</v>
       </c>
       <c r="AA42">
-        <v>2.9560499999999998</v>
+        <v>2.9615800000000001</v>
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.25">
@@ -37661,7 +37661,7 @@
         <v>6</v>
       </c>
       <c r="AA43">
-        <v>6.8728600000000001E-2</v>
+        <v>6.8857299999999996E-2</v>
       </c>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.25">
@@ -37723,7 +37723,7 @@
         <v>6</v>
       </c>
       <c r="AA44">
-        <v>7.97316E-2</v>
+        <v>7.9880900000000005E-2</v>
       </c>
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
@@ -37785,7 +37785,7 @@
         <v>6</v>
       </c>
       <c r="AA45">
-        <v>0.996645</v>
+        <v>0.99851100000000004</v>
       </c>
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.25">
@@ -37847,7 +37847,7 @@
         <v>6</v>
       </c>
       <c r="AA46">
-        <v>0.17269899999999999</v>
+        <v>0.17302200000000001</v>
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
@@ -37909,7 +37909,7 @@
         <v>6</v>
       </c>
       <c r="AA47">
-        <v>27.2974</v>
+        <v>27.348500000000001</v>
       </c>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
@@ -37947,7 +37947,7 @@
         <v>38</v>
       </c>
       <c r="AA48">
-        <v>6.2148299999999997E-2</v>
+        <v>6.6108399999999998E-2</v>
       </c>
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.25">
@@ -37975,7 +37975,7 @@
         <v>39</v>
       </c>
       <c r="AA50">
-        <v>2.3865700000000002E-3</v>
+        <v>1.2785700000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.25">
@@ -38040,7 +38040,7 @@
         <v>38</v>
       </c>
       <c r="X54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="Y54" t="s">
         <v>39</v>
@@ -38092,7 +38092,7 @@
         <v>42</v>
       </c>
       <c r="V55" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
@@ -39142,7 +39142,7 @@
         <v>38</v>
       </c>
       <c r="X79" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="Y79" t="s">
         <v>39</v>
@@ -39194,7 +39194,7 @@
         <v>42</v>
       </c>
       <c r="V80" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
@@ -41312,7 +41312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{496F406B-9F45-42EE-B158-3DE2F835AB32}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="P9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
@@ -41388,7 +41388,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
@@ -41440,7 +41440,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -41455,7 +41455,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -42854,7 +42854,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
@@ -42906,7 +42906,7 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -42921,7 +42921,7 @@
         <v>42</v>
       </c>
       <c r="V31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -43954,7 +43954,7 @@
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H55" t="s">
         <v>39</v>
@@ -44006,7 +44006,7 @@
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -44021,7 +44021,7 @@
         <v>42</v>
       </c>
       <c r="V56" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -45054,7 +45054,7 @@
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H80" t="s">
         <v>39</v>
@@ -45106,7 +45106,7 @@
         <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -45121,7 +45121,7 @@
         <v>42</v>
       </c>
       <c r="V81" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -46110,7 +46110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A53024F3-9755-4748-94E9-291178E5B6E2}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AH26" sqref="AH26"/>
     </sheetView>
   </sheetViews>
@@ -46183,7 +46183,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
@@ -46211,7 +46211,7 @@
         <v>38</v>
       </c>
       <c r="X5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="Y5" t="s">
         <v>39</v>
@@ -46235,7 +46235,7 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="R6" t="s">
         <v>2</v>
@@ -46250,7 +46250,7 @@
         <v>42</v>
       </c>
       <c r="V6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
@@ -46401,14 +46401,14 @@
       </c>
       <c r="AD10">
         <f>AVERAGE(AA10,AA35,AA60,AA85)</f>
-        <v>8.5466625000000001</v>
+        <v>8.5403924999999994</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AH10">
         <f>AVERAGE(AA10,AA35,AA60,AA85,J85,J60,J35,J10)</f>
-        <v>8.6332249999999995</v>
+        <v>8.6300899999999992</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
@@ -46484,14 +46484,14 @@
       </c>
       <c r="AD11">
         <f t="shared" ref="AD11:AD26" si="1">AVERAGE(AA11,AA36,AA61,AA86)</f>
-        <v>6.7500999999999998</v>
+        <v>6.7451500000000006</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AH11">
         <f t="shared" ref="AH11:AH26" si="2">AVERAGE(AA11,AA36,AA61,AA86,J86,J61,J36,J11)</f>
-        <v>6.8184662500000002</v>
+        <v>6.8159912500000015</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
@@ -46567,14 +46567,14 @@
       </c>
       <c r="AD12">
         <f t="shared" si="1"/>
-        <v>2.6905625</v>
+        <v>2.6885874999999997</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AH12">
         <f t="shared" si="2"/>
-        <v>2.7178125</v>
+        <v>2.7168249999999996</v>
       </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
@@ -46650,14 +46650,14 @@
       </c>
       <c r="AD13">
         <f t="shared" si="1"/>
-        <v>6.2556025000000001E-2</v>
+        <v>6.2510150000000014E-2</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AH13">
         <f t="shared" si="2"/>
-        <v>6.3189612500000006E-2</v>
+        <v>6.3166675000000005E-2</v>
       </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
@@ -46733,14 +46733,14 @@
       </c>
       <c r="AD14">
         <f t="shared" si="1"/>
-        <v>7.2570775000000004E-2</v>
+        <v>7.2517575000000001E-2</v>
       </c>
       <c r="AG14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>7.3305787499999997E-2</v>
+        <v>7.3279187499999995E-2</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
@@ -46816,14 +46816,14 @@
       </c>
       <c r="AD15">
         <f t="shared" si="1"/>
-        <v>0.90713450000000007</v>
+        <v>0.90646950000000004</v>
       </c>
       <c r="AG15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AH15">
         <f t="shared" si="2"/>
-        <v>0.91632237500000002</v>
+        <v>0.91598987500000006</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
@@ -46899,14 +46899,14 @@
       </c>
       <c r="AD16">
         <f t="shared" si="1"/>
-        <v>0.15718824999999997</v>
+        <v>0.15707325</v>
       </c>
       <c r="AG16" s="1" t="s">
         <v>19</v>
       </c>
       <c r="AH16">
         <f t="shared" si="2"/>
-        <v>0.15878037499999997</v>
+        <v>0.15872287499999999</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -46982,14 +46982,14 @@
       </c>
       <c r="AD17">
         <f t="shared" si="1"/>
-        <v>6.7500999999999998</v>
+        <v>6.7451500000000006</v>
       </c>
       <c r="AG17" s="1" t="s">
         <v>21</v>
       </c>
       <c r="AH17">
         <f t="shared" si="2"/>
-        <v>6.8184662500000002</v>
+        <v>6.8159912500000015</v>
       </c>
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
@@ -47065,14 +47065,14 @@
       </c>
       <c r="AD18">
         <f t="shared" si="1"/>
-        <v>2.6905625</v>
+        <v>2.6885874999999997</v>
       </c>
       <c r="AG18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="AH18">
         <f t="shared" si="2"/>
-        <v>2.7178125</v>
+        <v>2.7168249999999996</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
@@ -47148,14 +47148,14 @@
       </c>
       <c r="AD19">
         <f t="shared" si="1"/>
-        <v>6.2556025000000001E-2</v>
+        <v>6.2510150000000014E-2</v>
       </c>
       <c r="AG19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="AH19">
         <f t="shared" si="2"/>
-        <v>6.3189612500000006E-2</v>
+        <v>6.3166675000000005E-2</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
@@ -47231,14 +47231,14 @@
       </c>
       <c r="AD20">
         <f t="shared" si="1"/>
-        <v>7.2570775000000004E-2</v>
+        <v>7.2517575000000001E-2</v>
       </c>
       <c r="AG20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="AH20">
         <f t="shared" si="2"/>
-        <v>7.3305787499999997E-2</v>
+        <v>7.3279187499999995E-2</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
@@ -47314,14 +47314,14 @@
       </c>
       <c r="AD21">
         <f t="shared" si="1"/>
-        <v>0.90713450000000007</v>
+        <v>0.90646950000000004</v>
       </c>
       <c r="AG21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AH21">
         <f t="shared" si="2"/>
-        <v>0.91632237500000002</v>
+        <v>0.91598987500000006</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
@@ -47397,14 +47397,14 @@
       </c>
       <c r="AD22">
         <f t="shared" si="1"/>
-        <v>0.15718824999999997</v>
+        <v>0.15707325</v>
       </c>
       <c r="AG22" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AH22">
         <f t="shared" si="2"/>
-        <v>0.15878037499999997</v>
+        <v>0.15872287499999999</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
@@ -47480,14 +47480,14 @@
       </c>
       <c r="AD23">
         <f t="shared" si="1"/>
-        <v>24.845775</v>
+        <v>24.827549999999999</v>
       </c>
       <c r="AG23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="AH23">
         <f t="shared" si="2"/>
-        <v>25.097424999999998</v>
+        <v>25.088312499999997</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
@@ -47515,14 +47515,14 @@
       </c>
       <c r="AD24">
         <f t="shared" si="1"/>
-        <v>-2.2687250000000003E-2</v>
+        <v>-1.9833750000000001E-2</v>
       </c>
       <c r="AG24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="AH24">
         <f t="shared" si="2"/>
-        <v>6.0879499999999982E-3</v>
+        <v>7.5146999999999992E-3</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
@@ -47585,14 +47585,14 @@
       </c>
       <c r="AD26">
         <f t="shared" si="1"/>
-        <v>5.2692950000000002E-2</v>
+        <v>5.0862774999999999E-2</v>
       </c>
       <c r="AG26" s="1" t="s">
         <v>39</v>
       </c>
       <c r="AH26">
         <f t="shared" si="2"/>
-        <v>3.222324E-2</v>
+        <v>3.1308152499999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
@@ -47649,7 +47649,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H30" t="s">
         <v>39</v>
@@ -47677,7 +47677,7 @@
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="Y30" t="s">
         <v>39</v>
@@ -47701,7 +47701,7 @@
         <v>42</v>
       </c>
       <c r="E31" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="R31" t="s">
         <v>2</v>
@@ -47716,7 +47716,7 @@
         <v>42</v>
       </c>
       <c r="V31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
@@ -48749,7 +48749,7 @@
         <v>38</v>
       </c>
       <c r="G55" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H55" t="s">
         <v>39</v>
@@ -48777,14 +48777,14 @@
         <v>38</v>
       </c>
       <c r="X55" t="s">
-        <v>267</v>
+        <v>301</v>
       </c>
       <c r="Y55" t="s">
         <v>39</v>
       </c>
       <c r="Z55">
-        <f>-0.0657692</f>
-        <v>-6.57692E-2</v>
+        <f>-0.0637831</f>
+        <v>-6.3783099999999995E-2</v>
       </c>
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.25">
@@ -48801,7 +48801,7 @@
         <v>42</v>
       </c>
       <c r="E56" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="R56" t="s">
         <v>2</v>
@@ -48816,7 +48816,7 @@
         <v>42</v>
       </c>
       <c r="V56" t="s">
-        <v>268</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.25">
@@ -48882,7 +48882,7 @@
         <v>48</v>
       </c>
       <c r="V59">
-        <v>0.61675100000000005</v>
+        <v>0.94295300000000004</v>
       </c>
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.25">
@@ -48944,7 +48944,7 @@
         <v>6</v>
       </c>
       <c r="AA60">
-        <v>8.5348000000000006</v>
+        <v>8.5857899999999994</v>
       </c>
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.25">
@@ -49006,7 +49006,7 @@
         <v>6</v>
       </c>
       <c r="AA61">
-        <v>6.7407300000000001</v>
+        <v>6.7809999999999997</v>
       </c>
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.25">
@@ -49068,7 +49068,7 @@
         <v>6</v>
       </c>
       <c r="AA62">
-        <v>2.6868300000000001</v>
+        <v>2.7028799999999999</v>
       </c>
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.25">
@@ -49130,7 +49130,7 @@
         <v>6</v>
       </c>
       <c r="AA63">
-        <v>6.2469200000000003E-2</v>
+        <v>6.2842400000000007E-2</v>
       </c>
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.25">
@@ -49192,7 +49192,7 @@
         <v>6</v>
       </c>
       <c r="AA64">
-        <v>7.2470000000000007E-2</v>
+        <v>7.2902999999999996E-2</v>
       </c>
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.25">
@@ -49254,7 +49254,7 @@
         <v>6</v>
       </c>
       <c r="AA65">
-        <v>0.90587499999999999</v>
+        <v>0.91128799999999999</v>
       </c>
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.25">
@@ -49316,7 +49316,7 @@
         <v>6</v>
       </c>
       <c r="AA66">
-        <v>0.15697</v>
+        <v>0.15790799999999999</v>
       </c>
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.25">
@@ -49378,7 +49378,7 @@
         <v>6</v>
       </c>
       <c r="AA67">
-        <v>6.7407300000000001</v>
+        <v>6.7809999999999997</v>
       </c>
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.25">
@@ -49440,7 +49440,7 @@
         <v>6</v>
       </c>
       <c r="AA68">
-        <v>2.6868300000000001</v>
+        <v>2.7028799999999999</v>
       </c>
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.25">
@@ -49502,7 +49502,7 @@
         <v>6</v>
       </c>
       <c r="AA69">
-        <v>6.2469200000000003E-2</v>
+        <v>6.2842400000000007E-2</v>
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
@@ -49564,7 +49564,7 @@
         <v>6</v>
       </c>
       <c r="AA70">
-        <v>7.2470000000000007E-2</v>
+        <v>7.2902999999999996E-2</v>
       </c>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
@@ -49626,7 +49626,7 @@
         <v>6</v>
       </c>
       <c r="AA71">
-        <v>0.90587499999999999</v>
+        <v>0.91128799999999999</v>
       </c>
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.25">
@@ -49688,7 +49688,7 @@
         <v>6</v>
       </c>
       <c r="AA72">
-        <v>0.15697</v>
+        <v>0.15790799999999999</v>
       </c>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.25">
@@ -49750,7 +49750,7 @@
         <v>6</v>
       </c>
       <c r="AA73">
-        <v>24.811299999999999</v>
+        <v>24.959499999999998</v>
       </c>
     </row>
     <row r="74" spans="1:27" x14ac:dyDescent="0.25">
@@ -49764,7 +49764,7 @@
         <v>38</v>
       </c>
       <c r="AA74">
-        <v>-2.7968900000000001E-2</v>
+        <v>-1.9811200000000001E-2</v>
       </c>
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.25">
@@ -49792,7 +49792,7 @@
         <v>39</v>
       </c>
       <c r="AA76">
-        <v>6.57692E-2</v>
+        <v>6.3783099999999995E-2</v>
       </c>
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.25">
@@ -49849,7 +49849,7 @@
         <v>38</v>
       </c>
       <c r="G80" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H80" t="s">
         <v>39</v>
@@ -49877,14 +49877,14 @@
         <v>38</v>
       </c>
       <c r="X80" t="s">
-        <v>269</v>
+        <v>303</v>
       </c>
       <c r="Y80" t="s">
         <v>39</v>
       </c>
       <c r="Z80">
-        <f>-0.0566468</f>
-        <v>-5.6646799999999997E-2</v>
+        <f>-0.0513122</f>
+        <v>-5.1312200000000002E-2</v>
       </c>
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.25">
@@ -49901,7 +49901,7 @@
         <v>42</v>
       </c>
       <c r="E81" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="R81" t="s">
         <v>2</v>
@@ -49916,7 +49916,7 @@
         <v>42</v>
       </c>
       <c r="V81" t="s">
-        <v>270</v>
+        <v>304</v>
       </c>
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.25">
@@ -49982,7 +49982,7 @@
         <v>48</v>
       </c>
       <c r="V84">
-        <v>1.08226</v>
+        <v>0.595688</v>
       </c>
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.25">
@@ -50044,7 +50044,7 @@
         <v>6</v>
       </c>
       <c r="AA85">
-        <v>8.6075700000000008</v>
+        <v>8.5314999999999994</v>
       </c>
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.25">
@@ -50106,7 +50106,7 @@
         <v>6</v>
       </c>
       <c r="AA86">
-        <v>6.7981999999999996</v>
+        <v>6.73813</v>
       </c>
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.25">
@@ -50168,7 +50168,7 @@
         <v>6</v>
       </c>
       <c r="AA87">
-        <v>2.70974</v>
+        <v>2.6857899999999999</v>
       </c>
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.25">
@@ -50230,7 +50230,7 @@
         <v>6</v>
       </c>
       <c r="AA88">
-        <v>6.3001799999999997E-2</v>
+        <v>6.2445100000000003E-2</v>
       </c>
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.25">
@@ -50292,7 +50292,7 @@
         <v>6</v>
       </c>
       <c r="AA89">
-        <v>7.3087899999999997E-2</v>
+        <v>7.2442099999999995E-2</v>
       </c>
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.25">
@@ -50354,7 +50354,7 @@
         <v>6</v>
       </c>
       <c r="AA90">
-        <v>0.91359900000000005</v>
+        <v>0.90552600000000005</v>
       </c>
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.25">
@@ -50416,7 +50416,7 @@
         <v>6</v>
       </c>
       <c r="AA91">
-        <v>0.158308</v>
+        <v>0.15690999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.25">
@@ -50478,7 +50478,7 @@
         <v>6</v>
       </c>
       <c r="AA92">
-        <v>6.7981999999999996</v>
+        <v>6.73813</v>
       </c>
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.25">
@@ -50540,7 +50540,7 @@
         <v>6</v>
       </c>
       <c r="AA93">
-        <v>2.70974</v>
+        <v>2.6857899999999999</v>
       </c>
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.25">
@@ -50602,7 +50602,7 @@
         <v>6</v>
       </c>
       <c r="AA94">
-        <v>6.3001799999999997E-2</v>
+        <v>6.2445100000000003E-2</v>
       </c>
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.25">
@@ -50664,7 +50664,7 @@
         <v>6</v>
       </c>
       <c r="AA95">
-        <v>7.3087899999999997E-2</v>
+        <v>7.2442099999999995E-2</v>
       </c>
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.25">
@@ -50726,7 +50726,7 @@
         <v>6</v>
       </c>
       <c r="AA96">
-        <v>0.91359900000000005</v>
+        <v>0.90552600000000005</v>
       </c>
     </row>
     <row r="97" spans="1:27" x14ac:dyDescent="0.25">
@@ -50788,7 +50788,7 @@
         <v>6</v>
       </c>
       <c r="AA97">
-        <v>0.158308</v>
+        <v>0.15690999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:27" x14ac:dyDescent="0.25">
@@ -50850,7 +50850,7 @@
         <v>6</v>
       </c>
       <c r="AA98">
-        <v>25.0228</v>
+        <v>24.8017</v>
       </c>
     </row>
     <row r="99" spans="1:27" x14ac:dyDescent="0.25">
@@ -50864,7 +50864,7 @@
         <v>38</v>
       </c>
       <c r="AA99">
-        <v>-1.8765899999999999E-2</v>
+        <v>-1.55096E-2</v>
       </c>
     </row>
     <row r="100" spans="1:27" x14ac:dyDescent="0.25">
@@ -50892,11 +50892,12 @@
         <v>39</v>
       </c>
       <c r="AA101">
-        <v>5.6646799999999997E-2</v>
+        <v>5.1312200000000002E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>